<commit_message>
fix infant mortality rates
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2945" uniqueCount="1250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2947" uniqueCount="1250">
   <si>
     <t>Metric</t>
   </si>
@@ -8932,7 +8932,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.11005502239999999</c:v>
+                  <c:v>0.103242926</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>9.4971746999999995E-3</c:v>
@@ -9078,7 +9078,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>9.3222245150000008E-2</c:v>
+                  <c:v>8.7651773500000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>9.1480569999999994E-3</c:v>
@@ -51551,8 +51551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="M129" sqref="M129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53173,21 +53173,21 @@
       </c>
       <c r="C94" s="65">
         <f>E114</f>
-        <v>0.11005502239999999</v>
+        <v>0.103242926</v>
       </c>
       <c r="D94" s="65">
         <f>E118</f>
-        <v>9.3222245150000008E-2</v>
+        <v>8.7651773500000002E-2</v>
       </c>
       <c r="E94" s="65"/>
       <c r="F94" s="65"/>
       <c r="G94" s="65">
         <f>I114</f>
-        <v>5.1002878209999998E-2</v>
+        <v>4.7225124899999998E-2</v>
       </c>
       <c r="H94" s="65">
         <f>I118</f>
-        <v>4.2630286615000006E-2</v>
+        <v>3.9540063350000001E-2</v>
       </c>
       <c r="I94" s="65"/>
       <c r="J94" s="65"/>
@@ -54802,11 +54802,11 @@
       <c r="K112" s="37" t="s">
         <v>1053</v>
       </c>
-      <c r="O112" t="s">
+      <c r="P112" t="s">
         <v>1057</v>
       </c>
     </row>
-    <row r="113" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>217</v>
       </c>
@@ -54834,17 +54834,20 @@
       <c r="L113" t="s">
         <v>1080</v>
       </c>
-      <c r="M113" t="s">
+      <c r="M113" s="37" t="s">
+        <v>1083</v>
+      </c>
+      <c r="N113" t="s">
         <v>1125</v>
       </c>
-      <c r="O113" s="37" t="s">
+      <c r="P113" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="Q113" t="s">
+      <c r="R113" t="s">
         <v>1125</v>
       </c>
     </row>
-    <row r="114" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>1078</v>
       </c>
@@ -54852,11 +54855,11 @@
         <v>0.17136388999999999</v>
       </c>
       <c r="D114">
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="E114">
         <f>(C114*D114)+(C115*D115)</f>
-        <v>0.11005502239999999</v>
+        <v>0.103242926</v>
       </c>
       <c r="G114" s="37" t="s">
         <v>1078</v>
@@ -54866,7 +54869,7 @@
       </c>
       <c r="I114">
         <f>(H114*D114)+(H115*D115)</f>
-        <v>5.1002878209999998E-2</v>
+        <v>4.7225124899999998E-2</v>
       </c>
       <c r="K114" s="37" t="s">
         <v>1078</v>
@@ -54874,22 +54877,25 @@
       <c r="L114" s="37">
         <v>7.0362258999999996E-2</v>
       </c>
-      <c r="M114">
-        <f>(L114*D114)+(L115*D115)</f>
-        <v>4.2908423740000007E-2</v>
-      </c>
-      <c r="O114" s="37" t="s">
+      <c r="M114" s="37">
+        <v>0.53</v>
+      </c>
+      <c r="N114">
+        <f>(L114*M114)+(L115*M115)</f>
+        <v>4.1688253283999999E-2</v>
+      </c>
+      <c r="P114" s="37" t="s">
         <v>1078</v>
       </c>
-      <c r="P114" s="37">
+      <c r="Q114" s="37">
         <v>3.5942957999999997E-2</v>
       </c>
-      <c r="Q114">
-        <f>(P114*D114)+(P115*D115)</f>
-        <v>2.0946311775E-2</v>
-      </c>
-    </row>
-    <row r="115" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R114">
+        <f>(Q114*M114)+(Q115*M115)</f>
+        <v>2.0279794165E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>1079</v>
       </c>
@@ -54898,7 +54904,7 @@
       </c>
       <c r="D115">
         <f>1-D114</f>
-        <v>0.44999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="G115" s="37" t="s">
         <v>1079</v>
@@ -54912,18 +54918,23 @@
       <c r="L115" s="37">
         <v>9.3537362000000006E-3</v>
       </c>
-      <c r="O115" s="37" t="s">
+      <c r="M115" s="37">
+        <f>1-M114</f>
+        <v>0.47</v>
+      </c>
+      <c r="P115" s="37" t="s">
         <v>1079</v>
       </c>
-      <c r="P115" s="37">
+      <c r="Q115" s="37">
         <v>2.6170774999999999E-3</v>
       </c>
     </row>
-    <row r="116" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K116" s="37"/>
-      <c r="O116" s="37"/>
-    </row>
-    <row r="117" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M116" s="37"/>
+      <c r="P116" s="37"/>
+    </row>
+    <row r="117" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B117" s="37" t="s">
         <v>1081</v>
       </c>
@@ -54948,11 +54959,14 @@
       <c r="K117" s="37" t="s">
         <v>1081</v>
       </c>
-      <c r="O117" s="37" t="s">
+      <c r="M117" s="37" t="s">
+        <v>1083</v>
+      </c>
+      <c r="P117" s="37" t="s">
         <v>1081</v>
       </c>
     </row>
-    <row r="118" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B118" s="37" t="s">
         <v>1078</v>
       </c>
@@ -54960,11 +54974,11 @@
         <v>0.14335649</v>
       </c>
       <c r="D118" s="37">
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="E118">
         <f>(C118*D118)+(C119*D119)</f>
-        <v>9.3222245150000008E-2</v>
+        <v>8.7651773500000002E-2</v>
       </c>
       <c r="G118" s="37" t="s">
         <v>1078</v>
@@ -54974,7 +54988,7 @@
       </c>
       <c r="I118">
         <f>(H118*D118)+(H119*D119)</f>
-        <v>4.2630286615000006E-2</v>
+        <v>3.9540063350000001E-2</v>
       </c>
       <c r="K118" s="37" t="s">
         <v>1078</v>
@@ -54982,22 +54996,25 @@
       <c r="L118" s="37">
         <v>6.1459527999999999E-2</v>
       </c>
-      <c r="M118">
-        <f>(L118*D118)+(L119*D119)</f>
-        <v>3.7321990735000005E-2</v>
-      </c>
-      <c r="O118" s="37" t="s">
+      <c r="M118" s="37">
+        <v>0.53</v>
+      </c>
+      <c r="N118">
+        <f>(L118*M118)+(L119*M119)</f>
+        <v>3.6249211300999999E-2</v>
+      </c>
+      <c r="P118" s="37" t="s">
         <v>1078</v>
       </c>
-      <c r="P118" s="37">
+      <c r="Q118" s="37">
         <v>2.6885009000000001E-2</v>
       </c>
-      <c r="Q118">
-        <f>(P118*D118)+(P119*D119)</f>
-        <v>1.5803535170000001E-2</v>
-      </c>
-    </row>
-    <row r="119" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R118">
+        <f>(Q118*M118)+(Q119*M119)</f>
+        <v>1.5311025222000002E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B119" s="37" t="s">
         <v>1079</v>
       </c>
@@ -55006,7 +55023,7 @@
       </c>
       <c r="D119" s="37">
         <f>1-D118</f>
-        <v>0.44999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="G119" s="37" t="s">
         <v>1079</v>
@@ -55020,20 +55037,18 @@
       <c r="L119" s="37">
         <v>7.8205562999999999E-3</v>
       </c>
-      <c r="O119" s="37" t="s">
+      <c r="M119" s="37">
+        <f>1-M118</f>
+        <v>0.47</v>
+      </c>
+      <c r="P119" s="37" t="s">
         <v>1079</v>
       </c>
-      <c r="P119" s="37">
+      <c r="Q119" s="37">
         <v>2.2595115999999998E-3</v>
       </c>
     </row>
-    <row r="120" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D120">
-        <f>100-17</f>
-        <v>83</v>
-      </c>
-    </row>
-    <row r="121" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C121">
         <v>0</v>
       </c>
@@ -55050,7 +55065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>1</v>
       </c>
@@ -55082,7 +55097,7 @@
         <v>0.24131406624814078</v>
       </c>
     </row>
-    <row r="123" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>2</v>
       </c>
@@ -55102,7 +55117,7 @@
         <v>77.145162397419966</v>
       </c>
     </row>
-    <row r="124" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>2</v>
       </c>
@@ -55116,7 +55131,7 @@
         <v>79.95327840327522</v>
       </c>
     </row>
-    <row r="125" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>3</v>
       </c>
@@ -55127,7 +55142,7 @@
         <v>82.863611000000006</v>
       </c>
     </row>
-    <row r="126" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>4</v>
       </c>
@@ -55135,7 +55150,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="127" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H127">
         <f>SUM(C122:G126)</f>
         <v>1300.0402769398795</v>

</xml_diff>

<commit_message>
add more years for pop validation
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9000" tabRatio="641" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9000" tabRatio="641"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="10" r:id="rId1"/>
@@ -3821,7 +3821,7 @@
     <numFmt numFmtId="173" formatCode="#\ ###\ ###\ ##0;\-#\ ###\ ###\ ##0;0"/>
     <numFmt numFmtId="174" formatCode="##0.0000;\-##0.0000;0.000"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4040,6 +4040,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="37">
@@ -4501,7 +4521,7 @@
     <xf numFmtId="0" fontId="1" fillId="35" borderId="8" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="8" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4607,6 +4627,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="173" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="173" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -27254,8 +27281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y184"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="I152" sqref="I152"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="G170" sqref="G170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33570,49 +33597,49 @@
       </c>
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B164" s="46" t="s">
+      <c r="B164" s="79" t="s">
         <v>328</v>
       </c>
-      <c r="C164" s="37">
+      <c r="C164" s="80">
         <v>29.832999999999998</v>
       </c>
-      <c r="D164" s="49">
+      <c r="D164" s="81">
         <v>36.995000000000005</v>
       </c>
-      <c r="E164" s="37">
+      <c r="E164" s="80">
         <v>30.677999999999997</v>
       </c>
-      <c r="F164" s="49">
+      <c r="F164" s="81">
         <v>40.189</v>
       </c>
-      <c r="G164" s="37">
+      <c r="G164" s="80">
         <v>28.76</v>
       </c>
-      <c r="H164" s="49">
+      <c r="H164" s="81">
         <v>45.019999999999989</v>
       </c>
-      <c r="I164" s="37">
+      <c r="I164" s="80">
         <v>27.613</v>
       </c>
-      <c r="J164" s="49">
+      <c r="J164" s="81">
         <v>49.994</v>
       </c>
-      <c r="K164" s="37">
+      <c r="K164" s="80">
         <v>30.65</v>
       </c>
-      <c r="L164" s="49">
+      <c r="L164" s="81">
         <v>57.32</v>
       </c>
-      <c r="M164" s="37">
+      <c r="M164" s="80">
         <v>39.680999999999997</v>
       </c>
-      <c r="N164" s="49">
+      <c r="N164" s="81">
         <v>73.600999999999999</v>
       </c>
-      <c r="O164" s="37">
+      <c r="O164" s="80">
         <v>50.151000000000003</v>
       </c>
-      <c r="P164" s="49">
+      <c r="P164" s="81">
         <v>94.126999999999995</v>
       </c>
     </row>
@@ -33722,35 +33749,35 @@
         <v>240.16582243333008</v>
       </c>
       <c r="H169">
-        <v>2010</v>
+        <v>1990</v>
       </c>
       <c r="I169">
-        <f>SUM(K148:L149)/SUM(K148:L163)</f>
-        <v>0.30836194815624002</v>
+        <f>SUM(C$148:D$149)/SUM($C$148:$D$163)</f>
+        <v>0.35549337624979127</v>
       </c>
       <c r="J169" s="37">
-        <f>SUM(K150:L151)/SUM(K148:L163)</f>
-        <v>0.23369136293850706</v>
+        <f>SUM(C$150:D$151)/SUM($C$148:$D$163)</f>
+        <v>0.2487095769816785</v>
       </c>
       <c r="K169" s="37">
-        <f>SUM(K152:L153)/SUM(K148:L163)</f>
-        <v>0.18557385199250581</v>
+        <f>SUM(C$152:D$153)/SUM($C$148:$D$163)</f>
+        <v>0.16036853215010419</v>
       </c>
       <c r="L169" s="37">
-        <f>SUM(K154:L155)/SUM(K148:L163)</f>
-        <v>0.12474426428389926</v>
+        <f>SUM(C$154:D$155)/SUM($C$148:$D$163)</f>
+        <v>0.10367995328041812</v>
       </c>
       <c r="M169" s="37">
-        <f>SUM(K156:L157)/SUM(K148:L163)</f>
-        <v>7.4102333959600239E-2</v>
+        <f>SUM(C$156:D$157)/SUM($C$148:$D$163)</f>
+        <v>5.6436483847615897E-2</v>
       </c>
       <c r="N169" s="37">
-        <f>SUM(K158:L159)/SUM(K148:L163)</f>
-        <v>4.3525843368171176E-2</v>
+        <f>SUM(C$158:D$159)/SUM($C$148:$D$163)</f>
+        <v>3.896677223603634E-2</v>
       </c>
       <c r="O169" s="37">
-        <f>SUM(K160:L163)/SUM(K148:L163)</f>
-        <v>3.0000395301076618E-2</v>
+        <f>SUM(C$160:D$163)/SUM($C$148:$D$163)</f>
+        <v>3.6345305254355149E-2</v>
       </c>
       <c r="P169" s="50"/>
       <c r="Q169" s="50"/>
@@ -33767,36 +33794,36 @@
       <c r="E170" s="50"/>
       <c r="F170" s="50"/>
       <c r="G170" s="50"/>
-      <c r="H170" s="16">
-        <v>2015</v>
+      <c r="H170">
+        <v>1995</v>
       </c>
       <c r="I170">
-        <f>SUM(M148:N149)/SUM($M$148:$N$163)</f>
-        <v>0.28891821483642321</v>
+        <f>SUM(E148:F149)/SUM($E$148:$F$163)</f>
+        <v>0.329724598997091</v>
       </c>
       <c r="J170" s="37">
-        <f>SUM(M150:N151)/SUM($M$148:$N$163)</f>
-        <v>0.23718746949260416</v>
+        <f>SUM(E150:F151)/SUM($E$148:$F$163)</f>
+        <v>0.25572087374171532</v>
       </c>
       <c r="K170" s="37">
-        <f>SUM(M152:N153)/SUM($M$148:$N$163)</f>
-        <v>0.17828937166347358</v>
+        <f>SUM(E152:F153)/SUM($E$148:$F$163)</f>
+        <v>0.17060427628122893</v>
       </c>
       <c r="L170" s="37">
-        <f>SUM(M154:N155)/SUM($M$148:$N$163)</f>
-        <v>0.13331999164158853</v>
+        <f>SUM(E154:F155)/SUM($E$148:$F$163)</f>
+        <v>0.10858198757068795</v>
       </c>
       <c r="M170" s="37">
-        <f>SUM(M156:N157)/SUM($M$148:$N$163)</f>
-        <v>8.1694197496718149E-2</v>
+        <f>SUM(E156:F157)/SUM($E$148:$F$163)</f>
+        <v>6.5205652654415941E-2</v>
       </c>
       <c r="N170" s="37">
-        <f>SUM(M158:N159)/SUM($M$148:$N$163)</f>
-        <v>4.6954659763098365E-2</v>
+        <f>SUM(E158:F159)/SUM($E$148:$F$163)</f>
+        <v>3.4783877060073805E-2</v>
       </c>
       <c r="O170" s="37">
-        <f>SUM(M160:N163)/SUM($M$148:$N$163)</f>
-        <v>3.3636095106093979E-2</v>
+        <f>SUM(E160:F163)/SUM($E$148:$F$163)</f>
+        <v>3.5378733694786835E-2</v>
       </c>
       <c r="P170" s="50"/>
       <c r="Q170" s="50"/>
@@ -33810,35 +33837,35 @@
         <v>110.9988196360878</v>
       </c>
       <c r="H171">
-        <v>2020</v>
+        <v>2000</v>
       </c>
       <c r="I171">
-        <f>SUM(O148:P149)/SUM($O$148:$P$163)</f>
-        <v>0.26132180153505447</v>
+        <f>SUM(G148:H149)/SUM($G$148:$H$163)</f>
+        <v>0.31791370276114633</v>
       </c>
       <c r="J171" s="37">
-        <f>SUM(O150:P151)/SUM($O$148:$P$163)</f>
-        <v>0.23769507469573828</v>
+        <f>SUM(G150:H151)/SUM($G$148:$H$163)</f>
+        <v>0.2550967008423784</v>
       </c>
       <c r="K171" s="37">
-        <f>SUM(O152:P153)/SUM($O$148:$P$163)</f>
-        <v>0.17890745452917378</v>
+        <f>SUM(G152:H153)/SUM($G$148:$H$163)</f>
+        <v>0.17860301741785722</v>
       </c>
       <c r="L171" s="37">
-        <f>SUM(O154:P155)/SUM($O$148:$P$163)</f>
-        <v>0.13929816949373025</v>
+        <f>SUM(G154:H155)/SUM($G$148:$H$163)</f>
+        <v>0.11147734029810565</v>
       </c>
       <c r="M171" s="37">
-        <f>SUM(O156:P157)/SUM($O$148:$P$163)</f>
-        <v>9.1428627157405837E-2</v>
+        <f>SUM(G156:H157)/SUM($G$148:$H$163)</f>
+        <v>6.8597356533520656E-2</v>
       </c>
       <c r="N171" s="37">
-        <f>SUM(O158:P159)/SUM($O$148:$P$163)</f>
-        <v>5.231696438411218E-2</v>
+        <f>SUM(G158:H159)/SUM($G$148:$H$163)</f>
+        <v>3.5690977363141703E-2</v>
       </c>
       <c r="O171" s="37">
-        <f>SUM(O160:P163)/SUM($O$148:$P$163)</f>
-        <v>3.9031908204785269E-2</v>
+        <f>SUM(G160:H163)/SUM($G$148:$H$163)</f>
+        <v>3.2620904783850206E-2</v>
       </c>
       <c r="P171" s="50"/>
       <c r="Q171" s="50"/>
@@ -33851,7 +33878,37 @@
       <c r="C172">
         <v>97.33925564881072</v>
       </c>
-      <c r="O172" s="77"/>
+      <c r="H172">
+        <v>2005</v>
+      </c>
+      <c r="I172">
+        <f>SUM(I148:J149)/SUM($I$148:$J$163)</f>
+        <v>0.31717005556362726</v>
+      </c>
+      <c r="J172" s="37">
+        <f>SUM(I150:J151)/SUM($I$148:$J$163)</f>
+        <v>0.24080056277770526</v>
+      </c>
+      <c r="K172" s="37">
+        <f>SUM(I152:J153)/SUM($I$148:$J$163)</f>
+        <v>0.185498404943294</v>
+      </c>
+      <c r="L172" s="37">
+        <f>SUM(I154:J155)/SUM($I$148:$J$163)</f>
+        <v>0.11701056357393393</v>
+      </c>
+      <c r="M172" s="37">
+        <f>SUM(I156:J157)/SUM($I$148:$J$163)</f>
+        <v>6.9963874202437451E-2</v>
+      </c>
+      <c r="N172" s="37">
+        <f>SUM(I158:J159)/SUM($I$148:$J$163)</f>
+        <v>4.0111619767156471E-2</v>
+      </c>
+      <c r="O172" s="37">
+        <f>SUM(I160:J163)/SUM($I$148:$J$163)</f>
+        <v>2.9444919171845576E-2</v>
+      </c>
       <c r="P172" s="50"/>
       <c r="Q172" s="50"/>
       <c r="R172" s="50"/>
@@ -33863,7 +33920,37 @@
       <c r="C173">
         <v>86.235432425086415</v>
       </c>
-      <c r="O173" s="77"/>
+      <c r="H173">
+        <v>2010</v>
+      </c>
+      <c r="I173">
+        <f>SUM(K148:L149)/SUM(K148:L163)</f>
+        <v>0.30836194815624002</v>
+      </c>
+      <c r="J173" s="37">
+        <f>SUM(K150:L151)/SUM(K148:L163)</f>
+        <v>0.23369136293850706</v>
+      </c>
+      <c r="K173" s="37">
+        <f>SUM(K152:L153)/SUM(K148:L163)</f>
+        <v>0.18557385199250581</v>
+      </c>
+      <c r="L173" s="37">
+        <f>SUM(K154:L155)/SUM(K148:L163)</f>
+        <v>0.12474426428389926</v>
+      </c>
+      <c r="M173" s="37">
+        <f>SUM(K156:L157)/SUM(K148:L163)</f>
+        <v>7.4102333959600239E-2</v>
+      </c>
+      <c r="N173" s="37">
+        <f>SUM(K158:L159)/SUM(K148:L163)</f>
+        <v>4.3525843368171176E-2</v>
+      </c>
+      <c r="O173" s="37">
+        <f>SUM(K160:L163)/SUM(K148:L163)</f>
+        <v>3.0000395301076618E-2</v>
+      </c>
       <c r="P173" s="50"/>
       <c r="Q173" s="50"/>
       <c r="R173" s="50"/>
@@ -33875,6 +33962,37 @@
       <c r="C174">
         <v>75.946598869604159</v>
       </c>
+      <c r="H174" s="16">
+        <v>2015</v>
+      </c>
+      <c r="I174">
+        <f>SUM(M148:N149)/SUM($M$148:$N$163)</f>
+        <v>0.28891821483642321</v>
+      </c>
+      <c r="J174" s="37">
+        <f>SUM(M150:N151)/SUM($M$148:$N$163)</f>
+        <v>0.23718746949260416</v>
+      </c>
+      <c r="K174" s="37">
+        <f>SUM(M152:N153)/SUM($M$148:$N$163)</f>
+        <v>0.17828937166347358</v>
+      </c>
+      <c r="L174" s="37">
+        <f>SUM(M154:N155)/SUM($M$148:$N$163)</f>
+        <v>0.13331999164158853</v>
+      </c>
+      <c r="M174" s="37">
+        <f>SUM(M156:N157)/SUM($M$148:$N$163)</f>
+        <v>8.1694197496718149E-2</v>
+      </c>
+      <c r="N174" s="37">
+        <f>SUM(M158:N159)/SUM($M$148:$N$163)</f>
+        <v>4.6954659763098365E-2</v>
+      </c>
+      <c r="O174" s="37">
+        <f>SUM(M160:N163)/SUM($M$148:$N$163)</f>
+        <v>3.3636095106093979E-2</v>
+      </c>
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B175">
@@ -33883,9 +34001,37 @@
       <c r="C175">
         <v>68.470328142000795</v>
       </c>
-      <c r="J175" s="37"/>
-      <c r="K175" s="37"/>
-      <c r="L175" s="37"/>
+      <c r="H175">
+        <v>2020</v>
+      </c>
+      <c r="I175">
+        <f>SUM(O148:P149)/SUM($O$148:$P$163)</f>
+        <v>0.26132180153505447</v>
+      </c>
+      <c r="J175" s="37">
+        <f>SUM(O150:P151)/SUM($O$148:$P$163)</f>
+        <v>0.23769507469573828</v>
+      </c>
+      <c r="K175" s="37">
+        <f>SUM(O152:P153)/SUM($O$148:$P$163)</f>
+        <v>0.17890745452917378</v>
+      </c>
+      <c r="L175" s="37">
+        <f>SUM(O154:P155)/SUM($O$148:$P$163)</f>
+        <v>0.13929816949373025</v>
+      </c>
+      <c r="M175" s="37">
+        <f>SUM(O156:P157)/SUM($O$148:$P$163)</f>
+        <v>9.1428627157405837E-2</v>
+      </c>
+      <c r="N175" s="37">
+        <f>SUM(O158:P159)/SUM($O$148:$P$163)</f>
+        <v>5.231696438411218E-2</v>
+      </c>
+      <c r="O175" s="37">
+        <f>SUM(O160:P163)/SUM($O$148:$P$163)</f>
+        <v>3.9031908204785269E-2</v>
+      </c>
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B176">
@@ -41946,7 +42092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+    <sheetView topLeftCell="A57" workbookViewId="0">
       <selection activeCell="M82" sqref="M82"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
increased infant mortality rates from 2000 on
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -51593,7 +51593,7 @@
   <dimension ref="A1:AX127"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="N114" sqref="N114"/>
+      <selection activeCell="M119" sqref="M119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53224,31 +53224,31 @@
       <c r="F94" s="64"/>
       <c r="G94" s="64">
         <f>I114</f>
-        <v>5.4780631519999998E-2</v>
+        <v>6.233613813999999E-2</v>
       </c>
       <c r="H94" s="64">
         <f>I118</f>
-        <v>4.5720509880000003E-2</v>
+        <v>5.1900956410000004E-2</v>
       </c>
       <c r="I94" s="64"/>
       <c r="J94" s="64"/>
       <c r="K94" s="64">
         <f>N114</f>
-        <v>4.5958849879999999E-2</v>
+        <v>5.2059702159999999E-2</v>
       </c>
       <c r="L94" s="64">
         <f>N118</f>
-        <v>4.0003939320000001E-2</v>
+        <v>4.5367836490000001E-2</v>
       </c>
       <c r="M94" s="64"/>
       <c r="N94" s="64"/>
       <c r="O94" s="64">
         <f>R114</f>
-        <v>2.2612605799999998E-2</v>
+        <v>2.5945193849999996E-2</v>
       </c>
       <c r="P94" s="64">
         <f>R118</f>
-        <v>1.7034810039999997E-2</v>
+        <v>1.9497359780000001E-2</v>
       </c>
       <c r="R94" s="37" t="s">
         <v>1228</v>
@@ -54914,7 +54914,7 @@
       </c>
       <c r="I114">
         <f>(H114*M114)+(H115*M115)</f>
-        <v>5.4780631519999998E-2</v>
+        <v>6.233613813999999E-2</v>
       </c>
       <c r="K114" s="37" t="s">
         <v>1078</v>
@@ -54923,11 +54923,11 @@
         <v>7.0362258999999996E-2</v>
       </c>
       <c r="M114" s="37">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="N114">
         <f>(L114*M114)+(L115*M115)</f>
-        <v>4.5958849879999999E-2</v>
+        <v>5.2059702159999999E-2</v>
       </c>
       <c r="P114" s="37" t="s">
         <v>1078</v>
@@ -54937,7 +54937,7 @@
       </c>
       <c r="R114">
         <f>(Q114*M114)+(Q115*M115)</f>
-        <v>2.2612605799999998E-2</v>
+        <v>2.5945193849999996E-2</v>
       </c>
     </row>
     <row r="115" spans="2:18" x14ac:dyDescent="0.25">
@@ -54965,7 +54965,7 @@
       </c>
       <c r="M115" s="37">
         <f>1-M114</f>
-        <v>0.4</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="P115" s="37" t="s">
         <v>1079</v>
@@ -55033,7 +55033,7 @@
       </c>
       <c r="I118">
         <f>(H118*M118)+(H119*M119)</f>
-        <v>4.5720509880000003E-2</v>
+        <v>5.1900956410000004E-2</v>
       </c>
       <c r="K118" s="37" t="s">
         <v>1078</v>
@@ -55042,11 +55042,11 @@
         <v>6.1459527999999999E-2</v>
       </c>
       <c r="M118" s="37">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="N118">
         <f>(L118*M118)+(L119*M119)</f>
-        <v>4.0003939320000001E-2</v>
+        <v>4.5367836490000001E-2</v>
       </c>
       <c r="P118" s="37" t="s">
         <v>1078</v>
@@ -55056,7 +55056,7 @@
       </c>
       <c r="R118">
         <f>(Q118*M118)+(Q119*M119)</f>
-        <v>1.7034810039999997E-2</v>
+        <v>1.9497359780000001E-2</v>
       </c>
     </row>
     <row r="119" spans="2:18" x14ac:dyDescent="0.25">
@@ -55084,7 +55084,7 @@
       </c>
       <c r="M119" s="37">
         <f>1-M118</f>
-        <v>0.4</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="P119" s="37" t="s">
         <v>1079</v>

</xml_diff>

<commit_message>
Increased infant mortality in 1985
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -51592,8 +51592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="M119" sqref="M119"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="I115" sqref="I115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53223,31 +53223,31 @@
       <c r="E94" s="64"/>
       <c r="F94" s="64"/>
       <c r="G94" s="64">
-        <f>I114</f>
-        <v>6.9891644759999996E-2</v>
+        <f>J114</f>
+        <v>7.5936050056000001E-2</v>
       </c>
       <c r="H94" s="64">
-        <f>I118</f>
-        <v>5.8081402939999999E-2</v>
+        <f>J118</f>
+        <v>6.3025760164000008E-2</v>
       </c>
       <c r="I94" s="64"/>
       <c r="J94" s="64"/>
       <c r="K94" s="64">
-        <f>N114</f>
+        <f>O114</f>
         <v>5.8160554439999998E-2</v>
       </c>
       <c r="L94" s="64">
-        <f>N118</f>
+        <f>O118</f>
         <v>5.073173366E-2</v>
       </c>
       <c r="M94" s="64"/>
       <c r="N94" s="64"/>
       <c r="O94" s="64">
-        <f>R114</f>
+        <f>S114</f>
         <v>2.9277781899999997E-2</v>
       </c>
       <c r="P94" s="64">
-        <f>R118</f>
+        <f>S118</f>
         <v>2.1959909520000001E-2</v>
       </c>
       <c r="R94" s="37" t="s">
@@ -54837,6 +54837,9 @@
       <c r="AS109" s="37"/>
       <c r="AT109" s="37"/>
     </row>
+    <row r="111" spans="2:46" x14ac:dyDescent="0.25">
+      <c r="J111" s="37"/>
+    </row>
     <row r="112" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>1043</v>
@@ -54844,14 +54847,15 @@
       <c r="G112" t="s">
         <v>1050</v>
       </c>
-      <c r="K112" s="37" t="s">
+      <c r="J112" s="37"/>
+      <c r="L112" s="37" t="s">
         <v>1053</v>
       </c>
-      <c r="P112" t="s">
+      <c r="Q112" t="s">
         <v>1057</v>
       </c>
     </row>
-    <row r="113" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>217</v>
       </c>
@@ -54870,29 +54874,29 @@
       <c r="H113" s="37" t="s">
         <v>1080</v>
       </c>
-      <c r="I113" s="37" t="s">
+      <c r="J113" s="37" t="s">
         <v>1082</v>
       </c>
-      <c r="K113" s="37" t="s">
+      <c r="L113" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="L113" t="s">
+      <c r="M113" t="s">
         <v>1080</v>
       </c>
-      <c r="M113" s="37" t="s">
+      <c r="N113" s="37" t="s">
         <v>1083</v>
       </c>
-      <c r="N113" t="s">
+      <c r="O113" t="s">
         <v>1125</v>
       </c>
-      <c r="P113" s="37" t="s">
+      <c r="Q113" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="R113" t="s">
+      <c r="S113" t="s">
         <v>1125</v>
       </c>
     </row>
-    <row r="114" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>1078</v>
       </c>
@@ -54913,34 +54917,37 @@
         <v>8.5002657999999995E-2</v>
       </c>
       <c r="I114">
-        <f>(H114*M114)+(H115*M115)</f>
-        <v>6.9891644759999996E-2</v>
-      </c>
-      <c r="K114" s="37" t="s">
+        <v>0.88</v>
+      </c>
+      <c r="J114">
+        <f>(H114*I114)+(H115*I115)</f>
+        <v>7.5936050056000001E-2</v>
+      </c>
+      <c r="L114" s="37" t="s">
         <v>1078</v>
       </c>
-      <c r="L114" s="37">
+      <c r="M114" s="37">
         <v>7.0362258999999996E-2</v>
       </c>
-      <c r="M114" s="37">
+      <c r="N114" s="37">
         <v>0.8</v>
       </c>
-      <c r="N114">
-        <f>(L114*M114)+(L115*M115)</f>
+      <c r="O114">
+        <f>(M114*N114)+(M115*N115)</f>
         <v>5.8160554439999998E-2</v>
       </c>
-      <c r="P114" s="37" t="s">
+      <c r="Q114" s="37" t="s">
         <v>1078</v>
       </c>
-      <c r="Q114" s="37">
+      <c r="R114" s="37">
         <v>3.5942957999999997E-2</v>
       </c>
-      <c r="R114">
-        <f>(Q114*M114)+(Q115*M115)</f>
+      <c r="S114">
+        <f>(R114*N114)+(R115*N115)</f>
         <v>2.9277781899999997E-2</v>
       </c>
     </row>
-    <row r="115" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>1079</v>
       </c>
@@ -54957,29 +54964,33 @@
       <c r="H115">
         <v>9.4475918000000002E-3</v>
       </c>
-      <c r="K115" s="37" t="s">
+      <c r="I115">
+        <f>1-I114</f>
+        <v>0.12</v>
+      </c>
+      <c r="L115" s="37" t="s">
         <v>1079</v>
       </c>
-      <c r="L115" s="37">
+      <c r="M115" s="37">
         <v>9.3537362000000006E-3</v>
       </c>
-      <c r="M115" s="37">
-        <f>1-M114</f>
+      <c r="N115" s="37">
+        <f>1-N114</f>
         <v>0.19999999999999996</v>
       </c>
-      <c r="P115" s="37" t="s">
+      <c r="Q115" s="37" t="s">
         <v>1079</v>
       </c>
-      <c r="Q115" s="37">
+      <c r="R115" s="37">
         <v>2.6170774999999999E-3</v>
       </c>
     </row>
-    <row r="116" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K116" s="37"/>
-      <c r="M116" s="37"/>
-      <c r="P116" s="37"/>
-    </row>
-    <row r="117" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="L116" s="37"/>
+      <c r="N116" s="37"/>
+      <c r="Q116" s="37"/>
+    </row>
+    <row r="117" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B117" s="37" t="s">
         <v>1081</v>
       </c>
@@ -54998,20 +55009,20 @@
       <c r="H117" s="37" t="s">
         <v>1080</v>
       </c>
-      <c r="I117" s="37" t="s">
+      <c r="J117" s="37" t="s">
         <v>1082</v>
       </c>
-      <c r="K117" s="37" t="s">
+      <c r="L117" s="37" t="s">
         <v>1081</v>
       </c>
-      <c r="M117" s="37" t="s">
+      <c r="N117" s="37" t="s">
         <v>1083</v>
       </c>
-      <c r="P117" s="37" t="s">
+      <c r="Q117" s="37" t="s">
         <v>1081</v>
       </c>
     </row>
-    <row r="118" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B118" s="37" t="s">
         <v>1078</v>
       </c>
@@ -55032,34 +55043,38 @@
         <v>7.0442296000000001E-2</v>
       </c>
       <c r="I118">
-        <f>(H118*M118)+(H119*M119)</f>
-        <v>5.8081402939999999E-2</v>
-      </c>
-      <c r="K118" s="37" t="s">
+        <f>I114</f>
+        <v>0.88</v>
+      </c>
+      <c r="J118">
+        <f>(H118*I118)+(H119*I119)</f>
+        <v>6.3025760164000008E-2</v>
+      </c>
+      <c r="L118" s="37" t="s">
         <v>1078</v>
       </c>
-      <c r="L118" s="37">
+      <c r="M118" s="37">
         <v>6.1459527999999999E-2</v>
       </c>
-      <c r="M118" s="37">
+      <c r="N118" s="37">
         <v>0.8</v>
       </c>
-      <c r="N118">
-        <f>(L118*M118)+(L119*M119)</f>
+      <c r="O118">
+        <f>(M118*N118)+(M119*N119)</f>
         <v>5.073173366E-2</v>
       </c>
-      <c r="P118" s="37" t="s">
+      <c r="Q118" s="37" t="s">
         <v>1078</v>
       </c>
-      <c r="Q118" s="37">
+      <c r="R118" s="37">
         <v>2.6885009000000001E-2</v>
       </c>
-      <c r="R118">
-        <f>(Q118*M118)+(Q119*M119)</f>
+      <c r="S118">
+        <f>(R118*N118)+(R119*N119)</f>
         <v>2.1959909520000001E-2</v>
       </c>
     </row>
-    <row r="119" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B119" s="37" t="s">
         <v>1079</v>
       </c>
@@ -55076,24 +55091,31 @@
       <c r="H119">
         <v>8.6378306999999998E-3</v>
       </c>
-      <c r="K119" s="37" t="s">
+      <c r="I119">
+        <f>1-I118</f>
+        <v>0.12</v>
+      </c>
+      <c r="L119" s="37" t="s">
         <v>1079</v>
       </c>
-      <c r="L119" s="37">
+      <c r="M119" s="37">
         <v>7.8205562999999999E-3</v>
       </c>
-      <c r="M119" s="37">
-        <f>1-M118</f>
+      <c r="N119" s="37">
+        <f>1-N118</f>
         <v>0.19999999999999996</v>
       </c>
-      <c r="P119" s="37" t="s">
+      <c r="Q119" s="37" t="s">
         <v>1079</v>
       </c>
-      <c r="Q119" s="37">
+      <c r="R119" s="37">
         <v>2.2595115999999998E-3</v>
       </c>
     </row>
-    <row r="121" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="J120" s="37"/>
+    </row>
+    <row r="121" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C121">
         <v>0</v>
       </c>
@@ -55110,7 +55132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>1</v>
       </c>
@@ -55142,7 +55164,7 @@
         <v>0.24131406624814078</v>
       </c>
     </row>
-    <row r="123" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>2</v>
       </c>
@@ -55162,7 +55184,7 @@
         <v>77.145162397419966</v>
       </c>
     </row>
-    <row r="124" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>2</v>
       </c>
@@ -55176,7 +55198,7 @@
         <v>79.95327840327522</v>
       </c>
     </row>
-    <row r="125" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>3</v>
       </c>
@@ -55187,7 +55209,7 @@
         <v>82.863611000000006</v>
       </c>
     </row>
-    <row r="126" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>4</v>
       </c>
@@ -55195,7 +55217,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="127" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H127">
         <f>SUM(C122:G126)</f>
         <v>1300.0402769398795</v>

</xml_diff>

<commit_message>
update pop plots and mortality:x!
:x!
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="8100" tabRatio="835" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="8100" tabRatio="835"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3139" uniqueCount="1327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3147" uniqueCount="1333">
   <si>
     <t>Metric</t>
   </si>
@@ -4034,12 +4034,31 @@
   <si>
     <t xml:space="preserve">CI </t>
   </si>
+  <si>
+    <t>40-49, Kenya KNBS</t>
+  </si>
+  <si>
+    <t>40-49, UN Kenya</t>
+  </si>
+  <si>
+    <t>40-49, Nyanza KNBS</t>
+  </si>
+  <si>
+    <t>50+, Kenya KNBS</t>
+  </si>
+  <si>
+    <t>50+, Nyanza KNBS</t>
+  </si>
+  <si>
+    <t>50+, UN Kenya</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="11">
+  <numFmts count="12">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
@@ -4696,7 +4715,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="54">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -4757,8 +4776,9 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="8" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="8" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="8" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4874,8 +4894,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="54" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="54">
+  <cellStyles count="55">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -4903,6 +4924,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="54" builtinId="3"/>
     <cellStyle name="Data" xfId="46"/>
     <cellStyle name="Data 2" xfId="48"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -18946,7 +18968,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Population!$B$198:$B$201</c:f>
+              <c:f>Population!$B$222:$B$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -19029,7 +19051,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Population!$B$198:$B$201</c:f>
+              <c:f>Population!$B$222:$B$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -19114,7 +19136,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Population!$B$198:$B$201</c:f>
+              <c:f>Population!$B$222:$B$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -19197,7 +19219,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Population!$B$198:$B$201</c:f>
+              <c:f>Population!$B$222:$B$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -19245,8 +19267,91 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="6"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Population!$E$221</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>40-49, UN Kenya</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Population!$B$222:$B$225</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Population!$E$222:$E$225</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6.2283021048104255</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6277512085148489</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8439021382339202</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3947238165336548</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000016-E7F8-4AF0-95D0-AAB85B337E39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="2"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Population!$D$197</c:f>
@@ -19276,7 +19381,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Population!$B$198:$B$201</c:f>
+              <c:f>Population!$B$222:$B$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -19322,7 +19427,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="5"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
               <c:f>Population!$D$203</c:f>
@@ -19349,7 +19454,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Population!$B$198:$B$201</c:f>
+              <c:f>Population!$B$222:$B$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -19395,7 +19500,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="9"/>
-          <c:order val="6"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
               <c:f>Population!$D$209</c:f>
@@ -19422,7 +19527,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Population!$B$198:$B$201</c:f>
+              <c:f>Population!$B$222:$B$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -19468,7 +19573,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="11"/>
-          <c:order val="7"/>
+          <c:order val="8"/>
           <c:tx>
             <c:strRef>
               <c:f>Population!$D$215</c:f>
@@ -19497,7 +19602,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Population!$B$198:$B$201</c:f>
+              <c:f>Population!$B$222:$B$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -19542,8 +19647,81 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="5"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Population!$D$221</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>40-49, Nyanza KNBS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Population!$B$222:$B$225</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Population!$D$222:$D$225</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>5.8398499983747545</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.4470028204570111</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2541443041895848</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000015-E7F8-4AF0-95D0-AAB85B337E39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="8"/>
+          <c:order val="10"/>
           <c:tx>
             <c:strRef>
               <c:f>Population!$C$197</c:f>
@@ -19573,7 +19751,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Population!$B$198:$B$201</c:f>
+              <c:f>Population!$B$222:$B$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -19622,7 +19800,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="9"/>
+          <c:order val="11"/>
           <c:tx>
             <c:strRef>
               <c:f>Population!$C$203</c:f>
@@ -19649,7 +19827,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Population!$B$198:$B$201</c:f>
+              <c:f>Population!$B$222:$B$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -19698,7 +19876,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
-          <c:order val="10"/>
+          <c:order val="12"/>
           <c:tx>
             <c:strRef>
               <c:f>Population!$C$209</c:f>
@@ -19725,7 +19903,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Population!$B$198:$B$201</c:f>
+              <c:f>Population!$B$222:$B$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -19774,7 +19952,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="10"/>
-          <c:order val="11"/>
+          <c:order val="13"/>
           <c:tx>
             <c:strRef>
               <c:f>Population!$C$215</c:f>
@@ -19802,7 +19980,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Population!$B$198:$B$201</c:f>
+              <c:f>Population!$B$222:$B$225</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -19846,6 +20024,81 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000D-E7F8-4AF0-95D0-AAB85B337E39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Population!$C$221</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>40-49, Kenya KNBS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Population!$B$222:$B$225</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Population!$C$222:$C$225</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6.3804945306367493</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.093696050427269</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5252004462106949</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.1196764929132392</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000014-E7F8-4AF0-95D0-AAB85B337E39}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -32072,16 +32325,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>528636</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>290511</xdr:colOff>
       <xdr:row>196</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>173830</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>217</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>222</xdr:row>
+      <xdr:rowOff>83343</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -34626,15 +34879,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y219"/>
+  <dimension ref="A1:Y231"/>
   <sheetViews>
-    <sheetView topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="I178" sqref="I178"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E229" sqref="E229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -36864,6 +37117,10 @@
       <c r="D53" s="4">
         <v>10942705</v>
       </c>
+      <c r="E53">
+        <f>C53/D53</f>
+        <v>0.19392325754920745</v>
+      </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B54">
@@ -36890,6 +37147,10 @@
       <c r="D55" s="4">
         <v>21448774</v>
       </c>
+      <c r="E55" s="37">
+        <f t="shared" ref="E55:E57" si="17">C55/D55</f>
+        <v>0.1635133084995907</v>
+      </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B56">
@@ -36901,6 +37162,25 @@
       <c r="D56" s="4">
         <v>28686607</v>
       </c>
+      <c r="E56" s="37">
+        <f t="shared" si="17"/>
+        <v>0.15310963753921822</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>2009</v>
+      </c>
+      <c r="C57" s="83">
+        <v>5442711</v>
+      </c>
+      <c r="D57">
+        <v>38610097</v>
+      </c>
+      <c r="E57" s="37">
+        <f t="shared" si="17"/>
+        <v>0.1409660017171156</v>
+      </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
@@ -37031,7 +37311,7 @@
         <v>355120</v>
       </c>
       <c r="E67" s="4">
-        <f t="shared" ref="E67:E85" si="17">SUM(C67:D67)</f>
+        <f t="shared" ref="E67:E85" si="18">SUM(C67:D67)</f>
         <v>707582</v>
       </c>
       <c r="G67" t="s">
@@ -37047,7 +37327,7 @@
         <v>4534902</v>
       </c>
       <c r="L67">
-        <f t="shared" ref="L67:L83" si="18">C67/E$85*100</f>
+        <f t="shared" ref="L67:L83" si="19">C67/E$85*100</f>
         <v>8.0247329581831046</v>
       </c>
       <c r="M67">
@@ -37082,7 +37362,7 @@
         <v>310927</v>
       </c>
       <c r="E68" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>619950</v>
       </c>
       <c r="G68" s="15" t="s">
@@ -37099,27 +37379,27 @@
       </c>
       <c r="K68" s="4"/>
       <c r="L68">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7.0357288244877951</v>
       </c>
       <c r="M68">
-        <f t="shared" ref="M68:M83" si="19">D68/E$85*100</f>
+        <f t="shared" ref="M68:M83" si="20">D68/E$85*100</f>
         <v>7.0790784382117735</v>
       </c>
       <c r="O68">
-        <f t="shared" ref="O68:O83" si="20">H68/J$85*100</f>
+        <f t="shared" ref="O68:O83" si="21">H68/J$85*100</f>
         <v>6.8415115387296943</v>
       </c>
       <c r="P68">
-        <f t="shared" ref="P68:P83" si="21">I68/J$85*100</f>
+        <f t="shared" ref="P68:P83" si="22">I68/J$85*100</f>
         <v>6.9740640033465802</v>
       </c>
       <c r="R68" s="7">
-        <f t="shared" ref="R68:R83" si="22">C68/H68*100</f>
+        <f t="shared" ref="R68:R83" si="23">C68/H68*100</f>
         <v>15.745945593399627</v>
       </c>
       <c r="S68" s="7">
-        <f t="shared" ref="S68:S83" si="23">D68/I68*100</f>
+        <f t="shared" ref="S68:S83" si="24">D68/I68*100</f>
         <v>15.541842865568986</v>
       </c>
     </row>
@@ -37134,7 +37414,7 @@
         <v>344306</v>
       </c>
       <c r="E69" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>681321</v>
       </c>
       <c r="G69" s="15" t="s">
@@ -37151,27 +37431,27 @@
         <v>4038635</v>
       </c>
       <c r="L69">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7.673041002723922</v>
       </c>
       <c r="M69">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7.8390399699831246</v>
       </c>
       <c r="O69">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.9847835180924491</v>
       </c>
       <c r="P69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>7.0939831276580909</v>
       </c>
       <c r="R69" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>16.820011429113297</v>
       </c>
       <c r="S69" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>16.919380043047106</v>
       </c>
     </row>
@@ -37186,7 +37466,7 @@
         <v>275864</v>
       </c>
       <c r="E70" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>556971</v>
       </c>
       <c r="G70" t="s">
@@ -37199,31 +37479,31 @@
         <v>1681984</v>
       </c>
       <c r="J70" s="4">
-        <f t="shared" ref="J70:J85" si="24">SUM(H70:I70)</f>
+        <f t="shared" ref="J70:J85" si="25">SUM(H70:I70)</f>
         <v>3403178</v>
       </c>
       <c r="L70">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.4001469879759467</v>
       </c>
       <c r="M70">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>6.2807761766551398</v>
       </c>
       <c r="O70">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.0001185247158899</v>
       </c>
       <c r="P70">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>5.8634316391271</v>
       </c>
       <c r="R70" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>16.332092721680418</v>
       </c>
       <c r="S70" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>16.401107263802746</v>
       </c>
     </row>
@@ -37238,7 +37518,7 @@
         <v>176491</v>
       </c>
       <c r="E71" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>401114</v>
       </c>
       <c r="G71" t="s">
@@ -37251,31 +37531,31 @@
         <v>1328529</v>
       </c>
       <c r="J71" s="4">
+        <f t="shared" si="25"/>
+        <v>2832918</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="19"/>
+        <v>5.1141388043702971</v>
+      </c>
+      <c r="M71">
+        <f t="shared" si="20"/>
+        <v>4.0182860692009195</v>
+      </c>
+      <c r="O71">
+        <f t="shared" si="21"/>
+        <v>5.2443317297636485</v>
+      </c>
+      <c r="P71">
+        <f t="shared" si="22"/>
+        <v>4.6312800669316045</v>
+      </c>
+      <c r="R71" s="7">
+        <f t="shared" si="23"/>
+        <v>14.93117803972244</v>
+      </c>
+      <c r="S71" s="7">
         <f t="shared" si="24"/>
-        <v>2832918</v>
-      </c>
-      <c r="L71">
-        <f t="shared" si="18"/>
-        <v>5.1141388043702971</v>
-      </c>
-      <c r="M71">
-        <f t="shared" si="19"/>
-        <v>4.0182860692009195</v>
-      </c>
-      <c r="O71">
-        <f t="shared" si="20"/>
-        <v>5.2443317297636485</v>
-      </c>
-      <c r="P71">
-        <f t="shared" si="21"/>
-        <v>4.6312800669316045</v>
-      </c>
-      <c r="R71" s="7">
-        <f t="shared" si="22"/>
-        <v>14.93117803972244</v>
-      </c>
-      <c r="S71" s="7">
-        <f t="shared" si="23"/>
         <v>13.284693070305579</v>
       </c>
     </row>
@@ -37290,7 +37570,7 @@
         <v>127695</v>
       </c>
       <c r="E72" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>290493</v>
       </c>
       <c r="G72" t="s">
@@ -37303,31 +37583,31 @@
         <v>1094909</v>
       </c>
       <c r="J72" s="4">
+        <f t="shared" si="25"/>
+        <v>2259503</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="19"/>
+        <v>3.706528579325695</v>
+      </c>
+      <c r="M72">
+        <f t="shared" si="20"/>
+        <v>2.9073156115983894</v>
+      </c>
+      <c r="O72">
+        <f t="shared" si="21"/>
+        <v>4.0597992051871996</v>
+      </c>
+      <c r="P72">
+        <f t="shared" si="22"/>
+        <v>3.8168758279300006</v>
+      </c>
+      <c r="R72" s="7">
+        <f t="shared" si="23"/>
+        <v>13.978948886908228</v>
+      </c>
+      <c r="S72" s="7">
         <f t="shared" si="24"/>
-        <v>2259503</v>
-      </c>
-      <c r="L72">
-        <f t="shared" si="18"/>
-        <v>3.706528579325695</v>
-      </c>
-      <c r="M72">
-        <f t="shared" si="19"/>
-        <v>2.9073156115983894</v>
-      </c>
-      <c r="O72">
-        <f t="shared" si="20"/>
-        <v>4.0597992051871996</v>
-      </c>
-      <c r="P72">
-        <f t="shared" si="21"/>
-        <v>3.8168758279300006</v>
-      </c>
-      <c r="R72" s="7">
-        <f t="shared" si="22"/>
-        <v>13.978948886908228</v>
-      </c>
-      <c r="S72" s="7">
-        <f t="shared" si="23"/>
         <v>11.662613057340838</v>
       </c>
     </row>
@@ -37342,7 +37622,7 @@
         <v>100423</v>
       </c>
       <c r="E73" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>223560</v>
       </c>
       <c r="G73" t="s">
@@ -37355,31 +37635,31 @@
         <v>840692</v>
       </c>
       <c r="J73" s="4">
+        <f t="shared" si="25"/>
+        <v>1685922</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="19"/>
+        <v>2.8035406434503378</v>
+      </c>
+      <c r="M73">
+        <f t="shared" si="20"/>
+        <v>2.2863961444343559</v>
+      </c>
+      <c r="O73">
+        <f t="shared" si="21"/>
+        <v>2.946489576797044</v>
+      </c>
+      <c r="P73">
+        <f t="shared" si="22"/>
+        <v>2.9306700132468801</v>
+      </c>
+      <c r="R73" s="7">
+        <f t="shared" si="23"/>
+        <v>14.56846065567952</v>
+      </c>
+      <c r="S73" s="7">
         <f t="shared" si="24"/>
-        <v>1685922</v>
-      </c>
-      <c r="L73">
-        <f t="shared" si="18"/>
-        <v>2.8035406434503378</v>
-      </c>
-      <c r="M73">
-        <f t="shared" si="19"/>
-        <v>2.2863961444343559</v>
-      </c>
-      <c r="O73">
-        <f t="shared" si="20"/>
-        <v>2.946489576797044</v>
-      </c>
-      <c r="P73">
-        <f t="shared" si="21"/>
-        <v>2.9306700132468801</v>
-      </c>
-      <c r="R73" s="7">
-        <f t="shared" si="22"/>
-        <v>14.56846065567952</v>
-      </c>
-      <c r="S73" s="7">
-        <f t="shared" si="23"/>
         <v>11.945278413497453</v>
       </c>
     </row>
@@ -37394,7 +37674,7 @@
         <v>90340</v>
       </c>
       <c r="E74" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>203842</v>
       </c>
       <c r="G74" t="s">
@@ -37407,31 +37687,31 @@
         <v>695263</v>
       </c>
       <c r="J74" s="4">
+        <f t="shared" si="25"/>
+        <v>1419012</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="19"/>
+        <v>2.5841742945897677</v>
+      </c>
+      <c r="M74">
+        <f t="shared" si="20"/>
+        <v>2.0568298864622614</v>
+      </c>
+      <c r="O74">
+        <f t="shared" si="21"/>
+        <v>2.5230042529456878</v>
+      </c>
+      <c r="P74">
+        <f t="shared" si="22"/>
+        <v>2.4237014571568012</v>
+      </c>
+      <c r="R74" s="7">
+        <f t="shared" si="23"/>
+        <v>15.682508715037949</v>
+      </c>
+      <c r="S74" s="7">
         <f t="shared" si="24"/>
-        <v>1419012</v>
-      </c>
-      <c r="L74">
-        <f t="shared" si="18"/>
-        <v>2.5841742945897677</v>
-      </c>
-      <c r="M74">
-        <f t="shared" si="19"/>
-        <v>2.0568298864622614</v>
-      </c>
-      <c r="O74">
-        <f t="shared" si="20"/>
-        <v>2.5230042529456878</v>
-      </c>
-      <c r="P74">
-        <f t="shared" si="21"/>
-        <v>2.4237014571568012</v>
-      </c>
-      <c r="R74" s="7">
-        <f t="shared" si="22"/>
-        <v>15.682508715037949</v>
-      </c>
-      <c r="S74" s="7">
-        <f t="shared" si="23"/>
         <v>12.993644131788978</v>
       </c>
     </row>
@@ -37446,7 +37726,7 @@
         <v>70808</v>
       </c>
       <c r="E75" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>155000</v>
       </c>
       <c r="G75" t="s">
@@ -37459,31 +37739,31 @@
         <v>516502</v>
       </c>
       <c r="J75" s="4">
+        <f t="shared" si="25"/>
+        <v>1033491</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="19"/>
+        <v>1.916854348030006</v>
+      </c>
+      <c r="M75">
+        <f t="shared" si="20"/>
+        <v>1.6121320633232215</v>
+      </c>
+      <c r="O75">
+        <f t="shared" si="21"/>
+        <v>1.8022345394966186</v>
+      </c>
+      <c r="P75">
+        <f t="shared" si="22"/>
+        <v>1.8005368472425576</v>
+      </c>
+      <c r="R75" s="7">
+        <f t="shared" si="23"/>
+        <v>16.285066026549888</v>
+      </c>
+      <c r="S75" s="7">
         <f t="shared" si="24"/>
-        <v>1033491</v>
-      </c>
-      <c r="L75">
-        <f t="shared" si="18"/>
-        <v>1.916854348030006</v>
-      </c>
-      <c r="M75">
-        <f t="shared" si="19"/>
-        <v>1.6121320633232215</v>
-      </c>
-      <c r="O75">
-        <f t="shared" si="20"/>
-        <v>1.8022345394966186</v>
-      </c>
-      <c r="P75">
-        <f t="shared" si="21"/>
-        <v>1.8005368472425576</v>
-      </c>
-      <c r="R75" s="7">
-        <f t="shared" si="22"/>
-        <v>16.285066026549888</v>
-      </c>
-      <c r="S75" s="7">
-        <f t="shared" si="23"/>
         <v>13.709143430228732</v>
       </c>
     </row>
@@ -37498,7 +37778,7 @@
         <v>58367</v>
       </c>
       <c r="E76" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>128165</v>
       </c>
       <c r="G76" t="s">
@@ -37511,31 +37791,31 @@
         <v>419341</v>
       </c>
       <c r="J76" s="4">
+        <f t="shared" si="25"/>
+        <v>838328</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="19"/>
+        <v>1.5891367325137584</v>
+      </c>
+      <c r="M76">
+        <f t="shared" si="20"/>
+        <v>1.3288796765900246</v>
+      </c>
+      <c r="O76">
+        <f t="shared" si="21"/>
+        <v>1.4605975040089243</v>
+      </c>
+      <c r="P76">
+        <f t="shared" si="22"/>
+        <v>1.4618315554625949</v>
+      </c>
+      <c r="R76" s="7">
+        <f t="shared" si="23"/>
+        <v>16.658750748829913</v>
+      </c>
+      <c r="S76" s="7">
         <f t="shared" si="24"/>
-        <v>838328</v>
-      </c>
-      <c r="L76">
-        <f t="shared" si="18"/>
-        <v>1.5891367325137584</v>
-      </c>
-      <c r="M76">
-        <f t="shared" si="19"/>
-        <v>1.3288796765900246</v>
-      </c>
-      <c r="O76">
-        <f t="shared" si="20"/>
-        <v>1.4605975040089243</v>
-      </c>
-      <c r="P76">
-        <f t="shared" si="21"/>
-        <v>1.4618315554625949</v>
-      </c>
-      <c r="R76" s="7">
-        <f t="shared" si="22"/>
-        <v>16.658750748829913</v>
-      </c>
-      <c r="S76" s="7">
-        <f t="shared" si="23"/>
         <v>13.918743933934435</v>
       </c>
     </row>
@@ -37550,7 +37830,7 @@
         <v>48982</v>
       </c>
       <c r="E77" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>103822</v>
       </c>
       <c r="G77" t="s">
@@ -37563,31 +37843,31 @@
         <v>344639</v>
       </c>
       <c r="J77" s="4">
+        <f t="shared" si="25"/>
+        <v>684806</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="19"/>
+        <v>1.2485781599910386</v>
+      </c>
+      <c r="M77">
+        <f t="shared" si="20"/>
+        <v>1.1152052412961533</v>
+      </c>
+      <c r="O77">
+        <f t="shared" si="21"/>
+        <v>1.1858293244091194</v>
+      </c>
+      <c r="P77">
+        <f t="shared" si="22"/>
+        <v>1.201418810569616</v>
+      </c>
+      <c r="R77" s="7">
+        <f t="shared" si="23"/>
+        <v>16.121493266542611</v>
+      </c>
+      <c r="S77" s="7">
         <f t="shared" si="24"/>
-        <v>684806</v>
-      </c>
-      <c r="L77">
-        <f t="shared" si="18"/>
-        <v>1.2485781599910386</v>
-      </c>
-      <c r="M77">
-        <f t="shared" si="19"/>
-        <v>1.1152052412961533</v>
-      </c>
-      <c r="O77">
-        <f t="shared" si="20"/>
-        <v>1.1858293244091194</v>
-      </c>
-      <c r="P77">
-        <f t="shared" si="21"/>
-        <v>1.201418810569616</v>
-      </c>
-      <c r="R77" s="7">
-        <f t="shared" si="22"/>
-        <v>16.121493266542611</v>
-      </c>
-      <c r="S77" s="7">
-        <f t="shared" si="23"/>
         <v>14.212552845151013</v>
       </c>
     </row>
@@ -37602,7 +37882,7 @@
         <v>33143</v>
       </c>
       <c r="E78" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>73250</v>
       </c>
       <c r="G78" t="s">
@@ -37615,31 +37895,31 @@
         <v>223591</v>
       </c>
       <c r="J78" s="4">
+        <f t="shared" si="25"/>
+        <v>459916</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="19"/>
+        <v>0.91314230967834764</v>
+      </c>
+      <c r="M78">
+        <f t="shared" si="20"/>
+        <v>0.75458836536438723</v>
+      </c>
+      <c r="O78">
+        <f t="shared" si="21"/>
+        <v>0.82383392595691274</v>
+      </c>
+      <c r="P78">
+        <f t="shared" si="22"/>
+        <v>0.77944293383532037</v>
+      </c>
+      <c r="R78" s="7">
+        <f t="shared" si="23"/>
+        <v>16.97112027927642</v>
+      </c>
+      <c r="S78" s="7">
         <f t="shared" si="24"/>
-        <v>459916</v>
-      </c>
-      <c r="L78">
-        <f t="shared" si="18"/>
-        <v>0.91314230967834764</v>
-      </c>
-      <c r="M78">
-        <f t="shared" si="19"/>
-        <v>0.75458836536438723</v>
-      </c>
-      <c r="O78">
-        <f t="shared" si="20"/>
-        <v>0.82383392595691274</v>
-      </c>
-      <c r="P78">
-        <f t="shared" si="21"/>
-        <v>0.77944293383532037</v>
-      </c>
-      <c r="R78" s="7">
-        <f t="shared" si="22"/>
-        <v>16.97112027927642</v>
-      </c>
-      <c r="S78" s="7">
-        <f t="shared" si="23"/>
         <v>14.823047439297646</v>
       </c>
     </row>
@@ -37654,7 +37934,7 @@
         <v>30966</v>
       </c>
       <c r="E79" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>70173</v>
       </c>
       <c r="G79" t="s">
@@ -37667,31 +37947,31 @@
         <v>194513</v>
       </c>
       <c r="J79" s="4">
+        <f t="shared" si="25"/>
+        <v>409228</v>
+      </c>
+      <c r="L79">
+        <f t="shared" si="19"/>
+        <v>0.89265142083823212</v>
+      </c>
+      <c r="M79">
+        <f t="shared" si="20"/>
+        <v>0.70502318202557446</v>
+      </c>
+      <c r="O79">
+        <f t="shared" si="21"/>
+        <v>0.7485010109461061</v>
+      </c>
+      <c r="P79">
+        <f t="shared" si="22"/>
+        <v>0.67807641358153803</v>
+      </c>
+      <c r="R79" s="7">
+        <f t="shared" si="23"/>
+        <v>18.260019095079524</v>
+      </c>
+      <c r="S79" s="7">
         <f t="shared" si="24"/>
-        <v>409228</v>
-      </c>
-      <c r="L79">
-        <f t="shared" si="18"/>
-        <v>0.89265142083823212</v>
-      </c>
-      <c r="M79">
-        <f t="shared" si="19"/>
-        <v>0.70502318202557446</v>
-      </c>
-      <c r="O79">
-        <f t="shared" si="20"/>
-        <v>0.7485010109461061</v>
-      </c>
-      <c r="P79">
-        <f t="shared" si="21"/>
-        <v>0.67807641358153803</v>
-      </c>
-      <c r="R79" s="7">
-        <f t="shared" si="22"/>
-        <v>18.260019095079524</v>
-      </c>
-      <c r="S79" s="7">
-        <f t="shared" si="23"/>
         <v>15.919758576547583</v>
       </c>
     </row>
@@ -37706,7 +37986,7 @@
         <v>25395</v>
       </c>
       <c r="E80" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>58795</v>
       </c>
       <c r="G80" t="s">
@@ -37719,31 +37999,31 @@
         <v>140969</v>
       </c>
       <c r="J80" s="4">
+        <f t="shared" si="25"/>
+        <v>301333</v>
+      </c>
+      <c r="L80">
+        <f t="shared" si="19"/>
+        <v>0.76043965251095347</v>
+      </c>
+      <c r="M80">
+        <f t="shared" si="20"/>
+        <v>0.57818458010525942</v>
+      </c>
+      <c r="O80">
+        <f t="shared" si="21"/>
+        <v>0.55903228055497456</v>
+      </c>
+      <c r="P80">
+        <f t="shared" si="22"/>
+        <v>0.49142090218224921</v>
+      </c>
+      <c r="R80" s="7">
+        <f t="shared" si="23"/>
+        <v>20.827617170936119</v>
+      </c>
+      <c r="S80" s="7">
         <f t="shared" si="24"/>
-        <v>301333</v>
-      </c>
-      <c r="L80">
-        <f t="shared" si="18"/>
-        <v>0.76043965251095347</v>
-      </c>
-      <c r="M80">
-        <f t="shared" si="19"/>
-        <v>0.57818458010525942</v>
-      </c>
-      <c r="O80">
-        <f t="shared" si="20"/>
-        <v>0.55903228055497456</v>
-      </c>
-      <c r="P80">
-        <f t="shared" si="21"/>
-        <v>0.49142090218224921</v>
-      </c>
-      <c r="R80" s="7">
-        <f t="shared" si="22"/>
-        <v>20.827617170936119</v>
-      </c>
-      <c r="S80" s="7">
-        <f t="shared" si="23"/>
         <v>18.014598954380041</v>
       </c>
     </row>
@@ -37758,7 +38038,7 @@
         <v>18984</v>
       </c>
       <c r="E81" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>41667</v>
       </c>
       <c r="G81" t="s">
@@ -37771,31 +38051,31 @@
         <v>118601</v>
       </c>
       <c r="J81" s="4">
+        <f t="shared" si="25"/>
+        <v>254125</v>
+      </c>
+      <c r="L81">
+        <f t="shared" si="19"/>
+        <v>0.51643870173371131</v>
+      </c>
+      <c r="M81">
+        <f t="shared" si="20"/>
+        <v>0.4322211486008366</v>
+      </c>
+      <c r="O81">
+        <f t="shared" si="21"/>
+        <v>0.47243951753468588</v>
+      </c>
+      <c r="P81">
+        <f t="shared" si="22"/>
+        <v>0.41344558321132258</v>
+      </c>
+      <c r="R81" s="7">
+        <f t="shared" si="23"/>
+        <v>16.737256869631949</v>
+      </c>
+      <c r="S81" s="7">
         <f t="shared" si="24"/>
-        <v>254125</v>
-      </c>
-      <c r="L81">
-        <f t="shared" si="18"/>
-        <v>0.51643870173371131</v>
-      </c>
-      <c r="M81">
-        <f t="shared" si="19"/>
-        <v>0.4322211486008366</v>
-      </c>
-      <c r="O81">
-        <f t="shared" si="20"/>
-        <v>0.47243951753468588</v>
-      </c>
-      <c r="P81">
-        <f t="shared" si="21"/>
-        <v>0.41344558321132258</v>
-      </c>
-      <c r="R81" s="7">
-        <f t="shared" si="22"/>
-        <v>16.737256869631949</v>
-      </c>
-      <c r="S81" s="7">
-        <f t="shared" si="23"/>
         <v>16.006610399575045</v>
       </c>
     </row>
@@ -37810,7 +38090,7 @@
         <v>12388</v>
       </c>
       <c r="E82" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>25810</v>
       </c>
       <c r="G82" t="s">
@@ -37823,31 +38103,31 @@
         <v>79166</v>
       </c>
       <c r="J82" s="4">
+        <f t="shared" si="25"/>
+        <v>160786</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="19"/>
+        <v>0.30558745556892269</v>
+      </c>
+      <c r="M82">
+        <f t="shared" si="20"/>
+        <v>0.28204570105705667</v>
+      </c>
+      <c r="O82">
+        <f t="shared" si="21"/>
+        <v>0.28452903855539291</v>
+      </c>
+      <c r="P82">
+        <f t="shared" si="22"/>
+        <v>0.27597434288503103</v>
+      </c>
+      <c r="R82" s="7">
+        <f t="shared" si="23"/>
+        <v>16.444498897329083</v>
+      </c>
+      <c r="S82" s="7">
         <f t="shared" si="24"/>
-        <v>160786</v>
-      </c>
-      <c r="L82">
-        <f t="shared" si="18"/>
-        <v>0.30558745556892269</v>
-      </c>
-      <c r="M82">
-        <f t="shared" si="19"/>
-        <v>0.28204570105705667</v>
-      </c>
-      <c r="O82">
-        <f t="shared" si="20"/>
-        <v>0.28452903855539291</v>
-      </c>
-      <c r="P82">
-        <f t="shared" si="21"/>
-        <v>0.27597434288503103</v>
-      </c>
-      <c r="R82" s="7">
-        <f t="shared" si="22"/>
-        <v>16.444498897329083</v>
-      </c>
-      <c r="S82" s="7">
-        <f t="shared" si="23"/>
         <v>15.648131773741254</v>
       </c>
     </row>
@@ -37862,7 +38142,7 @@
         <v>12850</v>
       </c>
       <c r="E83" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>27581</v>
       </c>
       <c r="G83" t="s">
@@ -37875,31 +38155,31 @@
         <v>95300</v>
       </c>
       <c r="J83" s="4">
+        <f t="shared" si="25"/>
+        <v>216338</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="19"/>
+        <v>0.33539031500415739</v>
+      </c>
+      <c r="M83">
+        <f t="shared" si="20"/>
+        <v>0.29256435732831598</v>
+      </c>
+      <c r="O83">
+        <f t="shared" si="21"/>
+        <v>0.42194101652373983</v>
+      </c>
+      <c r="P83">
+        <f t="shared" si="22"/>
+        <v>0.33221780659555183</v>
+      </c>
+      <c r="R83" s="7">
+        <f t="shared" si="23"/>
+        <v>12.170558006576448</v>
+      </c>
+      <c r="S83" s="7">
         <f t="shared" si="24"/>
-        <v>216338</v>
-      </c>
-      <c r="L83">
-        <f t="shared" si="18"/>
-        <v>0.33539031500415739</v>
-      </c>
-      <c r="M83">
-        <f t="shared" si="19"/>
-        <v>0.29256435732831598</v>
-      </c>
-      <c r="O83">
-        <f t="shared" si="20"/>
-        <v>0.42194101652373983</v>
-      </c>
-      <c r="P83">
-        <f t="shared" si="21"/>
-        <v>0.33221780659555183</v>
-      </c>
-      <c r="R83" s="7">
-        <f t="shared" si="22"/>
-        <v>12.170558006576448</v>
-      </c>
-      <c r="S83" s="7">
-        <f t="shared" si="23"/>
         <v>13.483735571878281</v>
       </c>
     </row>
@@ -37914,7 +38194,7 @@
         <v>11257</v>
       </c>
       <c r="E84" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>23100</v>
       </c>
       <c r="G84" t="s">
@@ -37927,7 +38207,7 @@
         <v>103487</v>
       </c>
       <c r="J84" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>190443</v>
       </c>
     </row>
@@ -37944,7 +38224,7 @@
         <v>2104306</v>
       </c>
       <c r="E85" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4392196</v>
       </c>
       <c r="G85" t="s">
@@ -37959,7 +38239,7 @@
         <v>14204982</v>
       </c>
       <c r="J85" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>28686000</v>
       </c>
     </row>
@@ -38046,7 +38326,7 @@
         <v>475717</v>
       </c>
       <c r="E91" s="4">
-        <f t="shared" ref="E91:E109" si="25">SUM(C91:D91)</f>
+        <f t="shared" ref="E91:E109" si="26">SUM(C91:D91)</f>
         <v>947849</v>
       </c>
       <c r="G91" t="s">
@@ -38071,7 +38351,7 @@
         <v>-7.771125257727272</v>
       </c>
       <c r="N91" s="8">
-        <f t="shared" ref="N91:N107" si="26">C91/E$109*100</f>
+        <f t="shared" ref="N91:N107" si="27">C91/E$109*100</f>
         <v>8.6745741230794735</v>
       </c>
       <c r="O91" s="8">
@@ -38098,7 +38378,7 @@
         <v>407362</v>
       </c>
       <c r="E92" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>814940</v>
       </c>
       <c r="G92" s="15" t="s">
@@ -38111,31 +38391,31 @@
         <v>2832669</v>
       </c>
       <c r="J92" s="4">
-        <f t="shared" ref="J92:J109" si="27">SUM(H92:I92)</f>
+        <f t="shared" ref="J92:J109" si="28">SUM(H92:I92)</f>
         <v>5597716</v>
       </c>
       <c r="L92" s="4">
-        <f t="shared" ref="L92:L106" si="28">H92/J$109*100</f>
+        <f t="shared" ref="L92:L106" si="29">H92/J$109*100</f>
         <v>7.1614608997226812</v>
       </c>
       <c r="M92" s="4">
-        <f t="shared" ref="M92:M107" si="29">-(I92/J$109)*100</f>
+        <f t="shared" ref="M92:M107" si="30">-(I92/J$109)*100</f>
         <v>-7.3366016148573783</v>
       </c>
       <c r="N92" s="8">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>7.4885107807487845</v>
       </c>
       <c r="O92" s="8">
-        <f t="shared" ref="O92:O107" si="30">-(D92/E$109)*100</f>
+        <f t="shared" ref="O92:O107" si="31">-(D92/E$109)*100</f>
         <v>-7.4845421702530226</v>
       </c>
       <c r="Q92" s="7">
-        <f t="shared" ref="Q92:Q107" si="31">C92/H92*100</f>
+        <f t="shared" ref="Q92:Q107" si="32">C92/H92*100</f>
         <v>14.740364268672469</v>
       </c>
       <c r="R92" s="7">
-        <f t="shared" ref="R92:R107" si="32">D92/I92*100</f>
+        <f t="shared" ref="R92:R107" si="33">D92/I92*100</f>
         <v>14.380854240294225</v>
       </c>
     </row>
@@ -38150,7 +38430,7 @@
         <v>370855</v>
       </c>
       <c r="E93" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>736716</v>
       </c>
       <c r="G93" s="15" t="s">
@@ -38163,31 +38443,31 @@
         <v>2565313</v>
       </c>
       <c r="J93" s="4">
+        <f t="shared" si="28"/>
+        <v>5034855</v>
+      </c>
+      <c r="L93" s="4">
+        <f t="shared" si="29"/>
+        <v>6.3961041071717588</v>
+      </c>
+      <c r="M93" s="4">
+        <f t="shared" si="30"/>
+        <v>-6.6441506220510149</v>
+      </c>
+      <c r="N93" s="8">
         <f t="shared" si="27"/>
-        <v>5034855</v>
-      </c>
-      <c r="L93" s="4">
-        <f t="shared" si="28"/>
-        <v>6.3961041071717588</v>
-      </c>
-      <c r="M93" s="4">
-        <f t="shared" si="29"/>
-        <v>-6.6441506220510149</v>
-      </c>
-      <c r="N93" s="8">
-        <f t="shared" si="26"/>
         <v>6.7220361323612448</v>
       </c>
       <c r="O93" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-6.8137918768790033</v>
       </c>
       <c r="Q93" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>14.814933295323588</v>
       </c>
       <c r="R93" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>14.456520510362672</v>
       </c>
     </row>
@@ -38202,7 +38482,7 @@
         <v>316129</v>
       </c>
       <c r="E94" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>629797</v>
       </c>
       <c r="G94" t="s">
@@ -38215,31 +38495,31 @@
         <v>2123653</v>
       </c>
       <c r="J94" s="4">
+        <f t="shared" si="28"/>
+        <v>4169543</v>
+      </c>
+      <c r="L94" s="4">
+        <f t="shared" si="29"/>
+        <v>5.2988470865535504</v>
+      </c>
+      <c r="M94" s="4">
+        <f t="shared" si="30"/>
+        <v>-5.500252951967461</v>
+      </c>
+      <c r="N94" s="8">
         <f t="shared" si="27"/>
-        <v>4169543</v>
-      </c>
-      <c r="L94" s="4">
-        <f t="shared" si="28"/>
-        <v>5.2988470865535504</v>
-      </c>
-      <c r="M94" s="4">
-        <f t="shared" si="29"/>
-        <v>-5.500252951967461</v>
-      </c>
-      <c r="N94" s="8">
-        <f t="shared" si="26"/>
         <v>5.7630838749292401</v>
       </c>
       <c r="O94" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-5.8083003121054935</v>
       </c>
       <c r="Q94" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>15.331616069290138</v>
       </c>
       <c r="R94" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>14.886094856363069</v>
       </c>
     </row>
@@ -38254,7 +38534,7 @@
         <v>227933</v>
       </c>
       <c r="E95" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>522624</v>
       </c>
       <c r="G95" t="s">
@@ -38267,31 +38547,31 @@
         <v>1754105</v>
       </c>
       <c r="J95" s="4">
+        <f t="shared" si="28"/>
+        <v>3775103</v>
+      </c>
+      <c r="L95" s="4">
+        <f t="shared" si="29"/>
+        <v>5.2343769040518078</v>
+      </c>
+      <c r="M95" s="4">
+        <f t="shared" si="30"/>
+        <v>-4.5431250794319418</v>
+      </c>
+      <c r="N95" s="8">
         <f t="shared" si="27"/>
-        <v>3775103</v>
-      </c>
-      <c r="L95" s="4">
-        <f t="shared" si="28"/>
-        <v>5.2343769040518078</v>
-      </c>
-      <c r="M95" s="4">
-        <f t="shared" si="29"/>
-        <v>-4.5431250794319418</v>
-      </c>
-      <c r="N95" s="8">
-        <f t="shared" si="26"/>
         <v>5.4144157204011014</v>
       </c>
       <c r="O95" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-4.187857852456248</v>
       </c>
       <c r="Q95" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>14.581459259237267</v>
       </c>
       <c r="R95" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>12.994262031064274</v>
       </c>
     </row>
@@ -38306,7 +38586,7 @@
         <v>183083</v>
       </c>
       <c r="E96" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>398538</v>
       </c>
       <c r="G96" t="s">
@@ -38319,31 +38599,31 @@
         <v>1529116</v>
       </c>
       <c r="J96" s="4">
+        <f t="shared" si="28"/>
+        <v>3201226</v>
+      </c>
+      <c r="L96" s="4">
+        <f t="shared" si="29"/>
+        <v>4.3307583505941469</v>
+      </c>
+      <c r="M96" s="4">
+        <f t="shared" si="30"/>
+        <v>-3.9604044506803495</v>
+      </c>
+      <c r="N96" s="8">
         <f t="shared" si="27"/>
-        <v>3201226</v>
-      </c>
-      <c r="L96" s="4">
-        <f t="shared" si="28"/>
-        <v>4.3307583505941469</v>
-      </c>
-      <c r="M96" s="4">
-        <f t="shared" si="29"/>
-        <v>-3.9604044506803495</v>
-      </c>
-      <c r="N96" s="8">
-        <f t="shared" si="26"/>
         <v>3.9585971035390264</v>
       </c>
       <c r="O96" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-3.3638199786834173</v>
       </c>
       <c r="Q96" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>12.885216881664482</v>
       </c>
       <c r="R96" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>11.973126957013072</v>
       </c>
     </row>
@@ -38358,7 +38638,7 @@
         <v>142868</v>
       </c>
       <c r="E97" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>296843</v>
       </c>
       <c r="G97" t="s">
@@ -38371,31 +38651,31 @@
         <v>1257035</v>
       </c>
       <c r="J97" s="4">
+        <f t="shared" si="28"/>
+        <v>2519506</v>
+      </c>
+      <c r="L97" s="4">
+        <f t="shared" si="29"/>
+        <v>3.2697949450891044</v>
+      </c>
+      <c r="M97" s="4">
+        <f t="shared" si="30"/>
+        <v>-3.2557157263811067</v>
+      </c>
+      <c r="N97" s="8">
         <f t="shared" si="27"/>
-        <v>2519506</v>
-      </c>
-      <c r="L97" s="4">
-        <f t="shared" si="28"/>
-        <v>3.2697949450891044</v>
-      </c>
-      <c r="M97" s="4">
-        <f t="shared" si="29"/>
-        <v>-3.2557157263811067</v>
-      </c>
-      <c r="N97" s="8">
-        <f t="shared" si="26"/>
         <v>2.829012967985991</v>
       </c>
       <c r="O97" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-2.6249418717988147</v>
       </c>
       <c r="Q97" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>12.196319757047885</v>
       </c>
       <c r="R97" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>11.365475106102853</v>
       </c>
     </row>
@@ -38410,7 +38690,7 @@
         <v>106733</v>
       </c>
       <c r="E98" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>230142</v>
       </c>
       <c r="G98" t="s">
@@ -38423,31 +38703,31 @@
         <v>1004361</v>
       </c>
       <c r="J98" s="4">
+        <f t="shared" si="28"/>
+        <v>2008632</v>
+      </c>
+      <c r="L98" s="4">
+        <f t="shared" si="29"/>
+        <v>2.6010579564200524</v>
+      </c>
+      <c r="M98" s="4">
+        <f t="shared" si="30"/>
+        <v>-2.6012910560675362</v>
+      </c>
+      <c r="N98" s="8">
         <f t="shared" si="27"/>
-        <v>2008632</v>
-      </c>
-      <c r="L98" s="4">
-        <f t="shared" si="28"/>
-        <v>2.6010579564200524</v>
-      </c>
-      <c r="M98" s="4">
-        <f t="shared" si="29"/>
-        <v>-2.6012910560675362</v>
-      </c>
-      <c r="N98" s="8">
-        <f t="shared" si="26"/>
         <v>2.2674178364421702</v>
       </c>
       <c r="O98" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-1.9610264076119419</v>
       </c>
       <c r="Q98" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>12.28841617451863</v>
       </c>
       <c r="R98" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>10.626955845557523</v>
       </c>
     </row>
@@ -38462,7 +38742,7 @@
         <v>77883</v>
       </c>
       <c r="E99" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>173521</v>
       </c>
       <c r="G99" t="s">
@@ -38475,31 +38755,31 @@
         <v>743594</v>
       </c>
       <c r="J99" s="4">
+        <f t="shared" si="28"/>
+        <v>1476169</v>
+      </c>
+      <c r="L99" s="4">
+        <f t="shared" si="29"/>
+        <v>1.8973663806128225</v>
+      </c>
+      <c r="M99" s="4">
+        <f t="shared" si="30"/>
+        <v>-1.9259055474530404</v>
+      </c>
+      <c r="N99" s="8">
         <f t="shared" si="27"/>
-        <v>1476169</v>
-      </c>
-      <c r="L99" s="4">
-        <f t="shared" si="28"/>
-        <v>1.8973663806128225</v>
-      </c>
-      <c r="M99" s="4">
-        <f t="shared" si="29"/>
-        <v>-1.9259055474530404</v>
-      </c>
-      <c r="N99" s="8">
-        <f t="shared" si="26"/>
         <v>1.7571757897856417</v>
       </c>
       <c r="O99" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-1.4309596816733428</v>
       </c>
       <c r="Q99" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>13.055045558475243</v>
       </c>
       <c r="R99" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>10.47386073583165</v>
       </c>
     </row>
@@ -38514,7 +38794,7 @@
         <v>75090</v>
       </c>
       <c r="E100" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>166874</v>
       </c>
       <c r="G100" t="s">
@@ -38527,31 +38807,31 @@
         <v>635276</v>
       </c>
       <c r="J100" s="4">
+        <f t="shared" si="28"/>
+        <v>1272745</v>
+      </c>
+      <c r="L100" s="4">
+        <f t="shared" si="29"/>
+        <v>1.6510422131288611</v>
+      </c>
+      <c r="M100" s="4">
+        <f t="shared" si="30"/>
+        <v>-1.6453623517185156</v>
+      </c>
+      <c r="N100" s="8">
         <f t="shared" si="27"/>
-        <v>1272745</v>
-      </c>
-      <c r="L100" s="4">
-        <f t="shared" si="28"/>
-        <v>1.6510422131288611</v>
-      </c>
-      <c r="M100" s="4">
-        <f t="shared" si="29"/>
-        <v>-1.6453623517185156</v>
-      </c>
-      <c r="N100" s="8">
-        <f t="shared" si="26"/>
         <v>1.6863654895510714</v>
       </c>
       <c r="O100" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-1.3796433431795294</v>
       </c>
       <c r="Q100" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>14.39819034337356</v>
       </c>
       <c r="R100" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>11.820059312802625</v>
       </c>
     </row>
@@ -38566,7 +38846,7 @@
         <v>60986</v>
       </c>
       <c r="E101" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>135460</v>
       </c>
       <c r="G101" t="s">
@@ -38579,31 +38859,31 @@
         <v>478346</v>
       </c>
       <c r="J101" s="4">
+        <f t="shared" si="28"/>
+        <v>956206</v>
+      </c>
+      <c r="L101" s="4">
+        <f t="shared" si="29"/>
+        <v>1.2376555282935444</v>
+      </c>
+      <c r="M101" s="4">
+        <f t="shared" si="30"/>
+        <v>-1.2389142663899548</v>
+      </c>
+      <c r="N101" s="8">
         <f t="shared" si="27"/>
-        <v>956206</v>
-      </c>
-      <c r="L101" s="4">
-        <f t="shared" si="28"/>
-        <v>1.2376555282935444</v>
-      </c>
-      <c r="M101" s="4">
-        <f t="shared" si="29"/>
-        <v>-1.2389142663899548</v>
-      </c>
-      <c r="N101" s="8">
-        <f t="shared" si="26"/>
         <v>1.3683254539879115</v>
       </c>
       <c r="O101" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-1.120507776363654</v>
       </c>
       <c r="Q101" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>15.58489934290378</v>
       </c>
       <c r="R101" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>12.749348797732186</v>
       </c>
     </row>
@@ -38618,7 +38898,7 @@
         <v>48144</v>
       </c>
       <c r="E102" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>103349</v>
       </c>
       <c r="G102" t="s">
@@ -38631,31 +38911,31 @@
         <v>359466</v>
       </c>
       <c r="J102" s="4">
+        <f t="shared" si="28"/>
+        <v>711953</v>
+      </c>
+      <c r="L102" s="4">
+        <f t="shared" si="29"/>
+        <v>0.9129399493609146</v>
+      </c>
+      <c r="M102" s="4">
+        <f t="shared" si="30"/>
+        <v>-0.93101553202521081</v>
+      </c>
+      <c r="N102" s="8">
         <f t="shared" si="27"/>
-        <v>711953</v>
-      </c>
-      <c r="L102" s="4">
-        <f t="shared" si="28"/>
-        <v>0.9129399493609146</v>
-      </c>
-      <c r="M102" s="4">
-        <f t="shared" si="29"/>
-        <v>-0.93101553202521081</v>
-      </c>
-      <c r="N102" s="8">
-        <f t="shared" si="26"/>
         <v>1.0142923260117982</v>
       </c>
       <c r="O102" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-0.88455918383320375</v>
       </c>
       <c r="Q102" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>15.661570497635374</v>
       </c>
       <c r="R102" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>13.393199913204587</v>
       </c>
     </row>
@@ -38670,7 +38950,7 @@
         <v>40141</v>
       </c>
       <c r="E103" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>86914</v>
       </c>
       <c r="G103" t="s">
@@ -38683,31 +38963,31 @@
         <v>295197</v>
       </c>
       <c r="J103" s="4">
+        <f t="shared" si="28"/>
+        <v>593778</v>
+      </c>
+      <c r="L103" s="4">
+        <f t="shared" si="29"/>
+        <v>0.77332362050268866</v>
+      </c>
+      <c r="M103" s="4">
+        <f t="shared" si="30"/>
+        <v>-0.76455907375731269</v>
+      </c>
+      <c r="N103" s="8">
         <f t="shared" si="27"/>
-        <v>593778</v>
-      </c>
-      <c r="L103" s="4">
-        <f t="shared" si="28"/>
-        <v>0.77332362050268866</v>
-      </c>
-      <c r="M103" s="4">
-        <f t="shared" si="29"/>
-        <v>-0.76455907375731269</v>
-      </c>
-      <c r="N103" s="8">
-        <f t="shared" si="26"/>
         <v>0.85936953110315795</v>
       </c>
       <c r="O103" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-0.7375184903258688</v>
       </c>
       <c r="Q103" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>15.665095903624144</v>
       </c>
       <c r="R103" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>13.598037920439571</v>
       </c>
     </row>
@@ -38722,7 +39002,7 @@
         <v>25151</v>
       </c>
       <c r="E104" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>57943</v>
       </c>
       <c r="G104" t="s">
@@ -38735,31 +39015,31 @@
         <v>183151</v>
       </c>
       <c r="J104" s="4">
+        <f t="shared" si="28"/>
+        <v>390763</v>
+      </c>
+      <c r="L104" s="4">
+        <f t="shared" si="29"/>
+        <v>0.53771426681471435</v>
+      </c>
+      <c r="M104" s="4">
+        <f t="shared" si="30"/>
+        <v>-0.47436037262480851</v>
+      </c>
+      <c r="N104" s="8">
         <f t="shared" si="27"/>
-        <v>390763</v>
-      </c>
-      <c r="L104" s="4">
-        <f t="shared" si="28"/>
-        <v>0.53771426681471435</v>
-      </c>
-      <c r="M104" s="4">
-        <f t="shared" si="29"/>
-        <v>-0.47436037262480851</v>
-      </c>
-      <c r="N104" s="8">
-        <f t="shared" si="26"/>
         <v>0.60249386748625822</v>
       </c>
       <c r="O104" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-0.46210427119867287</v>
       </c>
       <c r="Q104" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>15.794848081999113</v>
       </c>
       <c r="R104" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>13.732384753564</v>
       </c>
     </row>
@@ -38774,7 +39054,7 @@
         <v>23013</v>
       </c>
       <c r="E105" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>52517</v>
       </c>
       <c r="G105" t="s">
@@ -38787,31 +39067,31 @@
         <v>160301</v>
       </c>
       <c r="J105" s="4">
+        <f t="shared" si="28"/>
+        <v>339301</v>
+      </c>
+      <c r="L105" s="4">
+        <f t="shared" si="29"/>
+        <v>0.46360929888365732</v>
+      </c>
+      <c r="M105" s="4">
+        <f t="shared" si="30"/>
+        <v>-0.41517896212485556</v>
+      </c>
+      <c r="N105" s="8">
         <f t="shared" si="27"/>
-        <v>339301</v>
-      </c>
-      <c r="L105" s="4">
-        <f t="shared" si="28"/>
-        <v>0.46360929888365732</v>
-      </c>
-      <c r="M105" s="4">
-        <f t="shared" si="29"/>
-        <v>-0.41517896212485556</v>
-      </c>
-      <c r="N105" s="8">
-        <f t="shared" si="26"/>
         <v>0.54208279660632364</v>
       </c>
       <c r="O105" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-0.42282237656932359</v>
       </c>
       <c r="Q105" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>16.482681564245809</v>
       </c>
       <c r="R105" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>14.356117553851815</v>
       </c>
     </row>
@@ -38826,7 +39106,7 @@
         <v>15594</v>
       </c>
       <c r="E106" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>36832</v>
       </c>
       <c r="G106" t="s">
@@ -38839,31 +39119,31 @@
         <v>99833</v>
       </c>
       <c r="J106" s="4">
+        <f t="shared" si="28"/>
+        <v>218508</v>
+      </c>
+      <c r="L106" s="4">
+        <f t="shared" si="29"/>
+        <v>0.30736778516769847</v>
+      </c>
+      <c r="M106" s="4">
+        <f t="shared" si="30"/>
+        <v>-0.25856707896900644</v>
+      </c>
+      <c r="N106" s="8">
         <f t="shared" si="27"/>
-        <v>218508</v>
-      </c>
-      <c r="L106" s="4">
-        <f t="shared" si="28"/>
-        <v>0.30736778516769847</v>
-      </c>
-      <c r="M106" s="4">
-        <f t="shared" si="29"/>
-        <v>-0.25856707896900644</v>
-      </c>
-      <c r="N106" s="8">
-        <f t="shared" si="26"/>
         <v>0.3902099523564635</v>
       </c>
       <c r="O106" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-0.28651162995793827</v>
       </c>
       <c r="Q106" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>17.895934274278492</v>
       </c>
       <c r="R106" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>15.620085542856572</v>
       </c>
     </row>
@@ -38878,7 +39158,7 @@
         <v>19734</v>
       </c>
       <c r="E107" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>49371</v>
       </c>
       <c r="G107" t="s">
@@ -38891,7 +39171,7 @@
         <v>159125</v>
       </c>
       <c r="J107" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>383701</v>
       </c>
       <c r="L107" s="4">
@@ -38899,23 +39179,23 @@
         <v>0.58165096036925268</v>
       </c>
       <c r="M107" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>-0.41213312673107244</v>
       </c>
       <c r="N107" s="8">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.54452643177269555</v>
       </c>
       <c r="O107" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>-0.36257666446004577</v>
       </c>
       <c r="Q107" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>13.196868766030208</v>
       </c>
       <c r="R107" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>12.401571091908876</v>
       </c>
     </row>
@@ -38930,7 +39210,7 @@
         <v>1318</v>
       </c>
       <c r="E108" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2481</v>
       </c>
       <c r="G108" t="s">
@@ -38943,7 +39223,7 @@
         <v>11478</v>
       </c>
       <c r="J108" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>21086</v>
       </c>
     </row>
@@ -38960,7 +39240,7 @@
         <v>2617734</v>
       </c>
       <c r="E109" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>5442711</v>
       </c>
       <c r="G109" t="s">
@@ -38975,7 +39255,7 @@
         <v>19192458</v>
       </c>
       <c r="J109" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>38610097</v>
       </c>
     </row>
@@ -42311,6 +42591,170 @@
         <v>12.448317519648267</v>
       </c>
     </row>
+    <row r="221" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B221" s="37" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C221" s="37" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D221" s="37" t="s">
+        <v>1329</v>
+      </c>
+      <c r="E221" s="37" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="222" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B222" s="37">
+        <v>1979</v>
+      </c>
+      <c r="C222">
+        <f>SUM(H12:I13)/J$22*100</f>
+        <v>6.3804945306367493</v>
+      </c>
+      <c r="E222">
+        <f>SUM(O136:P137)/SUM(O128:P144)*100</f>
+        <v>6.2283021048104255</v>
+      </c>
+    </row>
+    <row r="223" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B223" s="37">
+        <v>1989</v>
+      </c>
+      <c r="C223">
+        <f>SUM(H38:I39)/J48*100</f>
+        <v>6.093696050427269</v>
+      </c>
+      <c r="D223">
+        <f>SUM(C38:D39)/E48*100</f>
+        <v>5.8398499983747545</v>
+      </c>
+      <c r="E223">
+        <f>SUM(C156:D157)/SUM(C148:D164)*100</f>
+        <v>5.6277512085148489</v>
+      </c>
+    </row>
+    <row r="224" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B224" s="37">
+        <v>1999</v>
+      </c>
+      <c r="C224">
+        <f>SUM(H75:I76)/J85*100</f>
+        <v>6.5252004462106949</v>
+      </c>
+      <c r="D224">
+        <f>SUM(C75:D76)/E85*100</f>
+        <v>6.4470028204570111</v>
+      </c>
+      <c r="E224">
+        <f>SUM(G156:H157)/SUM(G148:H164)*100</f>
+        <v>6.8439021382339202</v>
+      </c>
+    </row>
+    <row r="225" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B225" s="37">
+        <v>2009</v>
+      </c>
+      <c r="C225">
+        <f>SUM(H99:I100)/J109*100</f>
+        <v>7.1196764929132392</v>
+      </c>
+      <c r="D225">
+        <f>SUM(C99:D100)/E109*100</f>
+        <v>6.2541443041895848</v>
+      </c>
+      <c r="E225">
+        <f>SUM(K156:L157)/SUM(K148:L164)*100</f>
+        <v>7.3947238165336548</v>
+      </c>
+    </row>
+    <row r="226" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B226" s="37"/>
+    </row>
+    <row r="227" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B227" s="37" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C227" s="37" t="s">
+        <v>1330</v>
+      </c>
+      <c r="D227" s="37" t="s">
+        <v>1331</v>
+      </c>
+      <c r="E227" s="37" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="228" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B228" s="37">
+        <v>1979</v>
+      </c>
+      <c r="C228" s="37">
+        <f>SUM(H14:I19)/J22*100</f>
+        <v>8.8436690884882676</v>
+      </c>
+      <c r="D228" s="37"/>
+      <c r="E228" s="37">
+        <f>SUM(O138:P144)/SUM(O128:P144)*100</f>
+        <v>8.7303056434156332</v>
+      </c>
+      <c r="F228" s="37"/>
+    </row>
+    <row r="229" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B229" s="37">
+        <v>1989</v>
+      </c>
+      <c r="C229" s="37">
+        <f>SUM(H40:I46)/J48*100</f>
+        <v>8.6892726587972291</v>
+      </c>
+      <c r="D229" s="37">
+        <f>SUM(C40:D46)/E48*100</f>
+        <v>9.3887023182846985</v>
+      </c>
+      <c r="E229" s="37">
+        <f>SUM(C158:D164)/SUM(C148:D164)*100</f>
+        <v>7.7916762593924753</v>
+      </c>
+      <c r="F229" s="37"/>
+    </row>
+    <row r="230" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B230" s="37">
+        <v>1999</v>
+      </c>
+      <c r="C230" s="37">
+        <f>SUM(H77:I83)/J85*100</f>
+        <v>8.6681029073415594</v>
+      </c>
+      <c r="D230" s="37">
+        <f>SUM(C77:D83)/E85*100</f>
+        <v>9.1320605911029471</v>
+      </c>
+      <c r="E230" s="37">
+        <f>SUM(G158:H164)/SUM(G148:H164)*100</f>
+        <v>7.0462387449949659</v>
+      </c>
+      <c r="F230" s="37"/>
+    </row>
+    <row r="231" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B231" s="37">
+        <v>2009</v>
+      </c>
+      <c r="C231" s="37">
+        <f>SUM(H101:I107)/J109*100</f>
+        <v>9.3089898220146914</v>
+      </c>
+      <c r="D231" s="37">
+        <f>SUM(C101:D107)/E109*100</f>
+        <v>9.5979007520333148</v>
+      </c>
+      <c r="E231" s="37">
+        <f>SUM(K158:L164)/SUM(K148:L164)*100</f>
+        <v>7.546534336676511</v>
+      </c>
+      <c r="F231" s="37"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -42322,7 +42766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J203" sqref="J203"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Reduce riskAdj for Kenya
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="8100" tabRatio="835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="8100" tabRatio="835" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3156" uniqueCount="1334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3179" uniqueCount="1334">
   <si>
     <t>Metric</t>
   </si>
@@ -4781,7 +4781,7 @@
     <xf numFmtId="0" fontId="1" fillId="36" borderId="8" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4898,6 +4898,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="54" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -34888,7 +34889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A196" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H201" sqref="H201"/>
     </sheetView>
   </sheetViews>
@@ -42885,8 +42886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z212"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J203" sqref="J203"/>
+    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
+      <selection activeCell="N74" sqref="N74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44126,6 +44127,9 @@
       <c r="B60" t="s">
         <v>529</v>
       </c>
+      <c r="M60" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
@@ -44158,6 +44162,36 @@
       <c r="K61" t="s">
         <v>1247</v>
       </c>
+      <c r="M61" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="N61" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="O61" s="37" t="s">
+        <v>1246</v>
+      </c>
+      <c r="P61" s="37" t="s">
+        <v>1247</v>
+      </c>
+      <c r="Q61" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="R61" s="37" t="s">
+        <v>1246</v>
+      </c>
+      <c r="S61" s="37" t="s">
+        <v>1247</v>
+      </c>
+      <c r="T61" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="U61" s="37" t="s">
+        <v>1246</v>
+      </c>
+      <c r="V61" s="37" t="s">
+        <v>1247</v>
+      </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B62" s="21" t="s">
@@ -44190,6 +44224,36 @@
       <c r="K62" s="8">
         <v>8.7236999999999991</v>
       </c>
+      <c r="M62" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="N62" s="7">
+        <v>2.7391000000000001</v>
+      </c>
+      <c r="O62" s="7">
+        <v>1.4563999999999999</v>
+      </c>
+      <c r="P62" s="7">
+        <v>4.0217000000000001</v>
+      </c>
+      <c r="Q62" s="7">
+        <v>0.72650000000000003</v>
+      </c>
+      <c r="R62" s="7">
+        <v>7.0699999999999999E-2</v>
+      </c>
+      <c r="S62" s="7">
+        <v>1.3823000000000001</v>
+      </c>
+      <c r="T62" s="8">
+        <v>1.7202</v>
+      </c>
+      <c r="U62" s="8">
+        <v>1.0098</v>
+      </c>
+      <c r="V62" s="8">
+        <v>2.4306000000000001</v>
+      </c>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B63" s="21" t="s">
@@ -44222,6 +44286,36 @@
       <c r="K63" s="8">
         <v>13.867800000000001</v>
       </c>
+      <c r="M63" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="N63" s="7">
+        <v>6.4053000000000004</v>
+      </c>
+      <c r="O63" s="7">
+        <v>4.3030999999999997</v>
+      </c>
+      <c r="P63" s="7">
+        <v>8.5074000000000005</v>
+      </c>
+      <c r="Q63" s="7">
+        <v>1.4923999999999999</v>
+      </c>
+      <c r="R63" s="7">
+        <v>0.3841</v>
+      </c>
+      <c r="S63" s="7">
+        <v>2.6006999999999998</v>
+      </c>
+      <c r="T63" s="8">
+        <v>4.2165999999999997</v>
+      </c>
+      <c r="U63" s="8">
+        <v>2.9613</v>
+      </c>
+      <c r="V63" s="8">
+        <v>5.4720000000000004</v>
+      </c>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B64" s="21" t="s">
@@ -44254,8 +44348,38 @@
       <c r="K64" s="8">
         <v>31.781400000000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M64" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="N64" s="7">
+        <v>10.4094</v>
+      </c>
+      <c r="O64" s="7">
+        <v>7.1454000000000004</v>
+      </c>
+      <c r="P64" s="7">
+        <v>13.673500000000001</v>
+      </c>
+      <c r="Q64" s="7">
+        <v>6.5209999999999999</v>
+      </c>
+      <c r="R64" s="7">
+        <v>3.2902</v>
+      </c>
+      <c r="S64" s="7">
+        <v>9.7518999999999991</v>
+      </c>
+      <c r="T64" s="8">
+        <v>8.8091000000000008</v>
+      </c>
+      <c r="U64" s="8">
+        <v>6.2962999999999996</v>
+      </c>
+      <c r="V64" s="8">
+        <v>11.321999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B65" s="21" t="s">
         <v>140</v>
       </c>
@@ -44286,8 +44410,38 @@
       <c r="K65" s="8">
         <v>29.873699999999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M65" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="N65" s="7">
+        <v>11.0425</v>
+      </c>
+      <c r="O65" s="7">
+        <v>7.4653999999999998</v>
+      </c>
+      <c r="P65" s="7">
+        <v>14.6195</v>
+      </c>
+      <c r="Q65" s="7">
+        <v>6.8056999999999999</v>
+      </c>
+      <c r="R65" s="7">
+        <v>4.1223000000000001</v>
+      </c>
+      <c r="S65" s="7">
+        <v>9.4891000000000005</v>
+      </c>
+      <c r="T65" s="8">
+        <v>9.0631000000000004</v>
+      </c>
+      <c r="U65" s="8">
+        <v>6.5701999999999998</v>
+      </c>
+      <c r="V65" s="8">
+        <v>11.555899999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B66" s="21" t="s">
         <v>141</v>
       </c>
@@ -44318,8 +44472,38 @@
       <c r="K66" s="8">
         <v>31.8049</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M66" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="N66" s="7">
+        <v>8.7939000000000007</v>
+      </c>
+      <c r="O66" s="7">
+        <v>5.7251000000000003</v>
+      </c>
+      <c r="P66" s="7">
+        <v>11.8628</v>
+      </c>
+      <c r="Q66" s="7">
+        <v>10.4316</v>
+      </c>
+      <c r="R66" s="7">
+        <v>6.2424999999999997</v>
+      </c>
+      <c r="S66" s="7">
+        <v>14.620699999999999</v>
+      </c>
+      <c r="T66" s="8">
+        <v>9.5152000000000001</v>
+      </c>
+      <c r="U66" s="8">
+        <v>6.9627999999999997</v>
+      </c>
+      <c r="V66" s="8">
+        <v>12.067600000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
         <v>142</v>
       </c>
@@ -44350,8 +44534,38 @@
       <c r="K67" s="8">
         <v>26.101800000000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M67" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="N67" s="7">
+        <v>14.269500000000001</v>
+      </c>
+      <c r="O67" s="7">
+        <v>6.7178000000000004</v>
+      </c>
+      <c r="P67" s="7">
+        <v>21.821300000000001</v>
+      </c>
+      <c r="Q67" s="7">
+        <v>5.6688000000000001</v>
+      </c>
+      <c r="R67" s="7">
+        <v>2.5625</v>
+      </c>
+      <c r="S67" s="7">
+        <v>8.7751000000000001</v>
+      </c>
+      <c r="T67" s="8">
+        <v>10.3165</v>
+      </c>
+      <c r="U67" s="8">
+        <v>5.8135000000000003</v>
+      </c>
+      <c r="V67" s="8">
+        <v>14.819599999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B68" s="21" t="s">
         <v>143</v>
       </c>
@@ -44382,8 +44596,38 @@
       <c r="K68" s="8">
         <v>24.3047</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M68" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="N68" s="7">
+        <v>6.4074</v>
+      </c>
+      <c r="O68" s="7">
+        <v>3.5684999999999998</v>
+      </c>
+      <c r="P68" s="7">
+        <v>9.2462999999999997</v>
+      </c>
+      <c r="Q68" s="7">
+        <v>4.2521000000000004</v>
+      </c>
+      <c r="R68" s="7">
+        <v>0.86850000000000005</v>
+      </c>
+      <c r="S68" s="7">
+        <v>7.6356999999999999</v>
+      </c>
+      <c r="T68" s="8">
+        <v>5.4607000000000001</v>
+      </c>
+      <c r="U68" s="8">
+        <v>3.2890999999999999</v>
+      </c>
+      <c r="V68" s="8">
+        <v>7.6322000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B69" s="21" t="s">
         <v>392</v>
       </c>
@@ -44414,8 +44658,38 @@
       <c r="K69" s="8">
         <v>28.742100000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M69" s="37" t="s">
+        <v>392</v>
+      </c>
+      <c r="N69" s="37" t="s">
+        <v>1248</v>
+      </c>
+      <c r="O69" s="37" t="s">
+        <v>1248</v>
+      </c>
+      <c r="P69" s="37" t="s">
+        <v>1248</v>
+      </c>
+      <c r="Q69" s="7">
+        <v>9.1097999999999999</v>
+      </c>
+      <c r="R69" s="7">
+        <v>2.3006000000000002</v>
+      </c>
+      <c r="S69" s="7">
+        <v>15.9191</v>
+      </c>
+      <c r="T69" s="84">
+        <v>9.1097999999999999</v>
+      </c>
+      <c r="U69" s="8">
+        <v>2.3006000000000002</v>
+      </c>
+      <c r="V69" s="8">
+        <v>15.9191</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B70" s="21" t="s">
         <v>144</v>
       </c>
@@ -44446,21 +44720,51 @@
       <c r="K70" s="8">
         <v>17.399100000000001</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M70" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="N70" s="8">
+        <v>7.9831000000000003</v>
+      </c>
+      <c r="O70" s="8">
+        <v>6.7652000000000001</v>
+      </c>
+      <c r="P70" s="8">
+        <v>9.2010000000000005</v>
+      </c>
+      <c r="Q70" s="8">
+        <v>4.5518000000000001</v>
+      </c>
+      <c r="R70" s="8">
+        <v>3.5501999999999998</v>
+      </c>
+      <c r="S70" s="8">
+        <v>5.5533999999999999</v>
+      </c>
+      <c r="T70" s="8">
+        <v>6.3609</v>
+      </c>
+      <c r="U70" s="8">
+        <v>5.4173999999999998</v>
+      </c>
+      <c r="V70">
+        <v>7.3044000000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N73" s="2"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>483</v>
       </c>
@@ -44474,7 +44778,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B76" s="21" t="s">
         <v>473</v>
       </c>
@@ -44488,7 +44792,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B77" s="21" t="s">
         <v>480</v>
       </c>
@@ -44502,7 +44806,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B78" s="21" t="s">
         <v>474</v>
       </c>
@@ -44516,7 +44820,7 @@
         <v>0.13300000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B79" s="21" t="s">
         <v>472</v>
       </c>
@@ -44530,7 +44834,7 @@
         <v>0.16300000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B80" s="21" t="s">
         <v>471</v>
       </c>

</xml_diff>

<commit_message>
move riskAdj decline to earlier
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3179" uniqueCount="1334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3208" uniqueCount="1346">
   <si>
     <t>Metric</t>
   </si>
@@ -4054,6 +4054,42 @@
   </si>
   <si>
     <t>yanza popuation validataion, %N</t>
+  </si>
+  <si>
+    <t>Total - LCI</t>
+  </si>
+  <si>
+    <t>Total - UCI</t>
+  </si>
+  <si>
+    <t>15–19</t>
+  </si>
+  <si>
+    <t>20–24</t>
+  </si>
+  <si>
+    <t>25–29</t>
+  </si>
+  <si>
+    <t>30–34</t>
+  </si>
+  <si>
+    <t>35–39</t>
+  </si>
+  <si>
+    <t>40–44</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 45–49</t>
+  </si>
+  <si>
+    <t>50–54</t>
+  </si>
+  <si>
+    <t>55–59</t>
+  </si>
+  <si>
+    <t>60–64</t>
   </si>
 </sst>
 </file>
@@ -34136,16 +34172,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>594032</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>41583</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>92036</xdr:rowOff>
+      <xdr:colOff>389469</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -34162,8 +34198,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4251632" y="2581275"/>
-          <a:ext cx="5682943" cy="3835361"/>
+          <a:off x="5594658" y="2495550"/>
+          <a:ext cx="4615086" cy="3114675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -34174,16 +34210,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>219076</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>152402</xdr:rowOff>
+      <xdr:rowOff>47627</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>84928</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>179891</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -34200,8 +34236,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10039351" y="2628902"/>
-          <a:ext cx="5095874" cy="3780626"/>
+          <a:off x="9372601" y="2524127"/>
+          <a:ext cx="4543424" cy="3370764"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -34212,16 +34248,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>638174</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>256148</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>142899</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>218048</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>38124</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -34238,7 +34274,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5514974" y="6562725"/>
+          <a:off x="12792074" y="2628900"/>
           <a:ext cx="4561449" cy="3333774"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -34500,16 +34536,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>183</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>198</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -34526,6 +34562,82 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>383114</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8496300" y="3867151"/>
+          <a:ext cx="5974289" cy="2819400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>412806</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10715625" y="5724526"/>
+          <a:ext cx="6223056" cy="2971799"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -42884,10 +42996,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z212"/>
+  <dimension ref="A1:AD213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
-      <selection activeCell="N74" sqref="N74"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42895,12 +43007,12 @@
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>391</v>
       </c>
@@ -42915,529 +43027,631 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
     </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>80</v>
       </c>
       <c r="C3" t="s">
         <v>222</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" t="s">
         <v>217</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" t="s">
         <v>144</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1335</v>
+      </c>
+      <c r="N3" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="O3" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="L3" t="s">
+      <c r="P3" t="s">
         <v>1246</v>
       </c>
-      <c r="M3" t="s">
+      <c r="Q3" t="s">
         <v>1247</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="R3" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="O3" t="s">
+      <c r="S3" t="s">
         <v>1246</v>
       </c>
-      <c r="P3" t="s">
+      <c r="T3" t="s">
         <v>1247</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="U3" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="R3" t="s">
+      <c r="V3" t="s">
         <v>1246</v>
       </c>
-      <c r="S3" t="s">
+      <c r="W3" t="s">
         <v>1247</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>137</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
+        <v>1.6608000000000001</v>
+      </c>
+      <c r="E4" s="8">
+        <v>4.2827999999999999</v>
+      </c>
+      <c r="F4">
         <v>0.4</v>
       </c>
-      <c r="E4">
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.75190000000000001</v>
+      </c>
+      <c r="I4">
         <v>1.6</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="8">
+        <v>0.95489999999999997</v>
+      </c>
+      <c r="K4" s="8">
+        <v>2.3138000000000001</v>
+      </c>
+      <c r="N4" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="K4" s="8">
+      <c r="O4" s="8">
         <v>4.3395999999999999</v>
       </c>
-      <c r="L4" s="8">
+      <c r="P4" s="8">
         <v>0.63719999999999999</v>
       </c>
-      <c r="M4" s="8">
+      <c r="Q4" s="8">
         <v>8.0419999999999998</v>
       </c>
-      <c r="N4" s="8">
+      <c r="R4" s="8">
         <v>0.1419</v>
       </c>
-      <c r="O4" s="37">
+      <c r="S4" s="37">
         <v>0</v>
       </c>
-      <c r="P4" s="8">
+      <c r="T4" s="8">
         <v>0.43490000000000001</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="U4" s="8">
         <v>4.0270000000000001</v>
       </c>
-      <c r="R4" s="7">
+      <c r="V4" s="7">
         <v>0.75009999999999999</v>
       </c>
-      <c r="S4" s="7">
+      <c r="W4" s="7">
         <v>7.3038999999999996</v>
       </c>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="21"/>
-      <c r="Z4" s="21"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>138</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="8">
         <v>9</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
+        <v>6.4348000000000001</v>
+      </c>
+      <c r="E5" s="8">
+        <v>11.627800000000001</v>
+      </c>
+      <c r="F5">
         <v>2.4</v>
       </c>
-      <c r="E5">
+      <c r="G5" s="8">
+        <v>1.2017</v>
+      </c>
+      <c r="H5" s="8">
+        <v>3.6107</v>
+      </c>
+      <c r="I5">
         <v>6</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="8">
+        <v>4.4225000000000003</v>
+      </c>
+      <c r="K5" s="8">
+        <v>7.5117000000000003</v>
+      </c>
+      <c r="N5" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="K5" s="8">
+      <c r="O5" s="8">
         <v>29.970300000000002</v>
       </c>
-      <c r="L5" s="8">
+      <c r="P5" s="8">
         <v>19.9102</v>
       </c>
-      <c r="M5" s="8">
+      <c r="Q5" s="8">
         <v>40.0304</v>
       </c>
-      <c r="N5" s="8">
+      <c r="R5" s="8">
         <v>5.6208</v>
       </c>
-      <c r="O5" s="37">
+      <c r="S5" s="37">
         <v>0</v>
       </c>
-      <c r="P5" s="8">
+      <c r="T5" s="8">
         <v>11.2532</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="U5" s="8">
         <v>21.856100000000001</v>
       </c>
-      <c r="R5" s="7">
+      <c r="V5" s="7">
         <v>14.6593</v>
       </c>
-      <c r="S5" s="7">
+      <c r="W5" s="7">
         <v>29.052900000000001</v>
       </c>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>139</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="8">
         <v>12.9</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="8">
+        <v>9.6156000000000006</v>
+      </c>
+      <c r="E6" s="8">
+        <v>16.187200000000001</v>
+      </c>
+      <c r="F6">
         <v>7.3</v>
       </c>
-      <c r="E6">
+      <c r="G6" s="8">
+        <v>4.3966000000000003</v>
+      </c>
+      <c r="H6" s="8">
+        <v>10.2454</v>
+      </c>
+      <c r="I6">
         <v>10.4</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="8">
+        <v>7.9425999999999997</v>
+      </c>
+      <c r="K6" s="8">
+        <v>12.833500000000001</v>
+      </c>
+      <c r="N6" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="K6" s="8">
+      <c r="O6" s="8">
         <v>21.8535</v>
       </c>
-      <c r="L6" s="8">
+      <c r="P6" s="8">
         <v>9.8117999999999999</v>
       </c>
-      <c r="M6" s="8">
+      <c r="Q6" s="8">
         <v>33.895200000000003</v>
       </c>
-      <c r="N6" s="8">
+      <c r="R6" s="8">
         <v>23.183499999999999</v>
       </c>
-      <c r="O6" s="8">
+      <c r="S6" s="8">
         <v>10.3553</v>
       </c>
-      <c r="P6" s="8">
+      <c r="T6" s="8">
         <v>36.011600000000001</v>
       </c>
-      <c r="Q6" s="8">
+      <c r="U6" s="8">
         <v>18.897300000000001</v>
       </c>
-      <c r="R6" s="7">
+      <c r="V6" s="7">
         <v>12.1366</v>
       </c>
-      <c r="S6" s="7">
+      <c r="W6" s="7">
         <v>25.658000000000001</v>
       </c>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="21"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>140</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>11.7</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
+        <v>8.1616</v>
+      </c>
+      <c r="E7" s="8">
+        <v>15.2371</v>
+      </c>
+      <c r="F7">
         <v>6.6</v>
       </c>
-      <c r="E7">
+      <c r="G7" s="8">
+        <v>3.8715000000000002</v>
+      </c>
+      <c r="H7" s="8">
+        <v>9.3497000000000003</v>
+      </c>
+      <c r="I7">
         <v>9.4</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="8">
+        <v>6.9930000000000003</v>
+      </c>
+      <c r="K7" s="8">
+        <v>11.7536</v>
+      </c>
+      <c r="N7" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="K7" s="8">
+      <c r="O7" s="8">
         <v>16.320799999999998</v>
       </c>
-      <c r="L7" s="8">
+      <c r="P7" s="8">
         <v>4.9405000000000001</v>
       </c>
-      <c r="M7" s="8">
+      <c r="Q7" s="8">
         <v>27.701000000000001</v>
       </c>
-      <c r="N7" s="8">
+      <c r="R7" s="8">
         <v>17.728400000000001</v>
       </c>
-      <c r="O7" s="8">
+      <c r="S7" s="8">
         <v>1.7278</v>
       </c>
-      <c r="P7" s="8">
+      <c r="T7" s="8">
         <v>33.729100000000003</v>
       </c>
-      <c r="Q7" s="8">
+      <c r="U7" s="8">
         <v>11.5449</v>
       </c>
-      <c r="R7" s="7">
+      <c r="V7" s="7">
         <v>6.8776999999999999</v>
       </c>
-      <c r="S7" s="7">
+      <c r="W7" s="7">
         <v>16.2121</v>
       </c>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>141</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <v>11.8</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
+        <v>8.0726999999999993</v>
+      </c>
+      <c r="E8" s="8">
+        <v>15.4283</v>
+      </c>
+      <c r="F8">
         <v>8.4</v>
       </c>
-      <c r="E8">
+      <c r="G8" s="8">
+        <v>4.9302000000000001</v>
+      </c>
+      <c r="H8" s="8">
+        <v>11.888199999999999</v>
+      </c>
+      <c r="I8">
         <v>10.1</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="8">
+        <v>7.3860000000000001</v>
+      </c>
+      <c r="K8" s="8">
+        <v>12.894</v>
+      </c>
+      <c r="N8" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="K8" s="8">
+      <c r="O8" s="8">
         <v>17.982800000000001</v>
       </c>
-      <c r="L8" s="8">
+      <c r="P8" s="8">
         <v>6.2957000000000001</v>
       </c>
-      <c r="M8" s="8">
+      <c r="Q8" s="8">
         <v>29.67</v>
       </c>
-      <c r="N8" s="8">
+      <c r="R8" s="8">
         <v>19.689599999999999</v>
       </c>
-      <c r="O8" s="8">
+      <c r="S8" s="8">
         <v>2.7372000000000001</v>
       </c>
-      <c r="P8" s="8">
+      <c r="T8" s="8">
         <v>36.642099999999999</v>
       </c>
-      <c r="Q8" s="8">
+      <c r="U8" s="8">
         <v>13.7293</v>
       </c>
-      <c r="R8" s="7">
+      <c r="V8" s="7">
         <v>6.1853999999999996</v>
       </c>
-      <c r="S8" s="7">
+      <c r="W8" s="7">
         <v>21.273299999999999</v>
       </c>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>142</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
         <v>9.5</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
+        <v>5.1764999999999999</v>
+      </c>
+      <c r="E9" s="8">
+        <v>13.7669</v>
+      </c>
+      <c r="F9">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E9">
+      <c r="G9" s="8">
+        <v>4.7293000000000003</v>
+      </c>
+      <c r="H9" s="8">
+        <v>12.793799999999999</v>
+      </c>
+      <c r="I9">
         <v>9.1</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="8">
+        <v>6.0197000000000003</v>
+      </c>
+      <c r="K9" s="8">
+        <v>12.234400000000001</v>
+      </c>
+      <c r="N9" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="K9" s="8">
+      <c r="O9" s="8">
         <v>33.171199999999999</v>
       </c>
-      <c r="L9" s="8">
+      <c r="P9" s="8">
         <v>15.0959</v>
       </c>
-      <c r="M9" s="8">
+      <c r="Q9" s="8">
         <v>51.246499999999997</v>
       </c>
-      <c r="N9" s="8">
+      <c r="R9" s="8">
         <v>24.622299999999999</v>
       </c>
-      <c r="O9" s="8">
+      <c r="S9" s="8">
         <v>7.0796999999999999</v>
       </c>
-      <c r="P9" s="8">
+      <c r="T9" s="8">
         <v>42.164999999999999</v>
       </c>
-      <c r="Q9" s="8">
+      <c r="U9" s="8">
         <v>17.517399999999999</v>
       </c>
-      <c r="R9" s="7">
+      <c r="V9" s="7">
         <v>9.5665999999999993</v>
       </c>
-      <c r="S9" s="7">
+      <c r="W9" s="7">
         <v>25.4681</v>
       </c>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>143</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="8">
         <v>3.9</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="8">
+        <v>0.91690000000000005</v>
+      </c>
+      <c r="E10" s="8">
+        <v>6.8102999999999998</v>
+      </c>
+      <c r="F10">
         <v>5.2</v>
       </c>
-      <c r="E10">
+      <c r="G10" s="8">
+        <v>1.1970000000000001</v>
+      </c>
+      <c r="H10" s="8">
+        <v>9.1257000000000001</v>
+      </c>
+      <c r="I10">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="8">
+        <v>2.1457999999999999</v>
+      </c>
+      <c r="K10" s="8">
+        <v>6.7401999999999997</v>
+      </c>
+      <c r="N10" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="K10" s="8">
+      <c r="O10" s="8">
         <v>15.8049</v>
       </c>
-      <c r="L10" s="8">
+      <c r="P10" s="8">
         <v>0</v>
       </c>
-      <c r="M10" s="8">
+      <c r="Q10" s="8">
         <v>33.246600000000001</v>
       </c>
-      <c r="N10" s="8">
+      <c r="R10" s="8">
         <v>18.665800000000001</v>
       </c>
-      <c r="O10" s="8">
+      <c r="S10" s="8">
         <v>3.1282999999999999</v>
       </c>
-      <c r="P10" s="8">
+      <c r="T10" s="8">
         <v>34.203200000000002</v>
       </c>
-      <c r="Q10" s="8">
+      <c r="U10" s="8">
         <v>7.2714999999999996</v>
       </c>
-      <c r="R10" s="7">
+      <c r="V10" s="7">
         <v>2.6181000000000001</v>
       </c>
-      <c r="S10" s="7">
+      <c r="W10" s="7">
         <v>11.924899999999999</v>
       </c>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>392</v>
       </c>
-      <c r="D11">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11">
         <v>5.7</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="G11" s="8">
+        <v>2.0832999999999999</v>
+      </c>
+      <c r="H11" s="8">
+        <v>9.2460000000000004</v>
+      </c>
+      <c r="N11" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="K11" t="s">
+      <c r="O11" t="s">
         <v>1248</v>
       </c>
-      <c r="L11" t="s">
+      <c r="P11" t="s">
         <v>1248</v>
       </c>
-      <c r="M11" t="s">
+      <c r="Q11" t="s">
         <v>1248</v>
       </c>
-      <c r="N11" s="8">
+      <c r="R11" s="8">
         <v>20.7746</v>
       </c>
-      <c r="O11" s="8">
+      <c r="S11" s="8">
         <v>4.2534999999999998</v>
       </c>
-      <c r="P11" s="8">
+      <c r="T11" s="8">
         <v>37.295699999999997</v>
       </c>
-      <c r="Q11" s="8">
+      <c r="U11" s="8">
         <v>5.1565000000000003</v>
       </c>
-      <c r="R11" s="7">
+      <c r="V11" s="7">
         <v>0.3695</v>
       </c>
-      <c r="S11" s="7">
+      <c r="W11" s="7">
         <v>9.9436</v>
       </c>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="21"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>144</v>
       </c>
-      <c r="C12">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="D12">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E12">
+      <c r="C12" s="8">
+        <v>8.6816999999999993</v>
+      </c>
+      <c r="D12" s="8">
+        <v>7.4393000000000002</v>
+      </c>
+      <c r="E12" s="8">
+        <v>9.9242000000000008</v>
+      </c>
+      <c r="F12" s="8">
+        <v>4.6345999999999998</v>
+      </c>
+      <c r="G12" s="8">
+        <v>3.7299000000000002</v>
+      </c>
+      <c r="H12" s="8">
+        <v>5.5392000000000001</v>
+      </c>
+      <c r="I12">
         <v>6.7</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="7">
+        <v>5.7725999999999997</v>
+      </c>
+      <c r="K12" s="7">
+        <v>7.6139000000000001</v>
+      </c>
+      <c r="N12" t="s">
         <v>144</v>
       </c>
-      <c r="K12" s="8">
+      <c r="O12" s="8">
         <v>18.2517</v>
       </c>
-      <c r="L12" s="8">
+      <c r="P12" s="8">
         <v>13.379</v>
       </c>
-      <c r="M12" s="8">
+      <c r="Q12" s="8">
         <v>23.124400000000001</v>
       </c>
-      <c r="N12" s="8">
+      <c r="R12" s="8">
         <v>12.285500000000001</v>
       </c>
-      <c r="O12" s="8">
+      <c r="S12" s="8">
         <v>7.8247999999999998</v>
       </c>
-      <c r="P12" s="8">
+      <c r="T12" s="8">
         <v>16.746300000000002</v>
       </c>
-      <c r="Q12" s="8">
+      <c r="U12" s="8">
         <v>15.355399999999999</v>
       </c>
-      <c r="R12" s="7">
+      <c r="V12" s="7">
         <v>11.407500000000001</v>
       </c>
-      <c r="S12" s="7">
+      <c r="W12" s="7">
         <v>19.3032</v>
       </c>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="21"/>
-      <c r="W12" s="21"/>
       <c r="X12" s="21"/>
-      <c r="Y12" s="21"/>
-      <c r="Z12" s="21"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>158</v>
-      </c>
-      <c r="C13">
-        <v>18.3</v>
-      </c>
-      <c r="D13">
-        <v>1.6</v>
-      </c>
-      <c r="E13">
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="D13" s="8">
+        <f>C12-D12</f>
+        <v>1.2423999999999991</v>
+      </c>
+      <c r="E13" s="8">
+        <f>E12-C12</f>
+        <v>1.2425000000000015</v>
+      </c>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13">
         <v>15.1</v>
       </c>
-      <c r="K13" t="s">
+      <c r="O13" t="s">
         <v>531</v>
       </c>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
       <c r="W13" s="21"/>
       <c r="X13" s="21"/>
       <c r="Y13" s="21"/>
       <c r="Z13" s="21"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA13" s="21"/>
+      <c r="AB13" s="21"/>
+      <c r="AC13" s="21"/>
+      <c r="AD13" s="21"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="S14" s="21"/>
       <c r="T14" s="21"/>
       <c r="U14" s="21"/>
@@ -43447,12 +43661,12 @@
       <c r="Y14" s="21"/>
       <c r="Z14" s="21"/>
     </row>
-    <row r="15" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
         <v>28</v>
       </c>
@@ -43627,6 +43841,12 @@
       <c r="E28" s="19">
         <v>7.0999999999999994E-2</v>
       </c>
+      <c r="F28" s="19">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G28" s="19">
+        <v>7.9000000000000001E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="21" t="s">
@@ -43640,6 +43860,14 @@
       </c>
       <c r="E29" s="19">
         <v>0.14899999999999999</v>
+      </c>
+      <c r="F29" s="18">
+        <f>0.072-F28</f>
+        <v>5.9999999999999915E-3</v>
+      </c>
+      <c r="G29" s="18">
+        <f>G28-0.072</f>
+        <v>7.0000000000000062E-3</v>
       </c>
     </row>
     <row r="30" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -43674,6 +43902,9 @@
       </c>
       <c r="D32" s="54"/>
       <c r="E32" s="54"/>
+      <c r="F32" t="s">
+        <v>153</v>
+      </c>
       <c r="S32" s="21"/>
       <c r="T32" s="21"/>
       <c r="U32" s="21"/>
@@ -43695,6 +43926,36 @@
         <v>223</v>
       </c>
       <c r="E33" s="54"/>
+      <c r="F33" s="54" t="s">
+        <v>246</v>
+      </c>
+      <c r="G33" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="H33" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="I33" s="54" t="s">
+        <v>576</v>
+      </c>
+      <c r="J33" s="54" t="s">
+        <v>222</v>
+      </c>
+      <c r="K33" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="L33" s="54" t="s">
+        <v>576</v>
+      </c>
+      <c r="M33" s="54" t="s">
+        <v>223</v>
+      </c>
+      <c r="N33" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="O33" s="54" t="s">
+        <v>576</v>
+      </c>
       <c r="T33" s="21"/>
       <c r="U33" s="21"/>
       <c r="V33" s="21"/>
@@ -43715,6 +43976,24 @@
         <v>0.02</v>
       </c>
       <c r="E34" s="54"/>
+      <c r="F34" t="s">
+        <v>1336</v>
+      </c>
+      <c r="G34" s="37">
+        <v>1</v>
+      </c>
+      <c r="H34" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="I34" s="40">
+        <v>1.6</v>
+      </c>
+      <c r="J34" s="40">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M34">
+        <v>0.9</v>
+      </c>
       <c r="T34" s="21"/>
       <c r="U34" s="21"/>
       <c r="V34" s="21"/>
@@ -43735,6 +44014,24 @@
         <v>2.93E-2</v>
       </c>
       <c r="E35" s="54"/>
+      <c r="F35" t="s">
+        <v>1337</v>
+      </c>
+      <c r="G35" s="37">
+        <v>3.1</v>
+      </c>
+      <c r="H35" s="40">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I35" s="40">
+        <v>4</v>
+      </c>
+      <c r="J35" s="40">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="M35">
+        <v>1.3</v>
+      </c>
       <c r="T35" s="21"/>
       <c r="U35" s="21"/>
       <c r="V35" s="21"/>
@@ -43755,6 +44052,24 @@
         <v>0.21</v>
       </c>
       <c r="E36" s="54"/>
+      <c r="F36" t="s">
+        <v>1338</v>
+      </c>
+      <c r="G36" s="37">
+        <v>6.3</v>
+      </c>
+      <c r="H36" s="40">
+        <v>4.8</v>
+      </c>
+      <c r="I36" s="40">
+        <v>7.7</v>
+      </c>
+      <c r="J36" s="40">
+        <v>7.9</v>
+      </c>
+      <c r="M36">
+        <v>4.3</v>
+      </c>
       <c r="T36" s="21"/>
       <c r="U36" s="21"/>
       <c r="V36" s="21"/>
@@ -43775,6 +44090,24 @@
         <v>0.24</v>
       </c>
       <c r="E37" s="54"/>
+      <c r="F37" t="s">
+        <v>1339</v>
+      </c>
+      <c r="G37" s="37">
+        <v>6.6</v>
+      </c>
+      <c r="H37" s="40">
+        <v>5.2</v>
+      </c>
+      <c r="I37" s="40">
+        <v>8</v>
+      </c>
+      <c r="J37" s="40">
+        <v>6.6</v>
+      </c>
+      <c r="M37">
+        <v>6.6</v>
+      </c>
       <c r="T37" s="21"/>
       <c r="U37" s="21"/>
       <c r="V37" s="21"/>
@@ -43795,6 +44128,24 @@
         <v>0.2</v>
       </c>
       <c r="E38" s="54"/>
+      <c r="F38" t="s">
+        <v>1340</v>
+      </c>
+      <c r="G38" s="37">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="H38" s="40">
+        <v>6.7</v>
+      </c>
+      <c r="I38" s="40">
+        <v>10.7</v>
+      </c>
+      <c r="J38" s="40">
+        <v>12.3</v>
+      </c>
+      <c r="M38">
+        <v>5</v>
+      </c>
       <c r="T38" s="21"/>
       <c r="U38" s="21"/>
       <c r="V38" s="21"/>
@@ -43815,6 +44166,24 @@
         <v>0.31</v>
       </c>
       <c r="E39" s="54"/>
+      <c r="F39" t="s">
+        <v>1341</v>
+      </c>
+      <c r="G39" s="37">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H39" s="40">
+        <v>7.1</v>
+      </c>
+      <c r="I39" s="40">
+        <v>11.6</v>
+      </c>
+      <c r="J39" s="40">
+        <v>10.6</v>
+      </c>
+      <c r="M39">
+        <v>8.1</v>
+      </c>
       <c r="T39" s="21"/>
       <c r="U39" s="21"/>
       <c r="V39" s="21"/>
@@ -43835,6 +44204,24 @@
         <v>0.16</v>
       </c>
       <c r="E40" s="54"/>
+      <c r="F40" s="21" t="s">
+        <v>1342</v>
+      </c>
+      <c r="G40" s="37">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="H40" s="40">
+        <v>7.1</v>
+      </c>
+      <c r="I40" s="40">
+        <v>12.5</v>
+      </c>
+      <c r="J40" s="40">
+        <v>10.7</v>
+      </c>
+      <c r="M40" s="21">
+        <v>8.9</v>
+      </c>
     </row>
     <row r="41" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="54"/>
@@ -43848,6 +44235,24 @@
         <v>0.21</v>
       </c>
       <c r="E41" s="54"/>
+      <c r="F41" s="21" t="s">
+        <v>1343</v>
+      </c>
+      <c r="G41" s="37">
+        <v>8.4</v>
+      </c>
+      <c r="H41" s="40">
+        <v>6.3</v>
+      </c>
+      <c r="I41" s="40">
+        <v>10.5</v>
+      </c>
+      <c r="J41" s="40">
+        <v>10</v>
+      </c>
+      <c r="M41" s="21">
+        <v>7</v>
+      </c>
     </row>
     <row r="42" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="54"/>
@@ -43861,6 +44266,24 @@
         <v>0.12</v>
       </c>
       <c r="E42" s="54"/>
+      <c r="F42" s="21" t="s">
+        <v>1344</v>
+      </c>
+      <c r="G42" s="37">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H42" s="40">
+        <v>2.4</v>
+      </c>
+      <c r="I42" s="40">
+        <v>6.4</v>
+      </c>
+      <c r="J42" s="40">
+        <v>5</v>
+      </c>
+      <c r="M42" s="21">
+        <v>4</v>
+      </c>
     </row>
     <row r="43" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="54"/>
@@ -43874,6 +44297,24 @@
         <v>0.12</v>
       </c>
       <c r="E43" s="54"/>
+      <c r="F43" s="21" t="s">
+        <v>1345</v>
+      </c>
+      <c r="G43" s="37">
+        <v>4</v>
+      </c>
+      <c r="H43" s="40">
+        <v>2</v>
+      </c>
+      <c r="I43" s="40">
+        <v>6.1</v>
+      </c>
+      <c r="J43" s="40">
+        <v>3</v>
+      </c>
+      <c r="M43" s="21">
+        <v>5</v>
+      </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="54"/>
@@ -43887,6 +44328,36 @@
         <v>5.11E-2</v>
       </c>
       <c r="E44" s="54"/>
+      <c r="F44" t="s">
+        <v>144</v>
+      </c>
+      <c r="G44">
+        <v>5.6</v>
+      </c>
+      <c r="H44" s="40">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I44" s="40">
+        <v>6.3</v>
+      </c>
+      <c r="J44" s="40">
+        <v>6.9</v>
+      </c>
+      <c r="K44" s="40">
+        <v>6</v>
+      </c>
+      <c r="L44" s="40">
+        <v>7.7</v>
+      </c>
+      <c r="M44" s="40">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N44" s="40">
+        <v>3.6</v>
+      </c>
+      <c r="O44" s="40">
+        <v>5.2</v>
+      </c>
       <c r="T44" s="21"/>
       <c r="U44" s="21"/>
       <c r="V44" s="21"/>
@@ -43907,6 +44378,14 @@
         <v>1.6500000000000001E-2</v>
       </c>
       <c r="E45" s="54"/>
+      <c r="H45">
+        <f>G44-H44</f>
+        <v>0.69999999999999929</v>
+      </c>
+      <c r="I45">
+        <f>I44-G44</f>
+        <v>0.70000000000000018</v>
+      </c>
       <c r="T45" s="21"/>
       <c r="U45" s="21"/>
       <c r="V45" s="21"/>
@@ -44747,8 +45226,26 @@
       <c r="U70" s="8">
         <v>5.4173999999999998</v>
       </c>
-      <c r="V70">
+      <c r="V70" s="8">
         <v>7.3044000000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="O71" s="8">
+        <f>N70-O70</f>
+        <v>1.2179000000000002</v>
+      </c>
+      <c r="P71" s="8">
+        <f>P70-N70</f>
+        <v>1.2179000000000002</v>
+      </c>
+      <c r="U71" s="8">
+        <f>T70-U70</f>
+        <v>0.94350000000000023</v>
+      </c>
+      <c r="V71" s="8">
+        <f>V70-T70</f>
+        <v>0.94350000000000023</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
@@ -45922,7 +46419,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>1011</v>
       </c>
@@ -45945,7 +46442,7 @@
         <v>23.7</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>156</v>
       </c>
@@ -45968,7 +46465,7 @@
         <v>41.1</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>157</v>
       </c>
@@ -45991,7 +46488,7 @@
         <v>38.6</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>1012</v>
       </c>
@@ -46014,12 +46511,12 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>1325</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>500</v>
       </c>
@@ -46035,8 +46532,26 @@
       <c r="G183" t="s">
         <v>1326</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I183" t="s">
+        <v>222</v>
+      </c>
+      <c r="J183" t="s">
+        <v>575</v>
+      </c>
+      <c r="K183" t="s">
+        <v>576</v>
+      </c>
+      <c r="L183" t="s">
+        <v>223</v>
+      </c>
+      <c r="M183" t="s">
+        <v>575</v>
+      </c>
+      <c r="N183" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="184" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B184">
         <v>1990</v>
       </c>
@@ -46053,8 +46568,27 @@
         <f>E184-D184</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I184" s="40">
+        <v>5.9</v>
+      </c>
+      <c r="J184" s="40">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K184" s="40">
+        <v>7.1</v>
+      </c>
+      <c r="L184" s="40">
+        <v>5.3</v>
+      </c>
+      <c r="M184" s="40">
+        <v>4.2</v>
+      </c>
+      <c r="N184" s="40">
+        <v>6.3</v>
+      </c>
+      <c r="P184" s="37"/>
+    </row>
+    <row r="185" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B185">
         <v>1991</v>
       </c>
@@ -46072,8 +46606,28 @@
         <f t="shared" ref="G185:G212" si="0">E185-D185</f>
         <v>2.4000000000000004</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I185" s="40">
+        <v>7.6</v>
+      </c>
+      <c r="J185" s="40">
+        <v>6.4</v>
+      </c>
+      <c r="K185" s="40">
+        <v>9.1</v>
+      </c>
+      <c r="L185" s="40">
+        <v>6.4</v>
+      </c>
+      <c r="M185" s="40">
+        <v>5.2</v>
+      </c>
+      <c r="N185" s="40">
+        <v>7.8</v>
+      </c>
+      <c r="P185" s="37"/>
+      <c r="Q185" s="37"/>
+    </row>
+    <row r="186" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B186">
         <v>1992</v>
       </c>
@@ -46091,8 +46645,28 @@
         <f t="shared" si="0"/>
         <v>2.9000000000000004</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I186" s="40">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J186" s="40">
+        <v>7.8</v>
+      </c>
+      <c r="K186" s="40">
+        <v>11.1</v>
+      </c>
+      <c r="L186" s="40">
+        <v>7.5</v>
+      </c>
+      <c r="M186" s="40">
+        <v>6</v>
+      </c>
+      <c r="N186" s="40">
+        <v>9</v>
+      </c>
+      <c r="P186" s="37"/>
+      <c r="Q186" s="37"/>
+    </row>
+    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B187" s="37">
         <v>1993</v>
       </c>
@@ -46110,8 +46684,28 @@
         <f t="shared" si="0"/>
         <v>3.3000000000000007</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I187" s="40">
+        <v>10.8</v>
+      </c>
+      <c r="J187" s="40">
+        <v>9</v>
+      </c>
+      <c r="K187" s="40">
+        <v>12.9</v>
+      </c>
+      <c r="L187" s="40">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="M187" s="40">
+        <v>6.7</v>
+      </c>
+      <c r="N187" s="40">
+        <v>10.1</v>
+      </c>
+      <c r="P187" s="37"/>
+      <c r="Q187" s="37"/>
+    </row>
+    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B188" s="37">
         <v>1994</v>
       </c>
@@ -46129,8 +46723,28 @@
         <f t="shared" si="0"/>
         <v>3.5999999999999996</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I188" s="40">
+        <v>11.9</v>
+      </c>
+      <c r="J188" s="40">
+        <v>9.9</v>
+      </c>
+      <c r="K188" s="40">
+        <v>14.2</v>
+      </c>
+      <c r="L188" s="40">
+        <v>8.9</v>
+      </c>
+      <c r="M188" s="40">
+        <v>7.2</v>
+      </c>
+      <c r="N188" s="40">
+        <v>10.7</v>
+      </c>
+      <c r="P188" s="37"/>
+      <c r="Q188" s="37"/>
+    </row>
+    <row r="189" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B189" s="37">
         <v>1995</v>
       </c>
@@ -46148,8 +46762,28 @@
         <f t="shared" si="0"/>
         <v>3.6999999999999993</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I189" s="40">
+        <v>12.6</v>
+      </c>
+      <c r="J189" s="40">
+        <v>10.5</v>
+      </c>
+      <c r="K189" s="40">
+        <v>15</v>
+      </c>
+      <c r="L189" s="40">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="M189" s="40">
+        <v>7.4</v>
+      </c>
+      <c r="N189" s="40">
+        <v>11.1</v>
+      </c>
+      <c r="P189" s="37"/>
+      <c r="Q189" s="37"/>
+    </row>
+    <row r="190" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B190" s="37">
         <v>1996</v>
       </c>
@@ -46167,8 +46801,28 @@
         <f t="shared" si="0"/>
         <v>3.7999999999999989</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I190" s="40">
+        <v>12.9</v>
+      </c>
+      <c r="J190" s="40">
+        <v>10.7</v>
+      </c>
+      <c r="K190" s="40">
+        <v>15.4</v>
+      </c>
+      <c r="L190" s="40">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="M190" s="40">
+        <v>7.4</v>
+      </c>
+      <c r="N190" s="40">
+        <v>11.1</v>
+      </c>
+      <c r="P190" s="37"/>
+      <c r="Q190" s="37"/>
+    </row>
+    <row r="191" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B191" s="37">
         <v>1997</v>
       </c>
@@ -46186,8 +46840,28 @@
         <f t="shared" si="0"/>
         <v>3.7999999999999989</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I191" s="40">
+        <v>12.9</v>
+      </c>
+      <c r="J191" s="40">
+        <v>10.7</v>
+      </c>
+      <c r="K191" s="40">
+        <v>15.4</v>
+      </c>
+      <c r="L191" s="40">
+        <v>9</v>
+      </c>
+      <c r="M191" s="40">
+        <v>7.3</v>
+      </c>
+      <c r="N191" s="40">
+        <v>10.9</v>
+      </c>
+      <c r="P191" s="37"/>
+      <c r="Q191" s="37"/>
+    </row>
+    <row r="192" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B192" s="37">
         <v>1998</v>
       </c>
@@ -46205,8 +46879,28 @@
         <f t="shared" si="0"/>
         <v>3.7000000000000011</v>
       </c>
-    </row>
-    <row r="193" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I192" s="40">
+        <v>12.7</v>
+      </c>
+      <c r="J192" s="40">
+        <v>10.6</v>
+      </c>
+      <c r="K192" s="40">
+        <v>15.2</v>
+      </c>
+      <c r="L192" s="40">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="M192" s="40">
+        <v>7</v>
+      </c>
+      <c r="N192" s="40">
+        <v>10.5</v>
+      </c>
+      <c r="P192" s="37"/>
+      <c r="Q192" s="37"/>
+    </row>
+    <row r="193" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B193" s="37">
         <v>1999</v>
       </c>
@@ -46224,8 +46918,28 @@
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-    </row>
-    <row r="194" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I193" s="40">
+        <v>12.3</v>
+      </c>
+      <c r="J193" s="40">
+        <v>10.3</v>
+      </c>
+      <c r="K193" s="40">
+        <v>14.7</v>
+      </c>
+      <c r="L193" s="40">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="M193" s="40">
+        <v>6.7</v>
+      </c>
+      <c r="N193" s="40">
+        <v>10</v>
+      </c>
+      <c r="P193" s="37"/>
+      <c r="Q193" s="37"/>
+    </row>
+    <row r="194" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B194" s="37">
         <v>2000</v>
       </c>
@@ -46243,8 +46957,28 @@
         <f t="shared" si="0"/>
         <v>3.2999999999999989</v>
       </c>
-    </row>
-    <row r="195" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I194" s="40">
+        <v>11.8</v>
+      </c>
+      <c r="J194" s="40">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="K194" s="40">
+        <v>14.1</v>
+      </c>
+      <c r="L194" s="40">
+        <v>7.8</v>
+      </c>
+      <c r="M194" s="40">
+        <v>6.3</v>
+      </c>
+      <c r="N194" s="40">
+        <v>9.5</v>
+      </c>
+      <c r="P194" s="37"/>
+      <c r="Q194" s="37"/>
+    </row>
+    <row r="195" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B195" s="37">
         <v>2001</v>
       </c>
@@ -46262,8 +46996,28 @@
         <f t="shared" si="0"/>
         <v>3.1999999999999993</v>
       </c>
-    </row>
-    <row r="196" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I195" s="40">
+        <v>11.2</v>
+      </c>
+      <c r="J195" s="40">
+        <v>9.4</v>
+      </c>
+      <c r="K195" s="40">
+        <v>13.5</v>
+      </c>
+      <c r="L195" s="40">
+        <v>7.3</v>
+      </c>
+      <c r="M195" s="40">
+        <v>5.9</v>
+      </c>
+      <c r="N195" s="40">
+        <v>8.9</v>
+      </c>
+      <c r="P195" s="37"/>
+      <c r="Q195" s="37"/>
+    </row>
+    <row r="196" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B196" s="37">
         <v>2002</v>
       </c>
@@ -46281,8 +47035,28 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="197" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I196" s="40">
+        <v>10.6</v>
+      </c>
+      <c r="J196" s="40">
+        <v>8.9</v>
+      </c>
+      <c r="K196" s="40">
+        <v>12.7</v>
+      </c>
+      <c r="L196" s="40">
+        <v>6.9</v>
+      </c>
+      <c r="M196" s="40">
+        <v>5.5</v>
+      </c>
+      <c r="N196" s="40">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="P196" s="37"/>
+      <c r="Q196" s="37"/>
+    </row>
+    <row r="197" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B197" s="37">
         <v>2003</v>
       </c>
@@ -46300,8 +47074,28 @@
         <f t="shared" si="0"/>
         <v>2.8000000000000007</v>
       </c>
-    </row>
-    <row r="198" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I197" s="40">
+        <v>10</v>
+      </c>
+      <c r="J197" s="40">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K197" s="40">
+        <v>12</v>
+      </c>
+      <c r="L197" s="40">
+        <v>6.4</v>
+      </c>
+      <c r="M197" s="40">
+        <v>5.2</v>
+      </c>
+      <c r="N197" s="40">
+        <v>7.7</v>
+      </c>
+      <c r="P197" s="37"/>
+      <c r="Q197" s="37"/>
+    </row>
+    <row r="198" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B198" s="37">
         <v>2004</v>
       </c>
@@ -46319,8 +47113,28 @@
         <f t="shared" si="0"/>
         <v>2.6999999999999993</v>
       </c>
-    </row>
-    <row r="199" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I198" s="40">
+        <v>9.4</v>
+      </c>
+      <c r="J198" s="40">
+        <v>7.9</v>
+      </c>
+      <c r="K198" s="40">
+        <v>11.3</v>
+      </c>
+      <c r="L198" s="40">
+        <v>5.9</v>
+      </c>
+      <c r="M198" s="40">
+        <v>4.8</v>
+      </c>
+      <c r="N198" s="40">
+        <v>7.2</v>
+      </c>
+      <c r="P198" s="37"/>
+      <c r="Q198" s="37"/>
+    </row>
+    <row r="199" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B199" s="37">
         <v>2005</v>
       </c>
@@ -46338,8 +47152,28 @@
         <f t="shared" si="0"/>
         <v>2.4999999999999991</v>
       </c>
-    </row>
-    <row r="200" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I199" s="40">
+        <v>8.9</v>
+      </c>
+      <c r="J199" s="40">
+        <v>7.4</v>
+      </c>
+      <c r="K199" s="40">
+        <v>10.7</v>
+      </c>
+      <c r="L199" s="40">
+        <v>5.6</v>
+      </c>
+      <c r="M199" s="40">
+        <v>4.5</v>
+      </c>
+      <c r="N199" s="40">
+        <v>6.7</v>
+      </c>
+      <c r="P199" s="37"/>
+      <c r="Q199" s="37"/>
+    </row>
+    <row r="200" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B200" s="37">
         <v>2006</v>
       </c>
@@ -46357,8 +47191,28 @@
         <f t="shared" si="0"/>
         <v>2.2999999999999989</v>
       </c>
-    </row>
-    <row r="201" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I200" s="40">
+        <v>8.5</v>
+      </c>
+      <c r="J200" s="40">
+        <v>7.1</v>
+      </c>
+      <c r="K200" s="40">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="L200" s="40">
+        <v>5.3</v>
+      </c>
+      <c r="M200" s="40">
+        <v>4.3</v>
+      </c>
+      <c r="N200" s="40">
+        <v>6.4</v>
+      </c>
+      <c r="P200" s="37"/>
+      <c r="Q200" s="37"/>
+    </row>
+    <row r="201" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B201" s="37">
         <v>2007</v>
       </c>
@@ -46376,8 +47230,28 @@
         <f t="shared" si="0"/>
         <v>2.3000000000000007</v>
       </c>
-    </row>
-    <row r="202" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I201" s="40">
+        <v>8.1</v>
+      </c>
+      <c r="J201" s="40">
+        <v>6.8</v>
+      </c>
+      <c r="K201" s="40">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="L201" s="40">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="M201" s="40">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N201" s="40">
+        <v>6.1</v>
+      </c>
+      <c r="P201" s="37"/>
+      <c r="Q201" s="37"/>
+    </row>
+    <row r="202" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B202" s="37">
         <v>2008</v>
       </c>
@@ -46395,8 +47269,28 @@
         <f t="shared" si="0"/>
         <v>2.1999999999999993</v>
       </c>
-    </row>
-    <row r="203" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I202" s="40">
+        <v>7.9</v>
+      </c>
+      <c r="J202" s="40">
+        <v>6.5</v>
+      </c>
+      <c r="K202" s="40">
+        <v>9.4</v>
+      </c>
+      <c r="L202" s="40">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="M202" s="40">
+        <v>3.9</v>
+      </c>
+      <c r="N202" s="40">
+        <v>5.9</v>
+      </c>
+      <c r="P202" s="37"/>
+      <c r="Q202" s="37"/>
+    </row>
+    <row r="203" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B203" s="37">
         <v>2009</v>
       </c>
@@ -46414,8 +47308,28 @@
         <f t="shared" si="0"/>
         <v>2.0999999999999996</v>
       </c>
-    </row>
-    <row r="204" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I203" s="40">
+        <v>7.6</v>
+      </c>
+      <c r="J203" s="40">
+        <v>6.3</v>
+      </c>
+      <c r="K203" s="40">
+        <v>9.1</v>
+      </c>
+      <c r="L203" s="40">
+        <v>4.7</v>
+      </c>
+      <c r="M203" s="40">
+        <v>3.8</v>
+      </c>
+      <c r="N203" s="40">
+        <v>5.7</v>
+      </c>
+      <c r="P203" s="37"/>
+      <c r="Q203" s="37"/>
+    </row>
+    <row r="204" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B204" s="37">
         <v>2010</v>
       </c>
@@ -46433,8 +47347,28 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="205" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I204" s="40">
+        <v>7.4</v>
+      </c>
+      <c r="J204" s="40">
+        <v>6.1</v>
+      </c>
+      <c r="K204" s="40">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="L204" s="40">
+        <v>4.5</v>
+      </c>
+      <c r="M204" s="40">
+        <v>3.7</v>
+      </c>
+      <c r="N204" s="40">
+        <v>5.5</v>
+      </c>
+      <c r="P204" s="37"/>
+      <c r="Q204" s="37"/>
+    </row>
+    <row r="205" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B205" s="37">
         <v>2011</v>
       </c>
@@ -46452,8 +47386,28 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="206" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I205" s="40">
+        <v>7.1</v>
+      </c>
+      <c r="J205" s="40">
+        <v>5.9</v>
+      </c>
+      <c r="K205" s="40">
+        <v>8.5</v>
+      </c>
+      <c r="L205" s="40">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M205" s="40">
+        <v>3.6</v>
+      </c>
+      <c r="N205" s="40">
+        <v>5.3</v>
+      </c>
+      <c r="P205" s="37"/>
+      <c r="Q205" s="37"/>
+    </row>
+    <row r="206" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B206" s="37">
         <v>2012</v>
       </c>
@@ -46471,8 +47425,28 @@
         <f t="shared" si="0"/>
         <v>1.9000000000000004</v>
       </c>
-    </row>
-    <row r="207" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I206" s="40">
+        <v>7</v>
+      </c>
+      <c r="J206" s="40">
+        <v>5.8</v>
+      </c>
+      <c r="K206" s="40">
+        <v>8.4</v>
+      </c>
+      <c r="L206" s="40">
+        <v>4.3</v>
+      </c>
+      <c r="M206" s="40">
+        <v>3.4</v>
+      </c>
+      <c r="N206" s="40">
+        <v>5.2</v>
+      </c>
+      <c r="P206" s="37"/>
+      <c r="Q206" s="37"/>
+    </row>
+    <row r="207" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B207" s="37">
         <v>2013</v>
       </c>
@@ -46490,8 +47464,28 @@
         <f t="shared" si="0"/>
         <v>1.8999999999999995</v>
       </c>
-    </row>
-    <row r="208" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I207" s="40">
+        <v>6.9</v>
+      </c>
+      <c r="J207" s="40">
+        <v>5.7</v>
+      </c>
+      <c r="K207" s="40">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="L207" s="40">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="M207" s="40">
+        <v>3.3</v>
+      </c>
+      <c r="N207" s="40">
+        <v>5</v>
+      </c>
+      <c r="P207" s="37"/>
+      <c r="Q207" s="37"/>
+    </row>
+    <row r="208" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B208" s="37">
         <v>2014</v>
       </c>
@@ -46509,8 +47503,28 @@
         <f t="shared" si="0"/>
         <v>1.8000000000000007</v>
       </c>
-    </row>
-    <row r="209" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I208" s="40">
+        <v>6.7</v>
+      </c>
+      <c r="J208" s="40">
+        <v>5.6</v>
+      </c>
+      <c r="K208" s="40">
+        <v>8.1</v>
+      </c>
+      <c r="L208" s="40">
+        <v>4</v>
+      </c>
+      <c r="M208" s="40">
+        <v>3.2</v>
+      </c>
+      <c r="N208" s="40">
+        <v>4.8</v>
+      </c>
+      <c r="P208" s="37"/>
+      <c r="Q208" s="37"/>
+    </row>
+    <row r="209" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B209" s="37">
         <v>2015</v>
       </c>
@@ -46528,8 +47542,28 @@
         <f t="shared" si="0"/>
         <v>1.7999999999999998</v>
       </c>
-    </row>
-    <row r="210" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I209" s="40">
+        <v>6.6</v>
+      </c>
+      <c r="J209" s="40">
+        <v>5.5</v>
+      </c>
+      <c r="K209" s="40">
+        <v>7.9</v>
+      </c>
+      <c r="L209" s="40">
+        <v>3.8</v>
+      </c>
+      <c r="M209" s="40">
+        <v>3.1</v>
+      </c>
+      <c r="N209" s="40">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="P209" s="37"/>
+      <c r="Q209" s="37"/>
+    </row>
+    <row r="210" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B210" s="37">
         <v>2016</v>
       </c>
@@ -46547,8 +47581,28 @@
         <f t="shared" si="0"/>
         <v>1.7000000000000002</v>
       </c>
-    </row>
-    <row r="211" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I210" s="40">
+        <v>6.4</v>
+      </c>
+      <c r="J210" s="40">
+        <v>5.3</v>
+      </c>
+      <c r="K210" s="40">
+        <v>7.7</v>
+      </c>
+      <c r="L210" s="40">
+        <v>3.7</v>
+      </c>
+      <c r="M210" s="40">
+        <v>3</v>
+      </c>
+      <c r="N210" s="40">
+        <v>4.5</v>
+      </c>
+      <c r="P210" s="37"/>
+      <c r="Q210" s="37"/>
+    </row>
+    <row r="211" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B211" s="37">
         <v>2017</v>
       </c>
@@ -46566,8 +47620,28 @@
         <f t="shared" si="0"/>
         <v>1.5999999999999996</v>
       </c>
-    </row>
-    <row r="212" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I211" s="40">
+        <v>6.2</v>
+      </c>
+      <c r="J211" s="40">
+        <v>5.2</v>
+      </c>
+      <c r="K211" s="40">
+        <v>7.5</v>
+      </c>
+      <c r="L211" s="40">
+        <v>3.5</v>
+      </c>
+      <c r="M211" s="40">
+        <v>2.9</v>
+      </c>
+      <c r="N211" s="40">
+        <v>4.3</v>
+      </c>
+      <c r="P211" s="37"/>
+      <c r="Q211" s="37"/>
+    </row>
+    <row r="212" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B212" s="37">
         <v>2018</v>
       </c>
@@ -46584,6 +47658,32 @@
       <c r="G212" s="37">
         <f t="shared" si="0"/>
         <v>1.7000000000000002</v>
+      </c>
+      <c r="I212" s="40">
+        <v>6.1</v>
+      </c>
+      <c r="J212" s="40">
+        <v>5</v>
+      </c>
+      <c r="K212" s="40">
+        <v>7.2</v>
+      </c>
+      <c r="L212" s="40">
+        <v>3.4</v>
+      </c>
+      <c r="M212" s="40">
+        <v>2.8</v>
+      </c>
+      <c r="N212" s="40">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="P212" s="37"/>
+      <c r="Q212" s="37"/>
+    </row>
+    <row r="213" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K213" s="37" t="str">
+        <f t="shared" ref="K185:K213" si="1">LEFT(L213,4)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reduced riskAdj to reduce HIV prevalence in Nyanza
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="8100" tabRatio="835" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="4770" tabRatio="835" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="10" r:id="rId1"/>
@@ -4930,11 +4930,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="54" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="54" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5054,7 +5054,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5862,7 +5861,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7385,7 +7383,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9336,7 +9333,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9439,7 +9435,6 @@
         <c:idx val="13"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9521,7 +9516,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9954,7 +9948,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10061,7 +10054,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10553,7 +10545,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10665,7 +10656,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11122,7 +11112,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11234,7 +11223,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12047,7 +12035,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12167,7 +12154,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12795,7 +12781,6 @@
         <c:idx val="2"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14067,7 +14052,6 @@
         <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14174,7 +14158,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14642,7 +14625,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14757,7 +14739,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15864,7 +15845,6 @@
         <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15979,7 +15959,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17027,7 +17006,6 @@
         <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17134,7 +17112,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18086,7 +18063,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18193,7 +18169,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18814,7 +18789,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20435,7 +20409,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21033,7 +21006,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21140,7 +21112,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21738,7 +21709,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -32370,15 +32340,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>52385</xdr:colOff>
-      <xdr:row>201</xdr:row>
-      <xdr:rowOff>126205</xdr:rowOff>
+      <xdr:colOff>611979</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>7143</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>190499</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
       <xdr:row>230</xdr:row>
-      <xdr:rowOff>35719</xdr:rowOff>
+      <xdr:rowOff>107157</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -35001,8 +34971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y231"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H201" sqref="H201"/>
+    <sheetView topLeftCell="A166" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I178" sqref="I178:O184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37268,7 +37238,7 @@
         <v>21448774</v>
       </c>
       <c r="E55" s="37">
-        <f t="shared" ref="E55:E57" si="17">C55/D55</f>
+        <f>C55/D55</f>
         <v>0.1635133084995907</v>
       </c>
     </row>
@@ -37283,7 +37253,7 @@
         <v>28686607</v>
       </c>
       <c r="E56" s="37">
-        <f t="shared" si="17"/>
+        <f>C56/D56</f>
         <v>0.15310963753921822</v>
       </c>
     </row>
@@ -37291,14 +37261,14 @@
       <c r="B57">
         <v>2009</v>
       </c>
-      <c r="C57" s="83">
+      <c r="C57" s="82">
         <v>5442711</v>
       </c>
       <c r="D57">
         <v>38610097</v>
       </c>
       <c r="E57" s="37">
-        <f t="shared" si="17"/>
+        <f>C57/D57</f>
         <v>0.1409660017171156</v>
       </c>
     </row>
@@ -37431,7 +37401,7 @@
         <v>355120</v>
       </c>
       <c r="E67" s="4">
-        <f t="shared" ref="E67:E85" si="18">SUM(C67:D67)</f>
+        <f t="shared" ref="E67:E85" si="17">SUM(C67:D67)</f>
         <v>707582</v>
       </c>
       <c r="G67" t="s">
@@ -37447,7 +37417,7 @@
         <v>4534902</v>
       </c>
       <c r="L67">
-        <f t="shared" ref="L67:L83" si="19">C67/E$85*100</f>
+        <f t="shared" ref="L67:L83" si="18">C67/E$85*100</f>
         <v>8.0247329581831046</v>
       </c>
       <c r="M67">
@@ -37482,7 +37452,7 @@
         <v>310927</v>
       </c>
       <c r="E68" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>619950</v>
       </c>
       <c r="G68" s="15" t="s">
@@ -37499,27 +37469,27 @@
       </c>
       <c r="K68" s="4"/>
       <c r="L68">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>7.0357288244877951</v>
       </c>
       <c r="M68">
-        <f t="shared" ref="M68:M83" si="20">D68/E$85*100</f>
+        <f t="shared" ref="M68:M83" si="19">D68/E$85*100</f>
         <v>7.0790784382117735</v>
       </c>
       <c r="O68">
-        <f t="shared" ref="O68:O83" si="21">H68/J$85*100</f>
+        <f t="shared" ref="O68:O83" si="20">H68/J$85*100</f>
         <v>6.8415115387296943</v>
       </c>
       <c r="P68">
-        <f t="shared" ref="P68:P83" si="22">I68/J$85*100</f>
+        <f t="shared" ref="P68:P83" si="21">I68/J$85*100</f>
         <v>6.9740640033465802</v>
       </c>
       <c r="R68" s="7">
-        <f t="shared" ref="R68:R83" si="23">C68/H68*100</f>
+        <f t="shared" ref="R68:R83" si="22">C68/H68*100</f>
         <v>15.745945593399627</v>
       </c>
       <c r="S68" s="7">
-        <f t="shared" ref="S68:S83" si="24">D68/I68*100</f>
+        <f t="shared" ref="S68:S83" si="23">D68/I68*100</f>
         <v>15.541842865568986</v>
       </c>
     </row>
@@ -37534,7 +37504,7 @@
         <v>344306</v>
       </c>
       <c r="E69" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>681321</v>
       </c>
       <c r="G69" s="15" t="s">
@@ -37551,27 +37521,27 @@
         <v>4038635</v>
       </c>
       <c r="L69">
+        <f t="shared" si="18"/>
+        <v>7.673041002723922</v>
+      </c>
+      <c r="M69">
         <f t="shared" si="19"/>
-        <v>7.673041002723922</v>
-      </c>
-      <c r="M69">
+        <v>7.8390399699831246</v>
+      </c>
+      <c r="O69">
         <f t="shared" si="20"/>
-        <v>7.8390399699831246</v>
-      </c>
-      <c r="O69">
+        <v>6.9847835180924491</v>
+      </c>
+      <c r="P69">
         <f t="shared" si="21"/>
-        <v>6.9847835180924491</v>
-      </c>
-      <c r="P69">
+        <v>7.0939831276580909</v>
+      </c>
+      <c r="R69" s="7">
         <f t="shared" si="22"/>
-        <v>7.0939831276580909</v>
-      </c>
-      <c r="R69" s="7">
+        <v>16.820011429113297</v>
+      </c>
+      <c r="S69" s="7">
         <f t="shared" si="23"/>
-        <v>16.820011429113297</v>
-      </c>
-      <c r="S69" s="7">
-        <f t="shared" si="24"/>
         <v>16.919380043047106</v>
       </c>
     </row>
@@ -37586,7 +37556,7 @@
         <v>275864</v>
       </c>
       <c r="E70" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>556971</v>
       </c>
       <c r="G70" t="s">
@@ -37599,31 +37569,31 @@
         <v>1681984</v>
       </c>
       <c r="J70" s="4">
-        <f t="shared" ref="J70:J85" si="25">SUM(H70:I70)</f>
+        <f t="shared" ref="J70:J85" si="24">SUM(H70:I70)</f>
         <v>3403178</v>
       </c>
       <c r="L70">
+        <f t="shared" si="18"/>
+        <v>6.4001469879759467</v>
+      </c>
+      <c r="M70">
         <f t="shared" si="19"/>
-        <v>6.4001469879759467</v>
-      </c>
-      <c r="M70">
+        <v>6.2807761766551398</v>
+      </c>
+      <c r="O70">
         <f t="shared" si="20"/>
-        <v>6.2807761766551398</v>
-      </c>
-      <c r="O70">
+        <v>6.0001185247158899</v>
+      </c>
+      <c r="P70">
         <f t="shared" si="21"/>
-        <v>6.0001185247158899</v>
-      </c>
-      <c r="P70">
+        <v>5.8634316391271</v>
+      </c>
+      <c r="R70" s="7">
         <f t="shared" si="22"/>
-        <v>5.8634316391271</v>
-      </c>
-      <c r="R70" s="7">
+        <v>16.332092721680418</v>
+      </c>
+      <c r="S70" s="7">
         <f t="shared" si="23"/>
-        <v>16.332092721680418</v>
-      </c>
-      <c r="S70" s="7">
-        <f t="shared" si="24"/>
         <v>16.401107263802746</v>
       </c>
     </row>
@@ -37638,7 +37608,7 @@
         <v>176491</v>
       </c>
       <c r="E71" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>401114</v>
       </c>
       <c r="G71" t="s">
@@ -37651,31 +37621,31 @@
         <v>1328529</v>
       </c>
       <c r="J71" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>2832918</v>
       </c>
       <c r="L71">
+        <f t="shared" si="18"/>
+        <v>5.1141388043702971</v>
+      </c>
+      <c r="M71">
         <f t="shared" si="19"/>
-        <v>5.1141388043702971</v>
-      </c>
-      <c r="M71">
+        <v>4.0182860692009195</v>
+      </c>
+      <c r="O71">
         <f t="shared" si="20"/>
-        <v>4.0182860692009195</v>
-      </c>
-      <c r="O71">
+        <v>5.2443317297636485</v>
+      </c>
+      <c r="P71">
         <f t="shared" si="21"/>
-        <v>5.2443317297636485</v>
-      </c>
-      <c r="P71">
+        <v>4.6312800669316045</v>
+      </c>
+      <c r="R71" s="7">
         <f t="shared" si="22"/>
-        <v>4.6312800669316045</v>
-      </c>
-      <c r="R71" s="7">
+        <v>14.93117803972244</v>
+      </c>
+      <c r="S71" s="7">
         <f t="shared" si="23"/>
-        <v>14.93117803972244</v>
-      </c>
-      <c r="S71" s="7">
-        <f t="shared" si="24"/>
         <v>13.284693070305579</v>
       </c>
     </row>
@@ -37690,7 +37660,7 @@
         <v>127695</v>
       </c>
       <c r="E72" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>290493</v>
       </c>
       <c r="G72" t="s">
@@ -37703,31 +37673,31 @@
         <v>1094909</v>
       </c>
       <c r="J72" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>2259503</v>
       </c>
       <c r="L72">
+        <f t="shared" si="18"/>
+        <v>3.706528579325695</v>
+      </c>
+      <c r="M72">
         <f t="shared" si="19"/>
-        <v>3.706528579325695</v>
-      </c>
-      <c r="M72">
+        <v>2.9073156115983894</v>
+      </c>
+      <c r="O72">
         <f t="shared" si="20"/>
-        <v>2.9073156115983894</v>
-      </c>
-      <c r="O72">
+        <v>4.0597992051871996</v>
+      </c>
+      <c r="P72">
         <f t="shared" si="21"/>
-        <v>4.0597992051871996</v>
-      </c>
-      <c r="P72">
+        <v>3.8168758279300006</v>
+      </c>
+      <c r="R72" s="7">
         <f t="shared" si="22"/>
-        <v>3.8168758279300006</v>
-      </c>
-      <c r="R72" s="7">
+        <v>13.978948886908228</v>
+      </c>
+      <c r="S72" s="7">
         <f t="shared" si="23"/>
-        <v>13.978948886908228</v>
-      </c>
-      <c r="S72" s="7">
-        <f t="shared" si="24"/>
         <v>11.662613057340838</v>
       </c>
     </row>
@@ -37742,7 +37712,7 @@
         <v>100423</v>
       </c>
       <c r="E73" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>223560</v>
       </c>
       <c r="G73" t="s">
@@ -37755,31 +37725,31 @@
         <v>840692</v>
       </c>
       <c r="J73" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>1685922</v>
       </c>
       <c r="L73">
+        <f t="shared" si="18"/>
+        <v>2.8035406434503378</v>
+      </c>
+      <c r="M73">
         <f t="shared" si="19"/>
-        <v>2.8035406434503378</v>
-      </c>
-      <c r="M73">
+        <v>2.2863961444343559</v>
+      </c>
+      <c r="O73">
         <f t="shared" si="20"/>
-        <v>2.2863961444343559</v>
-      </c>
-      <c r="O73">
+        <v>2.946489576797044</v>
+      </c>
+      <c r="P73">
         <f t="shared" si="21"/>
-        <v>2.946489576797044</v>
-      </c>
-      <c r="P73">
+        <v>2.9306700132468801</v>
+      </c>
+      <c r="R73" s="7">
         <f t="shared" si="22"/>
-        <v>2.9306700132468801</v>
-      </c>
-      <c r="R73" s="7">
+        <v>14.56846065567952</v>
+      </c>
+      <c r="S73" s="7">
         <f t="shared" si="23"/>
-        <v>14.56846065567952</v>
-      </c>
-      <c r="S73" s="7">
-        <f t="shared" si="24"/>
         <v>11.945278413497453</v>
       </c>
     </row>
@@ -37794,7 +37764,7 @@
         <v>90340</v>
       </c>
       <c r="E74" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>203842</v>
       </c>
       <c r="G74" t="s">
@@ -37807,31 +37777,31 @@
         <v>695263</v>
       </c>
       <c r="J74" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>1419012</v>
       </c>
       <c r="L74">
+        <f t="shared" si="18"/>
+        <v>2.5841742945897677</v>
+      </c>
+      <c r="M74">
         <f t="shared" si="19"/>
-        <v>2.5841742945897677</v>
-      </c>
-      <c r="M74">
+        <v>2.0568298864622614</v>
+      </c>
+      <c r="O74">
         <f t="shared" si="20"/>
-        <v>2.0568298864622614</v>
-      </c>
-      <c r="O74">
+        <v>2.5230042529456878</v>
+      </c>
+      <c r="P74">
         <f t="shared" si="21"/>
-        <v>2.5230042529456878</v>
-      </c>
-      <c r="P74">
+        <v>2.4237014571568012</v>
+      </c>
+      <c r="R74" s="7">
         <f t="shared" si="22"/>
-        <v>2.4237014571568012</v>
-      </c>
-      <c r="R74" s="7">
+        <v>15.682508715037949</v>
+      </c>
+      <c r="S74" s="7">
         <f t="shared" si="23"/>
-        <v>15.682508715037949</v>
-      </c>
-      <c r="S74" s="7">
-        <f t="shared" si="24"/>
         <v>12.993644131788978</v>
       </c>
     </row>
@@ -37846,7 +37816,7 @@
         <v>70808</v>
       </c>
       <c r="E75" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>155000</v>
       </c>
       <c r="G75" t="s">
@@ -37859,31 +37829,31 @@
         <v>516502</v>
       </c>
       <c r="J75" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>1033491</v>
       </c>
       <c r="L75">
+        <f t="shared" si="18"/>
+        <v>1.916854348030006</v>
+      </c>
+      <c r="M75">
         <f t="shared" si="19"/>
-        <v>1.916854348030006</v>
-      </c>
-      <c r="M75">
+        <v>1.6121320633232215</v>
+      </c>
+      <c r="O75">
         <f t="shared" si="20"/>
-        <v>1.6121320633232215</v>
-      </c>
-      <c r="O75">
+        <v>1.8022345394966186</v>
+      </c>
+      <c r="P75">
         <f t="shared" si="21"/>
-        <v>1.8022345394966186</v>
-      </c>
-      <c r="P75">
+        <v>1.8005368472425576</v>
+      </c>
+      <c r="R75" s="7">
         <f t="shared" si="22"/>
-        <v>1.8005368472425576</v>
-      </c>
-      <c r="R75" s="7">
+        <v>16.285066026549888</v>
+      </c>
+      <c r="S75" s="7">
         <f t="shared" si="23"/>
-        <v>16.285066026549888</v>
-      </c>
-      <c r="S75" s="7">
-        <f t="shared" si="24"/>
         <v>13.709143430228732</v>
       </c>
     </row>
@@ -37898,7 +37868,7 @@
         <v>58367</v>
       </c>
       <c r="E76" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>128165</v>
       </c>
       <c r="G76" t="s">
@@ -37911,31 +37881,31 @@
         <v>419341</v>
       </c>
       <c r="J76" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>838328</v>
       </c>
       <c r="L76">
+        <f t="shared" si="18"/>
+        <v>1.5891367325137584</v>
+      </c>
+      <c r="M76">
         <f t="shared" si="19"/>
-        <v>1.5891367325137584</v>
-      </c>
-      <c r="M76">
+        <v>1.3288796765900246</v>
+      </c>
+      <c r="O76">
         <f t="shared" si="20"/>
-        <v>1.3288796765900246</v>
-      </c>
-      <c r="O76">
+        <v>1.4605975040089243</v>
+      </c>
+      <c r="P76">
         <f t="shared" si="21"/>
-        <v>1.4605975040089243</v>
-      </c>
-      <c r="P76">
+        <v>1.4618315554625949</v>
+      </c>
+      <c r="R76" s="7">
         <f t="shared" si="22"/>
-        <v>1.4618315554625949</v>
-      </c>
-      <c r="R76" s="7">
+        <v>16.658750748829913</v>
+      </c>
+      <c r="S76" s="7">
         <f t="shared" si="23"/>
-        <v>16.658750748829913</v>
-      </c>
-      <c r="S76" s="7">
-        <f t="shared" si="24"/>
         <v>13.918743933934435</v>
       </c>
     </row>
@@ -37950,7 +37920,7 @@
         <v>48982</v>
       </c>
       <c r="E77" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>103822</v>
       </c>
       <c r="G77" t="s">
@@ -37963,31 +37933,31 @@
         <v>344639</v>
       </c>
       <c r="J77" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>684806</v>
       </c>
       <c r="L77">
+        <f t="shared" si="18"/>
+        <v>1.2485781599910386</v>
+      </c>
+      <c r="M77">
         <f t="shared" si="19"/>
-        <v>1.2485781599910386</v>
-      </c>
-      <c r="M77">
+        <v>1.1152052412961533</v>
+      </c>
+      <c r="O77">
         <f t="shared" si="20"/>
-        <v>1.1152052412961533</v>
-      </c>
-      <c r="O77">
+        <v>1.1858293244091194</v>
+      </c>
+      <c r="P77">
         <f t="shared" si="21"/>
-        <v>1.1858293244091194</v>
-      </c>
-      <c r="P77">
+        <v>1.201418810569616</v>
+      </c>
+      <c r="R77" s="7">
         <f t="shared" si="22"/>
-        <v>1.201418810569616</v>
-      </c>
-      <c r="R77" s="7">
+        <v>16.121493266542611</v>
+      </c>
+      <c r="S77" s="7">
         <f t="shared" si="23"/>
-        <v>16.121493266542611</v>
-      </c>
-      <c r="S77" s="7">
-        <f t="shared" si="24"/>
         <v>14.212552845151013</v>
       </c>
     </row>
@@ -38002,7 +37972,7 @@
         <v>33143</v>
       </c>
       <c r="E78" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>73250</v>
       </c>
       <c r="G78" t="s">
@@ -38015,31 +37985,31 @@
         <v>223591</v>
       </c>
       <c r="J78" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>459916</v>
       </c>
       <c r="L78">
+        <f t="shared" si="18"/>
+        <v>0.91314230967834764</v>
+      </c>
+      <c r="M78">
         <f t="shared" si="19"/>
-        <v>0.91314230967834764</v>
-      </c>
-      <c r="M78">
+        <v>0.75458836536438723</v>
+      </c>
+      <c r="O78">
         <f t="shared" si="20"/>
-        <v>0.75458836536438723</v>
-      </c>
-      <c r="O78">
+        <v>0.82383392595691274</v>
+      </c>
+      <c r="P78">
         <f t="shared" si="21"/>
-        <v>0.82383392595691274</v>
-      </c>
-      <c r="P78">
+        <v>0.77944293383532037</v>
+      </c>
+      <c r="R78" s="7">
         <f t="shared" si="22"/>
-        <v>0.77944293383532037</v>
-      </c>
-      <c r="R78" s="7">
+        <v>16.97112027927642</v>
+      </c>
+      <c r="S78" s="7">
         <f t="shared" si="23"/>
-        <v>16.97112027927642</v>
-      </c>
-      <c r="S78" s="7">
-        <f t="shared" si="24"/>
         <v>14.823047439297646</v>
       </c>
     </row>
@@ -38054,7 +38024,7 @@
         <v>30966</v>
       </c>
       <c r="E79" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>70173</v>
       </c>
       <c r="G79" t="s">
@@ -38067,31 +38037,31 @@
         <v>194513</v>
       </c>
       <c r="J79" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>409228</v>
       </c>
       <c r="L79">
+        <f t="shared" si="18"/>
+        <v>0.89265142083823212</v>
+      </c>
+      <c r="M79">
         <f t="shared" si="19"/>
-        <v>0.89265142083823212</v>
-      </c>
-      <c r="M79">
+        <v>0.70502318202557446</v>
+      </c>
+      <c r="O79">
         <f t="shared" si="20"/>
-        <v>0.70502318202557446</v>
-      </c>
-      <c r="O79">
+        <v>0.7485010109461061</v>
+      </c>
+      <c r="P79">
         <f t="shared" si="21"/>
-        <v>0.7485010109461061</v>
-      </c>
-      <c r="P79">
+        <v>0.67807641358153803</v>
+      </c>
+      <c r="R79" s="7">
         <f t="shared" si="22"/>
-        <v>0.67807641358153803</v>
-      </c>
-      <c r="R79" s="7">
+        <v>18.260019095079524</v>
+      </c>
+      <c r="S79" s="7">
         <f t="shared" si="23"/>
-        <v>18.260019095079524</v>
-      </c>
-      <c r="S79" s="7">
-        <f t="shared" si="24"/>
         <v>15.919758576547583</v>
       </c>
     </row>
@@ -38106,7 +38076,7 @@
         <v>25395</v>
       </c>
       <c r="E80" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>58795</v>
       </c>
       <c r="G80" t="s">
@@ -38119,31 +38089,31 @@
         <v>140969</v>
       </c>
       <c r="J80" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>301333</v>
       </c>
       <c r="L80">
+        <f t="shared" si="18"/>
+        <v>0.76043965251095347</v>
+      </c>
+      <c r="M80">
         <f t="shared" si="19"/>
-        <v>0.76043965251095347</v>
-      </c>
-      <c r="M80">
+        <v>0.57818458010525942</v>
+      </c>
+      <c r="O80">
         <f t="shared" si="20"/>
-        <v>0.57818458010525942</v>
-      </c>
-      <c r="O80">
+        <v>0.55903228055497456</v>
+      </c>
+      <c r="P80">
         <f t="shared" si="21"/>
-        <v>0.55903228055497456</v>
-      </c>
-      <c r="P80">
+        <v>0.49142090218224921</v>
+      </c>
+      <c r="R80" s="7">
         <f t="shared" si="22"/>
-        <v>0.49142090218224921</v>
-      </c>
-      <c r="R80" s="7">
+        <v>20.827617170936119</v>
+      </c>
+      <c r="S80" s="7">
         <f t="shared" si="23"/>
-        <v>20.827617170936119</v>
-      </c>
-      <c r="S80" s="7">
-        <f t="shared" si="24"/>
         <v>18.014598954380041</v>
       </c>
     </row>
@@ -38158,7 +38128,7 @@
         <v>18984</v>
       </c>
       <c r="E81" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>41667</v>
       </c>
       <c r="G81" t="s">
@@ -38171,31 +38141,31 @@
         <v>118601</v>
       </c>
       <c r="J81" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>254125</v>
       </c>
       <c r="L81">
+        <f t="shared" si="18"/>
+        <v>0.51643870173371131</v>
+      </c>
+      <c r="M81">
         <f t="shared" si="19"/>
-        <v>0.51643870173371131</v>
-      </c>
-      <c r="M81">
+        <v>0.4322211486008366</v>
+      </c>
+      <c r="O81">
         <f t="shared" si="20"/>
-        <v>0.4322211486008366</v>
-      </c>
-      <c r="O81">
+        <v>0.47243951753468588</v>
+      </c>
+      <c r="P81">
         <f t="shared" si="21"/>
-        <v>0.47243951753468588</v>
-      </c>
-      <c r="P81">
+        <v>0.41344558321132258</v>
+      </c>
+      <c r="R81" s="7">
         <f t="shared" si="22"/>
-        <v>0.41344558321132258</v>
-      </c>
-      <c r="R81" s="7">
+        <v>16.737256869631949</v>
+      </c>
+      <c r="S81" s="7">
         <f t="shared" si="23"/>
-        <v>16.737256869631949</v>
-      </c>
-      <c r="S81" s="7">
-        <f t="shared" si="24"/>
         <v>16.006610399575045</v>
       </c>
     </row>
@@ -38210,7 +38180,7 @@
         <v>12388</v>
       </c>
       <c r="E82" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>25810</v>
       </c>
       <c r="G82" t="s">
@@ -38223,31 +38193,31 @@
         <v>79166</v>
       </c>
       <c r="J82" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>160786</v>
       </c>
       <c r="L82">
+        <f t="shared" si="18"/>
+        <v>0.30558745556892269</v>
+      </c>
+      <c r="M82">
         <f t="shared" si="19"/>
-        <v>0.30558745556892269</v>
-      </c>
-      <c r="M82">
+        <v>0.28204570105705667</v>
+      </c>
+      <c r="O82">
         <f t="shared" si="20"/>
-        <v>0.28204570105705667</v>
-      </c>
-      <c r="O82">
+        <v>0.28452903855539291</v>
+      </c>
+      <c r="P82">
         <f t="shared" si="21"/>
-        <v>0.28452903855539291</v>
-      </c>
-      <c r="P82">
+        <v>0.27597434288503103</v>
+      </c>
+      <c r="R82" s="7">
         <f t="shared" si="22"/>
-        <v>0.27597434288503103</v>
-      </c>
-      <c r="R82" s="7">
+        <v>16.444498897329083</v>
+      </c>
+      <c r="S82" s="7">
         <f t="shared" si="23"/>
-        <v>16.444498897329083</v>
-      </c>
-      <c r="S82" s="7">
-        <f t="shared" si="24"/>
         <v>15.648131773741254</v>
       </c>
     </row>
@@ -38262,7 +38232,7 @@
         <v>12850</v>
       </c>
       <c r="E83" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>27581</v>
       </c>
       <c r="G83" t="s">
@@ -38275,31 +38245,31 @@
         <v>95300</v>
       </c>
       <c r="J83" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>216338</v>
       </c>
       <c r="L83">
+        <f t="shared" si="18"/>
+        <v>0.33539031500415739</v>
+      </c>
+      <c r="M83">
         <f t="shared" si="19"/>
-        <v>0.33539031500415739</v>
-      </c>
-      <c r="M83">
+        <v>0.29256435732831598</v>
+      </c>
+      <c r="O83">
         <f t="shared" si="20"/>
-        <v>0.29256435732831598</v>
-      </c>
-      <c r="O83">
+        <v>0.42194101652373983</v>
+      </c>
+      <c r="P83">
         <f t="shared" si="21"/>
-        <v>0.42194101652373983</v>
-      </c>
-      <c r="P83">
+        <v>0.33221780659555183</v>
+      </c>
+      <c r="R83" s="7">
         <f t="shared" si="22"/>
-        <v>0.33221780659555183</v>
-      </c>
-      <c r="R83" s="7">
+        <v>12.170558006576448</v>
+      </c>
+      <c r="S83" s="7">
         <f t="shared" si="23"/>
-        <v>12.170558006576448</v>
-      </c>
-      <c r="S83" s="7">
-        <f t="shared" si="24"/>
         <v>13.483735571878281</v>
       </c>
     </row>
@@ -38314,7 +38284,7 @@
         <v>11257</v>
       </c>
       <c r="E84" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>23100</v>
       </c>
       <c r="G84" t="s">
@@ -38327,7 +38297,7 @@
         <v>103487</v>
       </c>
       <c r="J84" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>190443</v>
       </c>
     </row>
@@ -38344,7 +38314,7 @@
         <v>2104306</v>
       </c>
       <c r="E85" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>4392196</v>
       </c>
       <c r="G85" t="s">
@@ -38359,7 +38329,7 @@
         <v>14204982</v>
       </c>
       <c r="J85" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>28686000</v>
       </c>
     </row>
@@ -38446,7 +38416,7 @@
         <v>475717</v>
       </c>
       <c r="E91" s="4">
-        <f t="shared" ref="E91:E109" si="26">SUM(C91:D91)</f>
+        <f t="shared" ref="E91:E109" si="25">SUM(C91:D91)</f>
         <v>947849</v>
       </c>
       <c r="G91" t="s">
@@ -38471,7 +38441,7 @@
         <v>-7.771125257727272</v>
       </c>
       <c r="N91" s="8">
-        <f t="shared" ref="N91:N107" si="27">C91/E$109*100</f>
+        <f t="shared" ref="N91:N107" si="26">C91/E$109*100</f>
         <v>8.6745741230794735</v>
       </c>
       <c r="O91" s="8">
@@ -38498,7 +38468,7 @@
         <v>407362</v>
       </c>
       <c r="E92" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>814940</v>
       </c>
       <c r="G92" s="15" t="s">
@@ -38511,31 +38481,31 @@
         <v>2832669</v>
       </c>
       <c r="J92" s="4">
-        <f t="shared" ref="J92:J109" si="28">SUM(H92:I92)</f>
+        <f t="shared" ref="J92:J109" si="27">SUM(H92:I92)</f>
         <v>5597716</v>
       </c>
       <c r="L92" s="4">
-        <f t="shared" ref="L92:L106" si="29">H92/J$109*100</f>
+        <f t="shared" ref="L92:L106" si="28">H92/J$109*100</f>
         <v>7.1614608997226812</v>
       </c>
       <c r="M92" s="4">
-        <f t="shared" ref="M92:M107" si="30">-(I92/J$109)*100</f>
+        <f t="shared" ref="M92:M107" si="29">-(I92/J$109)*100</f>
         <v>-7.3366016148573783</v>
       </c>
       <c r="N92" s="8">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>7.4885107807487845</v>
       </c>
       <c r="O92" s="8">
-        <f t="shared" ref="O92:O107" si="31">-(D92/E$109)*100</f>
+        <f t="shared" ref="O92:O107" si="30">-(D92/E$109)*100</f>
         <v>-7.4845421702530226</v>
       </c>
       <c r="Q92" s="7">
-        <f t="shared" ref="Q92:Q107" si="32">C92/H92*100</f>
+        <f t="shared" ref="Q92:Q107" si="31">C92/H92*100</f>
         <v>14.740364268672469</v>
       </c>
       <c r="R92" s="7">
-        <f t="shared" ref="R92:R107" si="33">D92/I92*100</f>
+        <f t="shared" ref="R92:R107" si="32">D92/I92*100</f>
         <v>14.380854240294225</v>
       </c>
     </row>
@@ -38550,7 +38520,7 @@
         <v>370855</v>
       </c>
       <c r="E93" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>736716</v>
       </c>
       <c r="G93" s="15" t="s">
@@ -38563,31 +38533,31 @@
         <v>2565313</v>
       </c>
       <c r="J93" s="4">
+        <f t="shared" si="27"/>
+        <v>5034855</v>
+      </c>
+      <c r="L93" s="4">
         <f t="shared" si="28"/>
-        <v>5034855</v>
-      </c>
-      <c r="L93" s="4">
+        <v>6.3961041071717588</v>
+      </c>
+      <c r="M93" s="4">
         <f t="shared" si="29"/>
-        <v>6.3961041071717588</v>
-      </c>
-      <c r="M93" s="4">
+        <v>-6.6441506220510149</v>
+      </c>
+      <c r="N93" s="8">
+        <f t="shared" si="26"/>
+        <v>6.7220361323612448</v>
+      </c>
+      <c r="O93" s="8">
         <f t="shared" si="30"/>
-        <v>-6.6441506220510149</v>
-      </c>
-      <c r="N93" s="8">
-        <f t="shared" si="27"/>
-        <v>6.7220361323612448</v>
-      </c>
-      <c r="O93" s="8">
+        <v>-6.8137918768790033</v>
+      </c>
+      <c r="Q93" s="7">
         <f t="shared" si="31"/>
-        <v>-6.8137918768790033</v>
-      </c>
-      <c r="Q93" s="7">
+        <v>14.814933295323588</v>
+      </c>
+      <c r="R93" s="7">
         <f t="shared" si="32"/>
-        <v>14.814933295323588</v>
-      </c>
-      <c r="R93" s="7">
-        <f t="shared" si="33"/>
         <v>14.456520510362672</v>
       </c>
     </row>
@@ -38602,7 +38572,7 @@
         <v>316129</v>
       </c>
       <c r="E94" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>629797</v>
       </c>
       <c r="G94" t="s">
@@ -38615,31 +38585,31 @@
         <v>2123653</v>
       </c>
       <c r="J94" s="4">
+        <f t="shared" si="27"/>
+        <v>4169543</v>
+      </c>
+      <c r="L94" s="4">
         <f t="shared" si="28"/>
-        <v>4169543</v>
-      </c>
-      <c r="L94" s="4">
+        <v>5.2988470865535504</v>
+      </c>
+      <c r="M94" s="4">
         <f t="shared" si="29"/>
-        <v>5.2988470865535504</v>
-      </c>
-      <c r="M94" s="4">
+        <v>-5.500252951967461</v>
+      </c>
+      <c r="N94" s="8">
+        <f t="shared" si="26"/>
+        <v>5.7630838749292401</v>
+      </c>
+      <c r="O94" s="8">
         <f t="shared" si="30"/>
-        <v>-5.500252951967461</v>
-      </c>
-      <c r="N94" s="8">
-        <f t="shared" si="27"/>
-        <v>5.7630838749292401</v>
-      </c>
-      <c r="O94" s="8">
+        <v>-5.8083003121054935</v>
+      </c>
+      <c r="Q94" s="7">
         <f t="shared" si="31"/>
-        <v>-5.8083003121054935</v>
-      </c>
-      <c r="Q94" s="7">
+        <v>15.331616069290138</v>
+      </c>
+      <c r="R94" s="7">
         <f t="shared" si="32"/>
-        <v>15.331616069290138</v>
-      </c>
-      <c r="R94" s="7">
-        <f t="shared" si="33"/>
         <v>14.886094856363069</v>
       </c>
     </row>
@@ -38654,7 +38624,7 @@
         <v>227933</v>
       </c>
       <c r="E95" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>522624</v>
       </c>
       <c r="G95" t="s">
@@ -38667,31 +38637,31 @@
         <v>1754105</v>
       </c>
       <c r="J95" s="4">
+        <f t="shared" si="27"/>
+        <v>3775103</v>
+      </c>
+      <c r="L95" s="4">
         <f t="shared" si="28"/>
-        <v>3775103</v>
-      </c>
-      <c r="L95" s="4">
+        <v>5.2343769040518078</v>
+      </c>
+      <c r="M95" s="4">
         <f t="shared" si="29"/>
-        <v>5.2343769040518078</v>
-      </c>
-      <c r="M95" s="4">
+        <v>-4.5431250794319418</v>
+      </c>
+      <c r="N95" s="8">
+        <f t="shared" si="26"/>
+        <v>5.4144157204011014</v>
+      </c>
+      <c r="O95" s="8">
         <f t="shared" si="30"/>
-        <v>-4.5431250794319418</v>
-      </c>
-      <c r="N95" s="8">
-        <f t="shared" si="27"/>
-        <v>5.4144157204011014</v>
-      </c>
-      <c r="O95" s="8">
+        <v>-4.187857852456248</v>
+      </c>
+      <c r="Q95" s="7">
         <f t="shared" si="31"/>
-        <v>-4.187857852456248</v>
-      </c>
-      <c r="Q95" s="7">
+        <v>14.581459259237267</v>
+      </c>
+      <c r="R95" s="7">
         <f t="shared" si="32"/>
-        <v>14.581459259237267</v>
-      </c>
-      <c r="R95" s="7">
-        <f t="shared" si="33"/>
         <v>12.994262031064274</v>
       </c>
     </row>
@@ -38706,7 +38676,7 @@
         <v>183083</v>
       </c>
       <c r="E96" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>398538</v>
       </c>
       <c r="G96" t="s">
@@ -38719,31 +38689,31 @@
         <v>1529116</v>
       </c>
       <c r="J96" s="4">
+        <f t="shared" si="27"/>
+        <v>3201226</v>
+      </c>
+      <c r="L96" s="4">
         <f t="shared" si="28"/>
-        <v>3201226</v>
-      </c>
-      <c r="L96" s="4">
+        <v>4.3307583505941469</v>
+      </c>
+      <c r="M96" s="4">
         <f t="shared" si="29"/>
-        <v>4.3307583505941469</v>
-      </c>
-      <c r="M96" s="4">
+        <v>-3.9604044506803495</v>
+      </c>
+      <c r="N96" s="8">
+        <f t="shared" si="26"/>
+        <v>3.9585971035390264</v>
+      </c>
+      <c r="O96" s="8">
         <f t="shared" si="30"/>
-        <v>-3.9604044506803495</v>
-      </c>
-      <c r="N96" s="8">
-        <f t="shared" si="27"/>
-        <v>3.9585971035390264</v>
-      </c>
-      <c r="O96" s="8">
+        <v>-3.3638199786834173</v>
+      </c>
+      <c r="Q96" s="7">
         <f t="shared" si="31"/>
-        <v>-3.3638199786834173</v>
-      </c>
-      <c r="Q96" s="7">
+        <v>12.885216881664482</v>
+      </c>
+      <c r="R96" s="7">
         <f t="shared" si="32"/>
-        <v>12.885216881664482</v>
-      </c>
-      <c r="R96" s="7">
-        <f t="shared" si="33"/>
         <v>11.973126957013072</v>
       </c>
     </row>
@@ -38758,7 +38728,7 @@
         <v>142868</v>
       </c>
       <c r="E97" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>296843</v>
       </c>
       <c r="G97" t="s">
@@ -38771,31 +38741,31 @@
         <v>1257035</v>
       </c>
       <c r="J97" s="4">
+        <f t="shared" si="27"/>
+        <v>2519506</v>
+      </c>
+      <c r="L97" s="4">
         <f t="shared" si="28"/>
-        <v>2519506</v>
-      </c>
-      <c r="L97" s="4">
+        <v>3.2697949450891044</v>
+      </c>
+      <c r="M97" s="4">
         <f t="shared" si="29"/>
-        <v>3.2697949450891044</v>
-      </c>
-      <c r="M97" s="4">
+        <v>-3.2557157263811067</v>
+      </c>
+      <c r="N97" s="8">
+        <f t="shared" si="26"/>
+        <v>2.829012967985991</v>
+      </c>
+      <c r="O97" s="8">
         <f t="shared" si="30"/>
-        <v>-3.2557157263811067</v>
-      </c>
-      <c r="N97" s="8">
-        <f t="shared" si="27"/>
-        <v>2.829012967985991</v>
-      </c>
-      <c r="O97" s="8">
+        <v>-2.6249418717988147</v>
+      </c>
+      <c r="Q97" s="7">
         <f t="shared" si="31"/>
-        <v>-2.6249418717988147</v>
-      </c>
-      <c r="Q97" s="7">
+        <v>12.196319757047885</v>
+      </c>
+      <c r="R97" s="7">
         <f t="shared" si="32"/>
-        <v>12.196319757047885</v>
-      </c>
-      <c r="R97" s="7">
-        <f t="shared" si="33"/>
         <v>11.365475106102853</v>
       </c>
     </row>
@@ -38810,7 +38780,7 @@
         <v>106733</v>
       </c>
       <c r="E98" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>230142</v>
       </c>
       <c r="G98" t="s">
@@ -38823,31 +38793,31 @@
         <v>1004361</v>
       </c>
       <c r="J98" s="4">
+        <f t="shared" si="27"/>
+        <v>2008632</v>
+      </c>
+      <c r="L98" s="4">
         <f t="shared" si="28"/>
-        <v>2008632</v>
-      </c>
-      <c r="L98" s="4">
+        <v>2.6010579564200524</v>
+      </c>
+      <c r="M98" s="4">
         <f t="shared" si="29"/>
-        <v>2.6010579564200524</v>
-      </c>
-      <c r="M98" s="4">
+        <v>-2.6012910560675362</v>
+      </c>
+      <c r="N98" s="8">
+        <f t="shared" si="26"/>
+        <v>2.2674178364421702</v>
+      </c>
+      <c r="O98" s="8">
         <f t="shared" si="30"/>
-        <v>-2.6012910560675362</v>
-      </c>
-      <c r="N98" s="8">
-        <f t="shared" si="27"/>
-        <v>2.2674178364421702</v>
-      </c>
-      <c r="O98" s="8">
+        <v>-1.9610264076119419</v>
+      </c>
+      <c r="Q98" s="7">
         <f t="shared" si="31"/>
-        <v>-1.9610264076119419</v>
-      </c>
-      <c r="Q98" s="7">
+        <v>12.28841617451863</v>
+      </c>
+      <c r="R98" s="7">
         <f t="shared" si="32"/>
-        <v>12.28841617451863</v>
-      </c>
-      <c r="R98" s="7">
-        <f t="shared" si="33"/>
         <v>10.626955845557523</v>
       </c>
     </row>
@@ -38862,7 +38832,7 @@
         <v>77883</v>
       </c>
       <c r="E99" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>173521</v>
       </c>
       <c r="G99" t="s">
@@ -38875,31 +38845,31 @@
         <v>743594</v>
       </c>
       <c r="J99" s="4">
+        <f t="shared" si="27"/>
+        <v>1476169</v>
+      </c>
+      <c r="L99" s="4">
         <f t="shared" si="28"/>
-        <v>1476169</v>
-      </c>
-      <c r="L99" s="4">
+        <v>1.8973663806128225</v>
+      </c>
+      <c r="M99" s="4">
         <f t="shared" si="29"/>
-        <v>1.8973663806128225</v>
-      </c>
-      <c r="M99" s="4">
+        <v>-1.9259055474530404</v>
+      </c>
+      <c r="N99" s="8">
+        <f t="shared" si="26"/>
+        <v>1.7571757897856417</v>
+      </c>
+      <c r="O99" s="8">
         <f t="shared" si="30"/>
-        <v>-1.9259055474530404</v>
-      </c>
-      <c r="N99" s="8">
-        <f t="shared" si="27"/>
-        <v>1.7571757897856417</v>
-      </c>
-      <c r="O99" s="8">
+        <v>-1.4309596816733428</v>
+      </c>
+      <c r="Q99" s="7">
         <f t="shared" si="31"/>
-        <v>-1.4309596816733428</v>
-      </c>
-      <c r="Q99" s="7">
+        <v>13.055045558475243</v>
+      </c>
+      <c r="R99" s="7">
         <f t="shared" si="32"/>
-        <v>13.055045558475243</v>
-      </c>
-      <c r="R99" s="7">
-        <f t="shared" si="33"/>
         <v>10.47386073583165</v>
       </c>
     </row>
@@ -38914,7 +38884,7 @@
         <v>75090</v>
       </c>
       <c r="E100" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>166874</v>
       </c>
       <c r="G100" t="s">
@@ -38927,31 +38897,31 @@
         <v>635276</v>
       </c>
       <c r="J100" s="4">
+        <f t="shared" si="27"/>
+        <v>1272745</v>
+      </c>
+      <c r="L100" s="4">
         <f t="shared" si="28"/>
-        <v>1272745</v>
-      </c>
-      <c r="L100" s="4">
+        <v>1.6510422131288611</v>
+      </c>
+      <c r="M100" s="4">
         <f t="shared" si="29"/>
-        <v>1.6510422131288611</v>
-      </c>
-      <c r="M100" s="4">
+        <v>-1.6453623517185156</v>
+      </c>
+      <c r="N100" s="8">
+        <f t="shared" si="26"/>
+        <v>1.6863654895510714</v>
+      </c>
+      <c r="O100" s="8">
         <f t="shared" si="30"/>
-        <v>-1.6453623517185156</v>
-      </c>
-      <c r="N100" s="8">
-        <f t="shared" si="27"/>
-        <v>1.6863654895510714</v>
-      </c>
-      <c r="O100" s="8">
+        <v>-1.3796433431795294</v>
+      </c>
+      <c r="Q100" s="7">
         <f t="shared" si="31"/>
-        <v>-1.3796433431795294</v>
-      </c>
-      <c r="Q100" s="7">
+        <v>14.39819034337356</v>
+      </c>
+      <c r="R100" s="7">
         <f t="shared" si="32"/>
-        <v>14.39819034337356</v>
-      </c>
-      <c r="R100" s="7">
-        <f t="shared" si="33"/>
         <v>11.820059312802625</v>
       </c>
     </row>
@@ -38966,7 +38936,7 @@
         <v>60986</v>
       </c>
       <c r="E101" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>135460</v>
       </c>
       <c r="G101" t="s">
@@ -38979,31 +38949,31 @@
         <v>478346</v>
       </c>
       <c r="J101" s="4">
+        <f t="shared" si="27"/>
+        <v>956206</v>
+      </c>
+      <c r="L101" s="4">
         <f t="shared" si="28"/>
-        <v>956206</v>
-      </c>
-      <c r="L101" s="4">
+        <v>1.2376555282935444</v>
+      </c>
+      <c r="M101" s="4">
         <f t="shared" si="29"/>
-        <v>1.2376555282935444</v>
-      </c>
-      <c r="M101" s="4">
+        <v>-1.2389142663899548</v>
+      </c>
+      <c r="N101" s="8">
+        <f t="shared" si="26"/>
+        <v>1.3683254539879115</v>
+      </c>
+      <c r="O101" s="8">
         <f t="shared" si="30"/>
-        <v>-1.2389142663899548</v>
-      </c>
-      <c r="N101" s="8">
-        <f t="shared" si="27"/>
-        <v>1.3683254539879115</v>
-      </c>
-      <c r="O101" s="8">
+        <v>-1.120507776363654</v>
+      </c>
+      <c r="Q101" s="7">
         <f t="shared" si="31"/>
-        <v>-1.120507776363654</v>
-      </c>
-      <c r="Q101" s="7">
+        <v>15.58489934290378</v>
+      </c>
+      <c r="R101" s="7">
         <f t="shared" si="32"/>
-        <v>15.58489934290378</v>
-      </c>
-      <c r="R101" s="7">
-        <f t="shared" si="33"/>
         <v>12.749348797732186</v>
       </c>
     </row>
@@ -39018,7 +38988,7 @@
         <v>48144</v>
       </c>
       <c r="E102" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>103349</v>
       </c>
       <c r="G102" t="s">
@@ -39031,31 +39001,31 @@
         <v>359466</v>
       </c>
       <c r="J102" s="4">
+        <f t="shared" si="27"/>
+        <v>711953</v>
+      </c>
+      <c r="L102" s="4">
         <f t="shared" si="28"/>
-        <v>711953</v>
-      </c>
-      <c r="L102" s="4">
+        <v>0.9129399493609146</v>
+      </c>
+      <c r="M102" s="4">
         <f t="shared" si="29"/>
-        <v>0.9129399493609146</v>
-      </c>
-      <c r="M102" s="4">
+        <v>-0.93101553202521081</v>
+      </c>
+      <c r="N102" s="8">
+        <f t="shared" si="26"/>
+        <v>1.0142923260117982</v>
+      </c>
+      <c r="O102" s="8">
         <f t="shared" si="30"/>
-        <v>-0.93101553202521081</v>
-      </c>
-      <c r="N102" s="8">
-        <f t="shared" si="27"/>
-        <v>1.0142923260117982</v>
-      </c>
-      <c r="O102" s="8">
+        <v>-0.88455918383320375</v>
+      </c>
+      <c r="Q102" s="7">
         <f t="shared" si="31"/>
-        <v>-0.88455918383320375</v>
-      </c>
-      <c r="Q102" s="7">
+        <v>15.661570497635374</v>
+      </c>
+      <c r="R102" s="7">
         <f t="shared" si="32"/>
-        <v>15.661570497635374</v>
-      </c>
-      <c r="R102" s="7">
-        <f t="shared" si="33"/>
         <v>13.393199913204587</v>
       </c>
     </row>
@@ -39070,7 +39040,7 @@
         <v>40141</v>
       </c>
       <c r="E103" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>86914</v>
       </c>
       <c r="G103" t="s">
@@ -39083,31 +39053,31 @@
         <v>295197</v>
       </c>
       <c r="J103" s="4">
+        <f t="shared" si="27"/>
+        <v>593778</v>
+      </c>
+      <c r="L103" s="4">
         <f t="shared" si="28"/>
-        <v>593778</v>
-      </c>
-      <c r="L103" s="4">
+        <v>0.77332362050268866</v>
+      </c>
+      <c r="M103" s="4">
         <f t="shared" si="29"/>
-        <v>0.77332362050268866</v>
-      </c>
-      <c r="M103" s="4">
+        <v>-0.76455907375731269</v>
+      </c>
+      <c r="N103" s="8">
+        <f t="shared" si="26"/>
+        <v>0.85936953110315795</v>
+      </c>
+      <c r="O103" s="8">
         <f t="shared" si="30"/>
-        <v>-0.76455907375731269</v>
-      </c>
-      <c r="N103" s="8">
-        <f t="shared" si="27"/>
-        <v>0.85936953110315795</v>
-      </c>
-      <c r="O103" s="8">
+        <v>-0.7375184903258688</v>
+      </c>
+      <c r="Q103" s="7">
         <f t="shared" si="31"/>
-        <v>-0.7375184903258688</v>
-      </c>
-      <c r="Q103" s="7">
+        <v>15.665095903624144</v>
+      </c>
+      <c r="R103" s="7">
         <f t="shared" si="32"/>
-        <v>15.665095903624144</v>
-      </c>
-      <c r="R103" s="7">
-        <f t="shared" si="33"/>
         <v>13.598037920439571</v>
       </c>
     </row>
@@ -39122,7 +39092,7 @@
         <v>25151</v>
       </c>
       <c r="E104" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>57943</v>
       </c>
       <c r="G104" t="s">
@@ -39135,31 +39105,31 @@
         <v>183151</v>
       </c>
       <c r="J104" s="4">
+        <f t="shared" si="27"/>
+        <v>390763</v>
+      </c>
+      <c r="L104" s="4">
         <f t="shared" si="28"/>
-        <v>390763</v>
-      </c>
-      <c r="L104" s="4">
+        <v>0.53771426681471435</v>
+      </c>
+      <c r="M104" s="4">
         <f t="shared" si="29"/>
-        <v>0.53771426681471435</v>
-      </c>
-      <c r="M104" s="4">
+        <v>-0.47436037262480851</v>
+      </c>
+      <c r="N104" s="8">
+        <f t="shared" si="26"/>
+        <v>0.60249386748625822</v>
+      </c>
+      <c r="O104" s="8">
         <f t="shared" si="30"/>
-        <v>-0.47436037262480851</v>
-      </c>
-      <c r="N104" s="8">
-        <f t="shared" si="27"/>
-        <v>0.60249386748625822</v>
-      </c>
-      <c r="O104" s="8">
+        <v>-0.46210427119867287</v>
+      </c>
+      <c r="Q104" s="7">
         <f t="shared" si="31"/>
-        <v>-0.46210427119867287</v>
-      </c>
-      <c r="Q104" s="7">
+        <v>15.794848081999113</v>
+      </c>
+      <c r="R104" s="7">
         <f t="shared" si="32"/>
-        <v>15.794848081999113</v>
-      </c>
-      <c r="R104" s="7">
-        <f t="shared" si="33"/>
         <v>13.732384753564</v>
       </c>
     </row>
@@ -39174,7 +39144,7 @@
         <v>23013</v>
       </c>
       <c r="E105" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>52517</v>
       </c>
       <c r="G105" t="s">
@@ -39187,31 +39157,31 @@
         <v>160301</v>
       </c>
       <c r="J105" s="4">
+        <f t="shared" si="27"/>
+        <v>339301</v>
+      </c>
+      <c r="L105" s="4">
         <f t="shared" si="28"/>
-        <v>339301</v>
-      </c>
-      <c r="L105" s="4">
+        <v>0.46360929888365732</v>
+      </c>
+      <c r="M105" s="4">
         <f t="shared" si="29"/>
-        <v>0.46360929888365732</v>
-      </c>
-      <c r="M105" s="4">
+        <v>-0.41517896212485556</v>
+      </c>
+      <c r="N105" s="8">
+        <f t="shared" si="26"/>
+        <v>0.54208279660632364</v>
+      </c>
+      <c r="O105" s="8">
         <f t="shared" si="30"/>
-        <v>-0.41517896212485556</v>
-      </c>
-      <c r="N105" s="8">
-        <f t="shared" si="27"/>
-        <v>0.54208279660632364</v>
-      </c>
-      <c r="O105" s="8">
+        <v>-0.42282237656932359</v>
+      </c>
+      <c r="Q105" s="7">
         <f t="shared" si="31"/>
-        <v>-0.42282237656932359</v>
-      </c>
-      <c r="Q105" s="7">
+        <v>16.482681564245809</v>
+      </c>
+      <c r="R105" s="7">
         <f t="shared" si="32"/>
-        <v>16.482681564245809</v>
-      </c>
-      <c r="R105" s="7">
-        <f t="shared" si="33"/>
         <v>14.356117553851815</v>
       </c>
     </row>
@@ -39226,7 +39196,7 @@
         <v>15594</v>
       </c>
       <c r="E106" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>36832</v>
       </c>
       <c r="G106" t="s">
@@ -39239,31 +39209,31 @@
         <v>99833</v>
       </c>
       <c r="J106" s="4">
+        <f t="shared" si="27"/>
+        <v>218508</v>
+      </c>
+      <c r="L106" s="4">
         <f t="shared" si="28"/>
-        <v>218508</v>
-      </c>
-      <c r="L106" s="4">
+        <v>0.30736778516769847</v>
+      </c>
+      <c r="M106" s="4">
         <f t="shared" si="29"/>
-        <v>0.30736778516769847</v>
-      </c>
-      <c r="M106" s="4">
+        <v>-0.25856707896900644</v>
+      </c>
+      <c r="N106" s="8">
+        <f t="shared" si="26"/>
+        <v>0.3902099523564635</v>
+      </c>
+      <c r="O106" s="8">
         <f t="shared" si="30"/>
-        <v>-0.25856707896900644</v>
-      </c>
-      <c r="N106" s="8">
-        <f t="shared" si="27"/>
-        <v>0.3902099523564635</v>
-      </c>
-      <c r="O106" s="8">
+        <v>-0.28651162995793827</v>
+      </c>
+      <c r="Q106" s="7">
         <f t="shared" si="31"/>
-        <v>-0.28651162995793827</v>
-      </c>
-      <c r="Q106" s="7">
+        <v>17.895934274278492</v>
+      </c>
+      <c r="R106" s="7">
         <f t="shared" si="32"/>
-        <v>17.895934274278492</v>
-      </c>
-      <c r="R106" s="7">
-        <f t="shared" si="33"/>
         <v>15.620085542856572</v>
       </c>
     </row>
@@ -39278,7 +39248,7 @@
         <v>19734</v>
       </c>
       <c r="E107" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>49371</v>
       </c>
       <c r="G107" t="s">
@@ -39291,7 +39261,7 @@
         <v>159125</v>
       </c>
       <c r="J107" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>383701</v>
       </c>
       <c r="L107" s="4">
@@ -39299,23 +39269,23 @@
         <v>0.58165096036925268</v>
       </c>
       <c r="M107" s="4">
+        <f t="shared" si="29"/>
+        <v>-0.41213312673107244</v>
+      </c>
+      <c r="N107" s="8">
+        <f t="shared" si="26"/>
+        <v>0.54452643177269555</v>
+      </c>
+      <c r="O107" s="8">
         <f t="shared" si="30"/>
-        <v>-0.41213312673107244</v>
-      </c>
-      <c r="N107" s="8">
-        <f t="shared" si="27"/>
-        <v>0.54452643177269555</v>
-      </c>
-      <c r="O107" s="8">
+        <v>-0.36257666446004577</v>
+      </c>
+      <c r="Q107" s="7">
         <f t="shared" si="31"/>
-        <v>-0.36257666446004577</v>
-      </c>
-      <c r="Q107" s="7">
+        <v>13.196868766030208</v>
+      </c>
+      <c r="R107" s="7">
         <f t="shared" si="32"/>
-        <v>13.196868766030208</v>
-      </c>
-      <c r="R107" s="7">
-        <f t="shared" si="33"/>
         <v>12.401571091908876</v>
       </c>
     </row>
@@ -39330,7 +39300,7 @@
         <v>1318</v>
       </c>
       <c r="E108" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>2481</v>
       </c>
       <c r="G108" t="s">
@@ -39343,7 +39313,7 @@
         <v>11478</v>
       </c>
       <c r="J108" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>21086</v>
       </c>
     </row>
@@ -39360,7 +39330,7 @@
         <v>2617734</v>
       </c>
       <c r="E109" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>5442711</v>
       </c>
       <c r="G109" t="s">
@@ -39375,7 +39345,7 @@
         <v>19192458</v>
       </c>
       <c r="J109" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>38610097</v>
       </c>
     </row>
@@ -42998,8 +42968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="L57" sqref="L57"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43016,7 +42986,7 @@
       <c r="B2" t="s">
         <v>391</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
         <v>158</v>
       </c>
       <c r="T2" s="21"/>
@@ -43204,6 +43174,10 @@
       <c r="W5" s="7">
         <v>29.052900000000001</v>
       </c>
+      <c r="X5" s="8">
+        <f>R12-S12</f>
+        <v>4.460700000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -43265,6 +43239,10 @@
       </c>
       <c r="W6" s="7">
         <v>25.658000000000001</v>
+      </c>
+      <c r="X6" s="8">
+        <f>T12-R12</f>
+        <v>4.4608000000000008</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -45158,7 +45136,7 @@
       <c r="S69" s="7">
         <v>15.9191</v>
       </c>
-      <c r="T69" s="84">
+      <c r="T69" s="83">
         <v>9.1097999999999999</v>
       </c>
       <c r="U69" s="8">
@@ -45231,6 +45209,18 @@
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D71" s="8">
+        <f>C70-D70</f>
+        <v>4.1184000000000012</v>
+      </c>
+      <c r="E71" s="8">
+        <f>E70-C70</f>
+        <v>4.1184999999999992</v>
+      </c>
+      <c r="F71" s="8">
+        <f>F70-G70</f>
+        <v>3.4876000000000005</v>
+      </c>
       <c r="O71" s="8">
         <f>N70-O70</f>
         <v>1.2179000000000002</v>
@@ -47682,7 +47672,7 @@
     </row>
     <row r="213" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K213" s="37" t="str">
-        <f t="shared" ref="K185:K213" si="1">LEFT(L213,4)</f>
+        <f>LEFT(L213,4)</f>
         <v/>
       </c>
     </row>
@@ -50134,11 +50124,11 @@
       <c r="Z33" s="4"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C34" s="82">
+      <c r="C34" s="84">
         <v>2015</v>
       </c>
-      <c r="D34" s="82"/>
-      <c r="E34" s="82"/>
+      <c r="D34" s="84"/>
+      <c r="E34" s="84"/>
       <c r="F34" s="23">
         <v>2015</v>
       </c>

</xml_diff>

<commit_message>
reduce VMMC scale up rate
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="4770" tabRatio="835" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9600" tabRatio="835" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="10" r:id="rId1"/>
@@ -30,7 +30,6 @@
     <sheet name="DALY" sheetId="1" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3208" uniqueCount="1346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3211" uniqueCount="1349">
   <si>
     <t>Metric</t>
   </si>
@@ -4090,6 +4089,15 @@
   </si>
   <si>
     <t>60–64</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>*HIV clinic</t>
+  </si>
+  <si>
+    <t>*family planning clinic</t>
   </si>
 </sst>
 </file>
@@ -12862,7 +12870,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13198,7 +13205,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18907,7 +18913,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20227,7 +20232,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -20302,7 +20306,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -42968,7 +42971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
@@ -53133,8 +53136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y256"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56718,7 +56721,9 @@
       <c r="A168" s="74" t="s">
         <v>601</v>
       </c>
-      <c r="B168" s="74"/>
+      <c r="B168" s="74">
+        <v>1</v>
+      </c>
       <c r="C168" s="74"/>
       <c r="D168" s="74">
         <v>0</v>
@@ -56748,7 +56753,9 @@
       <c r="A169" s="74" t="s">
         <v>459</v>
       </c>
-      <c r="B169" s="74"/>
+      <c r="B169" s="74">
+        <v>2</v>
+      </c>
       <c r="C169" s="74"/>
       <c r="D169" s="74">
         <v>0</v>
@@ -56778,7 +56785,9 @@
       <c r="A170" s="74" t="s">
         <v>338</v>
       </c>
-      <c r="B170" s="74"/>
+      <c r="B170" s="74">
+        <v>3</v>
+      </c>
       <c r="C170" s="74"/>
       <c r="D170" s="74">
         <f>0.8*M170</f>
@@ -56813,7 +56822,9 @@
       <c r="A171" s="74" t="s">
         <v>311</v>
       </c>
-      <c r="B171" s="74"/>
+      <c r="B171" s="74">
+        <v>4</v>
+      </c>
       <c r="C171" s="74"/>
       <c r="D171" s="74">
         <f t="shared" ref="D171:D183" si="0">0.8*M171</f>
@@ -56848,7 +56859,9 @@
       <c r="A172" s="74" t="s">
         <v>602</v>
       </c>
-      <c r="B172" s="74"/>
+      <c r="B172" s="74">
+        <v>5</v>
+      </c>
       <c r="C172" s="74"/>
       <c r="D172" s="74">
         <f t="shared" si="0"/>
@@ -56885,7 +56898,9 @@
       <c r="A173" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="B173" s="74"/>
+      <c r="B173" s="74">
+        <v>6</v>
+      </c>
       <c r="C173" s="74"/>
       <c r="D173" s="74">
         <f t="shared" si="0"/>
@@ -56920,7 +56935,9 @@
       <c r="A174" s="74" t="s">
         <v>314</v>
       </c>
-      <c r="B174" s="74"/>
+      <c r="B174" s="74">
+        <v>7</v>
+      </c>
       <c r="C174" s="74"/>
       <c r="D174" s="74">
         <f t="shared" si="0"/>
@@ -56957,7 +56974,9 @@
       <c r="A175" s="74" t="s">
         <v>315</v>
       </c>
-      <c r="B175" s="74"/>
+      <c r="B175" s="74">
+        <v>8</v>
+      </c>
       <c r="C175" s="74"/>
       <c r="D175" s="74">
         <f t="shared" si="0"/>
@@ -56994,7 +57013,9 @@
       <c r="A176" s="74" t="s">
         <v>316</v>
       </c>
-      <c r="B176" s="74"/>
+      <c r="B176" s="74">
+        <v>9</v>
+      </c>
       <c r="C176" s="74"/>
       <c r="D176" s="74">
         <f t="shared" si="0"/>
@@ -57031,7 +57052,9 @@
       <c r="A177" s="74" t="s">
         <v>317</v>
       </c>
-      <c r="B177" s="74"/>
+      <c r="B177" s="74">
+        <v>10</v>
+      </c>
       <c r="C177" s="74"/>
       <c r="D177" s="74">
         <f t="shared" si="0"/>
@@ -57068,7 +57091,9 @@
       <c r="A178" s="74" t="s">
         <v>603</v>
       </c>
-      <c r="B178" s="74"/>
+      <c r="B178" s="74">
+        <v>11</v>
+      </c>
       <c r="C178" s="74"/>
       <c r="D178" s="74">
         <f t="shared" si="0"/>
@@ -57105,7 +57130,9 @@
       <c r="A179" s="74" t="s">
         <v>319</v>
       </c>
-      <c r="B179" s="74"/>
+      <c r="B179" s="74">
+        <v>12</v>
+      </c>
       <c r="C179" s="74"/>
       <c r="D179" s="74">
         <f t="shared" si="0"/>
@@ -57142,7 +57169,9 @@
       <c r="A180" s="74" t="s">
         <v>324</v>
       </c>
-      <c r="B180" s="74"/>
+      <c r="B180" s="74">
+        <v>13</v>
+      </c>
       <c r="C180" s="74"/>
       <c r="D180" s="74">
         <f t="shared" si="0"/>
@@ -57179,7 +57208,9 @@
       <c r="A181" s="74" t="s">
         <v>462</v>
       </c>
-      <c r="B181" s="74"/>
+      <c r="B181" s="74">
+        <v>14</v>
+      </c>
       <c r="C181" s="74"/>
       <c r="D181" s="74">
         <f t="shared" si="0"/>
@@ -57216,7 +57247,9 @@
       <c r="A182" s="74" t="s">
         <v>463</v>
       </c>
-      <c r="B182" s="74"/>
+      <c r="B182" s="74">
+        <v>15</v>
+      </c>
       <c r="C182" s="74"/>
       <c r="D182" s="74">
         <f t="shared" si="0"/>
@@ -57253,7 +57286,9 @@
       <c r="A183" s="74" t="s">
         <v>464</v>
       </c>
-      <c r="B183" s="74"/>
+      <c r="B183" s="74">
+        <v>16</v>
+      </c>
       <c r="C183" s="74"/>
       <c r="D183" s="74">
         <f t="shared" si="0"/>
@@ -57383,7 +57418,9 @@
       <c r="A188" s="74" t="s">
         <v>601</v>
       </c>
-      <c r="B188" s="74"/>
+      <c r="B188" s="74">
+        <v>1</v>
+      </c>
       <c r="C188" s="74"/>
       <c r="D188" s="75">
         <v>0</v>
@@ -57416,7 +57453,9 @@
       <c r="A189" s="74" t="s">
         <v>459</v>
       </c>
-      <c r="B189" s="74"/>
+      <c r="B189" s="74">
+        <v>2</v>
+      </c>
       <c r="C189" s="74"/>
       <c r="D189" s="75">
         <v>0</v>
@@ -57449,7 +57488,9 @@
       <c r="A190" s="74" t="s">
         <v>338</v>
       </c>
-      <c r="B190" s="74"/>
+      <c r="B190" s="74">
+        <v>3</v>
+      </c>
       <c r="C190" s="74">
         <v>0.05</v>
       </c>
@@ -57489,7 +57530,9 @@
       <c r="A191" s="74" t="s">
         <v>311</v>
       </c>
-      <c r="B191" s="74"/>
+      <c r="B191" s="74">
+        <v>4</v>
+      </c>
       <c r="C191" s="74">
         <v>0.1</v>
       </c>
@@ -57530,7 +57573,7 @@
         <v>602</v>
       </c>
       <c r="B192" s="74">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C192" s="74">
         <v>0.4</v>
@@ -57574,7 +57617,7 @@
         <v>139</v>
       </c>
       <c r="B193" s="74">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C193" s="74"/>
       <c r="D193" s="75">
@@ -57614,7 +57657,7 @@
         <v>314</v>
       </c>
       <c r="B194" s="74">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C194" s="74">
         <v>0.70710678100000002</v>
@@ -57632,7 +57675,9 @@
         <v>31.768893464000001</v>
       </c>
       <c r="G194" s="72"/>
-      <c r="H194" s="72"/>
+      <c r="H194" s="72" t="s">
+        <v>1346</v>
+      </c>
       <c r="I194" s="72"/>
       <c r="J194" s="72" t="s">
         <v>314</v>
@@ -57658,7 +57703,7 @@
         <v>315</v>
       </c>
       <c r="B195" s="74">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C195" s="74">
         <v>0.5</v>
@@ -57702,7 +57747,7 @@
         <v>316</v>
       </c>
       <c r="B196" s="74">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C196" s="74">
         <v>0.35355339099999999</v>
@@ -57746,7 +57791,7 @@
         <v>317</v>
       </c>
       <c r="B197" s="74">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C197" s="74">
         <v>0.25</v>
@@ -57790,7 +57835,7 @@
         <v>603</v>
       </c>
       <c r="B198" s="74">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C198" s="74">
         <v>0.17677669500000001</v>
@@ -57834,7 +57879,7 @@
         <v>319</v>
       </c>
       <c r="B199" s="74">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C199" s="74">
         <v>0.125</v>
@@ -57878,7 +57923,7 @@
         <v>324</v>
       </c>
       <c r="B200" s="74">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C200" s="74">
         <v>8.8388348000000005E-2</v>
@@ -57922,7 +57967,7 @@
         <v>462</v>
       </c>
       <c r="B201" s="74">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="C201" s="74">
         <v>6.25E-2</v>
@@ -57966,7 +58011,7 @@
         <v>463</v>
       </c>
       <c r="B202" s="74">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C202" s="74">
         <v>4.4194174000000003E-2</v>
@@ -58010,7 +58055,7 @@
         <v>464</v>
       </c>
       <c r="B203" s="74">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="C203" s="74">
         <v>3.125E-2</v>
@@ -68076,8 +68121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R247"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="G249" sqref="G249"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="H131" sqref="H131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68958,6 +69003,9 @@
       <c r="G71" t="s">
         <v>106</v>
       </c>
+      <c r="H71" t="s">
+        <v>1347</v>
+      </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
@@ -69568,6 +69616,9 @@
       </c>
       <c r="F130" s="13">
         <v>1</v>
+      </c>
+      <c r="H130" t="s">
+        <v>1348</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add multiplier on HIV lambda for HPV+
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20361"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Kenya_model_Feb20\HHCoM\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Kenya_model_HPV-HIVacq\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955AA464-D7BB-4873-A8C3-9BF208CCA9CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="4770" tabRatio="835" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="10" r:id="rId1"/>
@@ -29,8 +30,7 @@
     <sheet name="MTCT" sheetId="14" r:id="rId15"/>
     <sheet name="DALY" sheetId="1" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3211" uniqueCount="1349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3264" uniqueCount="1350">
   <si>
     <t>Metric</t>
   </si>
@@ -3468,9 +3468,6 @@
     <t>%virally suppresion among all PLHIV</t>
   </si>
   <si>
-    <t xml:space="preserve">Source: </t>
-  </si>
-  <si>
     <t>Source: population_validation_targets_kenya.xlsx</t>
   </si>
   <si>
@@ -4099,13 +4096,19 @@
   </si>
   <si>
     <t>*family planning clinic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adapted risk distribution </t>
+  </si>
+  <si>
+    <t>0.971839 0.02640375 0.00175725</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="13">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -4118,6 +4121,7 @@
     <numFmt numFmtId="172" formatCode="##0.0;\-##0.0;0"/>
     <numFmt numFmtId="173" formatCode="#\ ###\ ###\ ##0;\-#\ ###\ ###\ ##0;0"/>
     <numFmt numFmtId="174" formatCode="##0.0000;\-##0.0000;0.000"/>
+    <numFmt numFmtId="175" formatCode="0.000000"/>
   </numFmts>
   <fonts count="33" x14ac:knownFonts="1">
     <font>
@@ -4826,7 +4830,7 @@
     <xf numFmtId="0" fontId="1" fillId="36" borderId="8" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4944,6 +4948,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4974,11 +4979,11 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Comma" xfId="54" builtinId="3"/>
-    <cellStyle name="Data" xfId="46"/>
-    <cellStyle name="Data 2" xfId="48"/>
+    <cellStyle name="Data" xfId="46" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Data 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Header" xfId="45"/>
+    <cellStyle name="Header" xfId="45" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
@@ -4988,17 +4993,17 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="43"/>
-    <cellStyle name="Normal 2 2" xfId="47"/>
+    <cellStyle name="Normal 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 2 2" xfId="47" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Note 2" xfId="51"/>
-    <cellStyle name="Note 3" xfId="52"/>
-    <cellStyle name="Note 4" xfId="53"/>
+    <cellStyle name="Note 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Note 3" xfId="52" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Note 4" xfId="53" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="44"/>
-    <cellStyle name="Style 1" xfId="50"/>
-    <cellStyle name="Title 2" xfId="42"/>
+    <cellStyle name="Percent 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Style 1" xfId="50" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Title 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
@@ -12871,7 +12876,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13207,7 +13211,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -32174,7 +32177,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -32204,7 +32213,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -32234,7 +32249,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -32264,7 +32285,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -32296,7 +32323,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -32326,7 +32359,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -32358,7 +32397,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -32393,7 +32438,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -32431,7 +32482,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -32560,7 +32617,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Baseline estimates of coverage of 90-90-90 targets in Nyanza region, Kenya AIDS Indicator Survey, 2012–2013*."/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Baseline estimates of coverage of 90-90-90 targets in Nyanza region, Kenya AIDS Indicator Survey, 2012–2013*.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -32615,7 +32678,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -32653,7 +32722,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="https://www.dovepress.com/cr_data/article_fulltext/s153000/153185/img/hiv-153185_T003.jpg"/>
+        <xdr:cNvPr id="6" name="Picture 5" descr="https://www.dovepress.com/cr_data/article_fulltext/s153000/153185/img/hiv-153185_T003.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -32708,7 +32783,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9219" name="AutoShape 3" descr="https://images.journals.lww.com/aidsonline/Original.00002030-201207310-00012.F3-12.jpeg"/>
+        <xdr:cNvPr id="9219" name="AutoShape 3" descr="https://images.journals.lww.com/aidsonline/Original.00002030-201207310-00012.F3-12.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000003240000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -32750,7 +32831,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -32788,7 +32875,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextBox 7"/>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -32891,7 +32984,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="An external file that holds a picture, illustration, etc.&#10;Object name is peerj-06-4427-g002.jpg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="An external file that holds a picture, illustration, etc.&#10;Object name is peerj-06-4427-g002.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -32951,7 +33050,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -32989,7 +33094,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -33030,7 +33141,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33101,7 +33212,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33169,7 +33280,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2049" name="AutoShape 1" descr="https://images.journals.lww.com/aidsonline/Original.00002030-200108004-00006.T2-6.jpeg"/>
+        <xdr:cNvPr id="2049" name="AutoShape 1" descr="https://images.journals.lww.com/aidsonline/Original.00002030-200108004-00006.T2-6.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -33211,7 +33328,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -33255,7 +33378,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -33293,7 +33422,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -33323,7 +33458,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -33355,7 +33496,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -33385,7 +33532,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -33417,7 +33570,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="TextBox 10"/>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -33527,7 +33686,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -33564,7 +33729,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="TextBox 13"/>
+        <xdr:cNvPr id="14" name="TextBox 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -33638,7 +33809,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -33776,7 +33953,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -33814,7 +33997,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -33851,7 +34040,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -33881,7 +34076,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -33911,7 +34112,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -33946,7 +34153,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -33976,7 +34189,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34006,7 +34225,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34041,7 +34266,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="An external file that holds a picture, illustration, etc.&#10;Object name is 12879_2019_3982_Fig1_HTML.jpg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="An external file that holds a picture, illustration, etc.&#10;Object name is 12879_2019_3982_Fig1_HTML.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -34101,7 +34332,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="image"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -34161,7 +34398,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34199,7 +34442,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34237,7 +34486,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34275,7 +34530,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="7" name="Group 6"/>
+        <xdr:cNvPr id="7" name="Group 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
@@ -34288,7 +34549,13 @@
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="5" name="Picture 4"/>
+          <xdr:cNvPr id="5" name="Picture 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000005000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -34311,7 +34578,13 @@
       </xdr:pic>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="TextBox 5"/>
+          <xdr:cNvPr id="6" name="TextBox 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000006000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -34381,7 +34654,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34419,7 +34698,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34457,7 +34742,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34495,7 +34786,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34525,7 +34822,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34555,7 +34858,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34593,7 +34902,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34636,7 +34951,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34680,7 +35001,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34974,7 +35301,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y231"/>
   <sheetViews>
     <sheetView topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -41402,7 +41729,7 @@
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B167" s="49"/>
       <c r="C167" s="49"/>
@@ -41411,7 +41738,7 @@
       <c r="F167" s="49"/>
       <c r="G167" s="77"/>
       <c r="H167" s="77" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="I167" s="49"/>
       <c r="J167" s="49"/>
@@ -41440,10 +41767,10 @@
         <v>196</v>
       </c>
       <c r="I168" t="s">
+        <v>1242</v>
+      </c>
+      <c r="J168" s="76" t="s">
         <v>1243</v>
-      </c>
-      <c r="J168" s="76" t="s">
-        <v>1244</v>
       </c>
       <c r="K168" s="76" t="s">
         <v>1011</v>
@@ -41455,10 +41782,10 @@
         <v>157</v>
       </c>
       <c r="N168" s="76" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="O168" s="49" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="P168" s="37"/>
       <c r="Q168" s="16"/>
@@ -41764,7 +42091,7 @@
         <v>63.501959516313946</v>
       </c>
       <c r="H176" s="77" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="J176" s="37"/>
       <c r="K176" s="37"/>
@@ -41781,10 +42108,10 @@
         <v>196</v>
       </c>
       <c r="I177" s="37" t="s">
+        <v>1242</v>
+      </c>
+      <c r="J177" s="76" t="s">
         <v>1243</v>
-      </c>
-      <c r="J177" s="76" t="s">
-        <v>1244</v>
       </c>
       <c r="K177" s="76" t="s">
         <v>1011</v>
@@ -41796,10 +42123,10 @@
         <v>157</v>
       </c>
       <c r="N177" s="76" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="O177" s="49" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="178" spans="2:15" x14ac:dyDescent="0.25">
@@ -42080,7 +42407,7 @@
     </row>
     <row r="186" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H186" s="77" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="I186" s="37"/>
       <c r="J186" s="37"/>
@@ -42095,10 +42422,10 @@
         <v>196</v>
       </c>
       <c r="I187" s="37" t="s">
+        <v>1242</v>
+      </c>
+      <c r="J187" s="76" t="s">
         <v>1243</v>
-      </c>
-      <c r="J187" s="76" t="s">
-        <v>1244</v>
       </c>
       <c r="K187" s="76" t="s">
         <v>1011</v>
@@ -42110,10 +42437,10 @@
         <v>157</v>
       </c>
       <c r="N187" s="76" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="O187" s="49" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="188" spans="2:15" x14ac:dyDescent="0.25">
@@ -42349,10 +42676,10 @@
     </row>
     <row r="196" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="H196" s="77" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="I196" s="49"/>
       <c r="J196" s="49"/>
@@ -42367,13 +42694,13 @@
         <v>1072</v>
       </c>
       <c r="C197" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D197" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E197" t="s">
         <v>1298</v>
-      </c>
-      <c r="D197" t="s">
-        <v>1306</v>
-      </c>
-      <c r="E197" t="s">
-        <v>1299</v>
       </c>
       <c r="F197" s="37"/>
       <c r="G197" s="37"/>
@@ -42381,10 +42708,10 @@
         <v>196</v>
       </c>
       <c r="I197" s="37" t="s">
+        <v>1242</v>
+      </c>
+      <c r="J197" s="76" t="s">
         <v>1243</v>
-      </c>
-      <c r="J197" s="76" t="s">
-        <v>1244</v>
       </c>
       <c r="K197" s="76" t="s">
         <v>1011</v>
@@ -42396,10 +42723,10 @@
         <v>157</v>
       </c>
       <c r="N197" s="76" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="O197" s="49" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="198" spans="1:15" x14ac:dyDescent="0.25">
@@ -42557,13 +42884,13 @@
         <v>1072</v>
       </c>
       <c r="C203" s="37" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D203" s="37" t="s">
+        <v>1306</v>
+      </c>
+      <c r="E203" s="37" t="s">
         <v>1300</v>
-      </c>
-      <c r="D203" s="37" t="s">
-        <v>1307</v>
-      </c>
-      <c r="E203" s="37" t="s">
-        <v>1301</v>
       </c>
       <c r="F203" s="37"/>
       <c r="G203" s="37"/>
@@ -42646,13 +42973,13 @@
         <v>1072</v>
       </c>
       <c r="C209" s="37" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D209" s="37" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E209" s="37" t="s">
         <v>1302</v>
-      </c>
-      <c r="D209" s="37" t="s">
-        <v>1308</v>
-      </c>
-      <c r="E209" s="37" t="s">
-        <v>1303</v>
       </c>
     </row>
     <row r="210" spans="2:5" x14ac:dyDescent="0.25">
@@ -42725,13 +43052,13 @@
         <v>1072</v>
       </c>
       <c r="C215" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D215" t="s">
+        <v>1308</v>
+      </c>
+      <c r="E215" t="s">
         <v>1304</v>
-      </c>
-      <c r="D215" t="s">
-        <v>1309</v>
-      </c>
-      <c r="E215" t="s">
-        <v>1305</v>
       </c>
     </row>
     <row r="216" spans="2:5" x14ac:dyDescent="0.25">
@@ -42804,13 +43131,13 @@
         <v>1072</v>
       </c>
       <c r="C221" s="37" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D221" s="37" t="s">
+        <v>1328</v>
+      </c>
+      <c r="E221" s="37" t="s">
         <v>1327</v>
-      </c>
-      <c r="D221" s="37" t="s">
-        <v>1329</v>
-      </c>
-      <c r="E221" s="37" t="s">
-        <v>1328</v>
       </c>
     </row>
     <row r="222" spans="2:5" x14ac:dyDescent="0.25">
@@ -42885,13 +43212,13 @@
         <v>1072</v>
       </c>
       <c r="C227" s="37" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D227" s="37" t="s">
         <v>1330</v>
       </c>
-      <c r="D227" s="37" t="s">
+      <c r="E227" s="37" t="s">
         <v>1331</v>
-      </c>
-      <c r="E227" s="37" t="s">
-        <v>1332</v>
       </c>
     </row>
     <row r="228" spans="2:6" x14ac:dyDescent="0.25">
@@ -42971,10 +43298,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AD213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+    <sheetView topLeftCell="A115" workbookViewId="0">
       <selection activeCell="I142" sqref="I142"/>
     </sheetView>
   </sheetViews>
@@ -43021,10 +43348,10 @@
         <v>144</v>
       </c>
       <c r="J3" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K3" t="s">
         <v>1334</v>
-      </c>
-      <c r="K3" t="s">
-        <v>1335</v>
       </c>
       <c r="N3" s="21" t="s">
         <v>80</v>
@@ -43033,28 +43360,28 @@
         <v>222</v>
       </c>
       <c r="P3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="Q3" t="s">
         <v>1246</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>1247</v>
       </c>
       <c r="R3" s="21" t="s">
         <v>217</v>
       </c>
       <c r="S3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="T3" t="s">
         <v>1246</v>
-      </c>
-      <c r="T3" t="s">
-        <v>1247</v>
       </c>
       <c r="U3" s="21" t="s">
         <v>144</v>
       </c>
       <c r="V3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="W3" t="s">
         <v>1246</v>
-      </c>
-      <c r="W3" t="s">
-        <v>1247</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -43519,13 +43846,13 @@
         <v>392</v>
       </c>
       <c r="O11" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="P11" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="Q11" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="R11" s="8">
         <v>20.7746</v>
@@ -43961,7 +44288,7 @@
       </c>
       <c r="E34" s="54"/>
       <c r="F34" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="G34" s="37">
         <v>1</v>
@@ -43999,7 +44326,7 @@
       </c>
       <c r="E35" s="54"/>
       <c r="F35" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="G35" s="37">
         <v>3.1</v>
@@ -44037,7 +44364,7 @@
       </c>
       <c r="E36" s="54"/>
       <c r="F36" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="G36" s="37">
         <v>6.3</v>
@@ -44075,7 +44402,7 @@
       </c>
       <c r="E37" s="54"/>
       <c r="F37" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="G37" s="37">
         <v>6.6</v>
@@ -44113,7 +44440,7 @@
       </c>
       <c r="E38" s="54"/>
       <c r="F38" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="G38" s="37">
         <v>8.6999999999999993</v>
@@ -44151,7 +44478,7 @@
       </c>
       <c r="E39" s="54"/>
       <c r="F39" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="G39" s="37">
         <v>9.3000000000000007</v>
@@ -44189,7 +44516,7 @@
       </c>
       <c r="E40" s="54"/>
       <c r="F40" s="21" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="G40" s="37">
         <v>9.8000000000000007</v>
@@ -44220,7 +44547,7 @@
       </c>
       <c r="E41" s="54"/>
       <c r="F41" s="21" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="G41" s="37">
         <v>8.4</v>
@@ -44251,7 +44578,7 @@
       </c>
       <c r="E42" s="54"/>
       <c r="F42" s="21" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="G42" s="37">
         <v>4.4000000000000004</v>
@@ -44282,7 +44609,7 @@
       </c>
       <c r="E43" s="54"/>
       <c r="F43" s="21" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="G43" s="37">
         <v>4</v>
@@ -44602,28 +44929,28 @@
         <v>222</v>
       </c>
       <c r="D61" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E61" t="s">
         <v>1246</v>
-      </c>
-      <c r="E61" t="s">
-        <v>1247</v>
       </c>
       <c r="F61" s="21" t="s">
         <v>217</v>
       </c>
       <c r="G61" t="s">
+        <v>1245</v>
+      </c>
+      <c r="H61" t="s">
         <v>1246</v>
-      </c>
-      <c r="H61" t="s">
-        <v>1247</v>
       </c>
       <c r="I61" s="21" t="s">
         <v>144</v>
       </c>
       <c r="J61" t="s">
+        <v>1245</v>
+      </c>
+      <c r="K61" t="s">
         <v>1246</v>
-      </c>
-      <c r="K61" t="s">
-        <v>1247</v>
       </c>
       <c r="M61" s="37" t="s">
         <v>80</v>
@@ -44632,28 +44959,28 @@
         <v>222</v>
       </c>
       <c r="O61" s="37" t="s">
+        <v>1245</v>
+      </c>
+      <c r="P61" s="37" t="s">
         <v>1246</v>
-      </c>
-      <c r="P61" s="37" t="s">
-        <v>1247</v>
       </c>
       <c r="Q61" s="37" t="s">
         <v>217</v>
       </c>
       <c r="R61" s="37" t="s">
+        <v>1245</v>
+      </c>
+      <c r="S61" s="37" t="s">
         <v>1246</v>
-      </c>
-      <c r="S61" s="37" t="s">
-        <v>1247</v>
       </c>
       <c r="T61" s="37" t="s">
         <v>144</v>
       </c>
       <c r="U61" s="37" t="s">
+        <v>1245</v>
+      </c>
+      <c r="V61" s="37" t="s">
         <v>1246</v>
-      </c>
-      <c r="V61" s="37" t="s">
-        <v>1247</v>
       </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
@@ -45095,13 +45422,13 @@
         <v>392</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="D69" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="E69" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="F69" s="8">
         <v>15.9094</v>
@@ -45113,7 +45440,7 @@
         <v>28.742100000000001</v>
       </c>
       <c r="I69" s="31" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="J69" s="8">
         <v>3.0767000000000002</v>
@@ -45125,13 +45452,13 @@
         <v>392</v>
       </c>
       <c r="N69" s="37" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="O69" s="37" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="P69" s="37" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="Q69" s="7">
         <v>9.1097999999999999</v>
@@ -46509,7 +46836,7 @@
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.25">
@@ -46526,7 +46853,7 @@
         <v>576</v>
       </c>
       <c r="G183" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="I183" t="s">
         <v>222</v>
@@ -47690,7 +48017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
@@ -48968,7 +49295,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -49357,17 +49684,17 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -49378,19 +49705,19 @@
         <v>561</v>
       </c>
       <c r="D74" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E74" t="s">
         <v>1234</v>
       </c>
-      <c r="E74" t="s">
+      <c r="F74" t="s">
         <v>1235</v>
       </c>
-      <c r="F74" t="s">
+      <c r="I74" t="s">
         <v>1236</v>
       </c>
-      <c r="I74" t="s">
-        <v>1237</v>
-      </c>
       <c r="J74" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -49582,7 +49909,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -49694,7 +50021,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:Z194"/>
   <sheetViews>
     <sheetView topLeftCell="A172" workbookViewId="0">
@@ -49939,7 +50266,7 @@
     </row>
     <row r="25" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="37" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>1125</v>
@@ -49951,13 +50278,13 @@
         <v>1127</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="G25" s="18" t="s">
         <v>1125</v>
       </c>
       <c r="H25" s="37" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="I25" s="37" t="s">
         <v>1127</v>
@@ -50936,7 +51263,7 @@
         <v>576</v>
       </c>
       <c r="J99" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -51605,7 +51932,7 @@
     <mergeCell ref="C34:E34"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A155" r:id="rId1"/>
+    <hyperlink ref="A155" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -51614,7 +51941,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -51680,7 +52007,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A2:H90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -52564,7 +52891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -53136,11 +53463,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y256"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Y293"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="B174" sqref="B174"/>
+    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
+      <selection activeCell="D281" sqref="D281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54918,10 +55245,7 @@
       <c r="H76" s="21">
         <v>2.343E-3</v>
       </c>
-      <c r="I76" s="41">
-        <f>E76+D76</f>
-        <v>1.0244E-2</v>
-      </c>
+      <c r="I76" s="41"/>
       <c r="K76" s="37" t="s">
         <v>137</v>
       </c>
@@ -55794,7 +56118,7 @@
       </c>
       <c r="H92" s="41"/>
       <c r="K92" s="71" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.25">
@@ -55839,7 +56163,7 @@
         <v>16.8</v>
       </c>
       <c r="K95" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.25">
@@ -55859,7 +56183,7 @@
         <v>490</v>
       </c>
       <c r="M96" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="N96" t="s">
         <v>492</v>
@@ -57679,7 +58003,7 @@
       </c>
       <c r="G194" s="72"/>
       <c r="H194" s="72" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="I194" s="72"/>
       <c r="J194" s="72" t="s">
@@ -58279,17 +58603,1021 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>1138</v>
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B257" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="C257" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="D257" s="37"/>
+      <c r="E257" s="37"/>
+      <c r="F257" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="G257" s="37"/>
+      <c r="H257" s="37"/>
+    </row>
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B258" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="C258" s="37" t="s">
+        <v>490</v>
+      </c>
+      <c r="D258" s="37" t="s">
+        <v>491</v>
+      </c>
+      <c r="E258" s="37" t="s">
+        <v>493</v>
+      </c>
+      <c r="F258" s="37" t="s">
+        <v>490</v>
+      </c>
+      <c r="G258" s="37" t="s">
+        <v>491</v>
+      </c>
+      <c r="H258" s="37" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>1</v>
+      </c>
+      <c r="B259" s="37" t="s">
+        <v>494</v>
+      </c>
+      <c r="C259" s="37">
+        <v>1</v>
+      </c>
+      <c r="D259" s="37">
+        <v>0</v>
+      </c>
+      <c r="E259" s="37">
+        <v>0</v>
+      </c>
+      <c r="F259" s="37">
+        <v>1</v>
+      </c>
+      <c r="G259" s="37">
+        <v>0</v>
+      </c>
+      <c r="H259" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>2</v>
+      </c>
+      <c r="B260" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="C260" s="37">
+        <v>1</v>
+      </c>
+      <c r="D260" s="37">
+        <v>0</v>
+      </c>
+      <c r="E260" s="37">
+        <v>0</v>
+      </c>
+      <c r="F260" s="37">
+        <v>1</v>
+      </c>
+      <c r="G260" s="37">
+        <v>0</v>
+      </c>
+      <c r="H260" s="37">
+        <v>0</v>
+      </c>
+      <c r="J260" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>3</v>
+      </c>
+      <c r="B261" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="C261" s="37">
+        <v>0.97183900000000001</v>
+      </c>
+      <c r="D261" s="37">
+        <v>2.6402999999999999E-2</v>
+      </c>
+      <c r="E261" s="37">
+        <f>1-(C261+D261)</f>
+        <v>1.7580000000000373E-3</v>
+      </c>
+      <c r="F261" s="37">
+        <v>0.97183900000000001</v>
+      </c>
+      <c r="G261" s="37">
+        <v>2.6402999999999999E-2</v>
+      </c>
+      <c r="H261" s="37">
+        <f>1-(F261+G261)</f>
+        <v>1.7580000000000373E-3</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>4</v>
+      </c>
+      <c r="B262" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="C262" s="37">
+        <v>0.87735600000000002</v>
+      </c>
+      <c r="D262" s="37">
+        <v>0.11361499999999999</v>
+      </c>
+      <c r="E262" s="37">
+        <f>1-(C262+D262)</f>
+        <v>9.0289999999999537E-3</v>
+      </c>
+      <c r="F262" s="37">
+        <v>0.87935600000000003</v>
+      </c>
+      <c r="G262" s="37">
+        <v>0.11615</v>
+      </c>
+      <c r="H262" s="37">
+        <f>1-(F262+G262)</f>
+        <v>4.493999999999998E-3</v>
+      </c>
+      <c r="J262">
+        <f>SUM(C262:E262)</f>
+        <v>1</v>
+      </c>
+      <c r="K262">
+        <f>SUM(F262:H262)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>5</v>
+      </c>
+      <c r="B263" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C263" s="37">
+        <v>0.70302699999999996</v>
+      </c>
+      <c r="D263" s="37">
+        <v>0.26659899999999997</v>
+      </c>
+      <c r="E263" s="37">
+        <f t="shared" ref="E263:E274" si="6">1-(C263+D263)</f>
+        <v>3.0374000000000123E-2</v>
+      </c>
+      <c r="F263" s="37">
+        <v>0.73402699999999999</v>
+      </c>
+      <c r="G263" s="37">
+        <v>0.25359900000000002</v>
+      </c>
+      <c r="H263" s="37">
+        <f t="shared" ref="H263:H274" si="7">1-(F263+G263)</f>
+        <v>1.2373999999999996E-2</v>
+      </c>
+      <c r="J263" s="37">
+        <f t="shared" ref="J263:J274" si="8">SUM(C263:E263)</f>
+        <v>1</v>
+      </c>
+      <c r="K263" s="37">
+        <f t="shared" ref="K263:K274" si="9">SUM(F263:H263)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>6</v>
+      </c>
+      <c r="B264" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C264" s="37">
+        <v>0.72545599999999999</v>
+      </c>
+      <c r="D264" s="37">
+        <v>0.26419700000000002</v>
+      </c>
+      <c r="E264" s="37">
+        <f t="shared" si="6"/>
+        <v>1.0346999999999995E-2</v>
+      </c>
+      <c r="F264" s="37">
+        <v>0.731456</v>
+      </c>
+      <c r="G264" s="37">
+        <v>0.22519700000000001</v>
+      </c>
+      <c r="H264" s="37">
+        <f t="shared" si="7"/>
+        <v>4.3347000000000024E-2</v>
+      </c>
+      <c r="J264" s="37">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K264" s="37">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>7</v>
+      </c>
+      <c r="B265" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="C265" s="37">
+        <v>0.73932100000000001</v>
+      </c>
+      <c r="D265" s="37">
+        <v>0.25078</v>
+      </c>
+      <c r="E265" s="85">
+        <f t="shared" si="6"/>
+        <v>9.8989999999999911E-3</v>
+      </c>
+      <c r="F265" s="37">
+        <v>0.731321</v>
+      </c>
+      <c r="G265" s="37">
+        <v>0.2505868</v>
+      </c>
+      <c r="H265" s="37">
+        <f t="shared" si="7"/>
+        <v>1.8092200000000003E-2</v>
+      </c>
+      <c r="J265" s="37">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K265" s="37">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>8</v>
+      </c>
+      <c r="B266" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="C266" s="37">
+        <v>0.76990499999999995</v>
+      </c>
+      <c r="D266" s="37">
+        <v>0.22307099999999999</v>
+      </c>
+      <c r="E266" s="37">
+        <f t="shared" si="6"/>
+        <v>7.0240000000000302E-3</v>
+      </c>
+      <c r="F266" s="37">
+        <v>0.76510500000000004</v>
+      </c>
+      <c r="G266" s="37">
+        <v>0.22507099999999999</v>
+      </c>
+      <c r="H266" s="37">
+        <f t="shared" si="7"/>
+        <v>9.8239999999999439E-3</v>
+      </c>
+      <c r="J266" s="37">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K266" s="37">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>9</v>
+      </c>
+      <c r="B267" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="C267" s="37">
+        <v>0.79022300000000001</v>
+      </c>
+      <c r="D267" s="37">
+        <v>0.20535</v>
+      </c>
+      <c r="E267" s="37">
+        <f t="shared" si="6"/>
+        <v>4.4269999999999587E-3</v>
+      </c>
+      <c r="F267" s="37">
+        <v>0.781223</v>
+      </c>
+      <c r="G267" s="37">
+        <v>0.21535000000000001</v>
+      </c>
+      <c r="H267" s="37">
+        <f t="shared" si="7"/>
+        <v>3.4269999999999579E-3</v>
+      </c>
+      <c r="J267" s="37">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K267" s="37">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>10</v>
+      </c>
+      <c r="B268" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="C268" s="37">
+        <v>0.82640999999999998</v>
+      </c>
+      <c r="D268" s="37">
+        <v>0.16399</v>
+      </c>
+      <c r="E268" s="85">
+        <f t="shared" si="6"/>
+        <v>9.6000000000000529E-3</v>
+      </c>
+      <c r="F268" s="37">
+        <v>0.82640999999999998</v>
+      </c>
+      <c r="G268" s="37">
+        <v>0.16399</v>
+      </c>
+      <c r="H268" s="37">
+        <f t="shared" si="7"/>
+        <v>9.6000000000000529E-3</v>
+      </c>
+      <c r="J268" s="37">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K268" s="37">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A269" s="37">
+        <v>11</v>
+      </c>
+      <c r="B269" s="37" t="s">
+        <v>392</v>
+      </c>
+      <c r="C269" s="37">
+        <v>0.87985000000000002</v>
+      </c>
+      <c r="D269" s="37">
+        <v>0.11162999999999999</v>
+      </c>
+      <c r="E269" s="37">
+        <f t="shared" si="6"/>
+        <v>8.519999999999972E-3</v>
+      </c>
+      <c r="F269" s="37">
+        <v>0.87985000000000002</v>
+      </c>
+      <c r="G269" s="37">
+        <v>0.11162999999999999</v>
+      </c>
+      <c r="H269" s="37">
+        <f t="shared" si="7"/>
+        <v>8.519999999999972E-3</v>
+      </c>
+      <c r="J269" s="37">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K269" s="37">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A270" s="37">
+        <v>12</v>
+      </c>
+      <c r="B270" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="C270" s="37">
+        <v>0.87985000000000002</v>
+      </c>
+      <c r="D270" s="37">
+        <v>0.11162999999999999</v>
+      </c>
+      <c r="E270" s="37">
+        <f t="shared" si="6"/>
+        <v>8.519999999999972E-3</v>
+      </c>
+      <c r="F270" s="37">
+        <v>0.87985000000000002</v>
+      </c>
+      <c r="G270" s="37">
+        <v>0.11162999999999999</v>
+      </c>
+      <c r="H270" s="37">
+        <f t="shared" si="7"/>
+        <v>8.519999999999972E-3</v>
+      </c>
+      <c r="J270" s="37">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K270" s="37">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A271" s="37">
+        <v>13</v>
+      </c>
+      <c r="B271" s="37" t="s">
+        <v>324</v>
+      </c>
+      <c r="C271" s="37">
+        <v>0.87985000000000002</v>
+      </c>
+      <c r="D271" s="37">
+        <v>0.11162999999999999</v>
+      </c>
+      <c r="E271" s="37">
+        <f t="shared" si="6"/>
+        <v>8.519999999999972E-3</v>
+      </c>
+      <c r="F271" s="37">
+        <v>0.87985000000000002</v>
+      </c>
+      <c r="G271" s="37">
+        <v>0.11162999999999999</v>
+      </c>
+      <c r="H271" s="37">
+        <f t="shared" si="7"/>
+        <v>8.519999999999972E-3</v>
+      </c>
+      <c r="J271" s="37">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K271" s="37">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A272" s="37">
+        <v>14</v>
+      </c>
+      <c r="B272" s="37" t="s">
+        <v>462</v>
+      </c>
+      <c r="C272" s="37">
+        <v>0.87985000000000002</v>
+      </c>
+      <c r="D272" s="37">
+        <v>0.11162999999999999</v>
+      </c>
+      <c r="E272" s="37">
+        <f t="shared" si="6"/>
+        <v>8.519999999999972E-3</v>
+      </c>
+      <c r="F272" s="37">
+        <v>0.87985000000000002</v>
+      </c>
+      <c r="G272" s="37">
+        <v>0.11162999999999999</v>
+      </c>
+      <c r="H272" s="37">
+        <f t="shared" si="7"/>
+        <v>8.519999999999972E-3</v>
+      </c>
+      <c r="J272" s="37">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K272" s="37">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A273" s="37">
+        <v>15</v>
+      </c>
+      <c r="B273" s="37" t="s">
+        <v>463</v>
+      </c>
+      <c r="C273" s="37">
+        <v>0.87985000000000002</v>
+      </c>
+      <c r="D273" s="37">
+        <v>0.11162999999999999</v>
+      </c>
+      <c r="E273" s="37">
+        <f t="shared" si="6"/>
+        <v>8.519999999999972E-3</v>
+      </c>
+      <c r="F273" s="37">
+        <v>0.87985000000000002</v>
+      </c>
+      <c r="G273" s="37">
+        <v>0.11162999999999999</v>
+      </c>
+      <c r="H273" s="37">
+        <f t="shared" si="7"/>
+        <v>8.519999999999972E-3</v>
+      </c>
+      <c r="J273" s="37">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K273" s="37">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A274" s="37">
+        <v>16</v>
+      </c>
+      <c r="B274" s="37" t="s">
+        <v>464</v>
+      </c>
+      <c r="C274" s="37">
+        <v>0.87985000000000002</v>
+      </c>
+      <c r="D274" s="37">
+        <v>0.11162999999999999</v>
+      </c>
+      <c r="E274" s="37">
+        <f t="shared" si="6"/>
+        <v>8.519999999999972E-3</v>
+      </c>
+      <c r="F274" s="37">
+        <v>0.87985000000000002</v>
+      </c>
+      <c r="G274" s="37">
+        <v>0.11162999999999999</v>
+      </c>
+      <c r="H274" s="37">
+        <f t="shared" si="7"/>
+        <v>8.519999999999972E-3</v>
+      </c>
+      <c r="J274" s="37">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K274" s="37">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B275" s="37"/>
+      <c r="C275" s="37"/>
+      <c r="D275" s="37"/>
+      <c r="E275" s="37"/>
+      <c r="F275" s="37"/>
+      <c r="G275" s="37"/>
+      <c r="H275" s="37"/>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B276" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C276" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="D276" s="37"/>
+      <c r="E276" s="37"/>
+      <c r="F276" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="G276" s="37"/>
+      <c r="H276" s="37"/>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B277" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="C277" s="37" t="s">
+        <v>490</v>
+      </c>
+      <c r="D277" s="37" t="s">
+        <v>491</v>
+      </c>
+      <c r="E277" s="37" t="s">
+        <v>493</v>
+      </c>
+      <c r="F277" s="37" t="s">
+        <v>490</v>
+      </c>
+      <c r="G277" s="37" t="s">
+        <v>491</v>
+      </c>
+      <c r="H277" s="37" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B278" s="37" t="s">
+        <v>494</v>
+      </c>
+      <c r="C278" s="29">
+        <v>1</v>
+      </c>
+      <c r="D278" s="37">
+        <v>0</v>
+      </c>
+      <c r="E278" s="37">
+        <v>0</v>
+      </c>
+      <c r="F278" s="37">
+        <v>1</v>
+      </c>
+      <c r="G278" s="37">
+        <v>0</v>
+      </c>
+      <c r="H278" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B279" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="C279" s="29">
+        <v>1</v>
+      </c>
+      <c r="D279" s="37">
+        <v>0</v>
+      </c>
+      <c r="E279" s="37">
+        <v>0</v>
+      </c>
+      <c r="F279" s="37">
+        <v>1</v>
+      </c>
+      <c r="G279" s="37">
+        <v>0</v>
+      </c>
+      <c r="H279" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B280" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="C280" s="29">
+        <v>1</v>
+      </c>
+      <c r="D280" s="37">
+        <v>0</v>
+      </c>
+      <c r="E280" s="37">
+        <v>0</v>
+      </c>
+      <c r="F280" s="37">
+        <v>1</v>
+      </c>
+      <c r="G280" s="37">
+        <v>0</v>
+      </c>
+      <c r="H280" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B281" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="C281" s="29">
+        <v>0.98975599999999997</v>
+      </c>
+      <c r="D281" s="37">
+        <v>1.0069E-2</v>
+      </c>
+      <c r="E281" s="37">
+        <v>1.7500000000000003E-4</v>
+      </c>
+      <c r="F281" s="37">
+        <v>0.96245199999999997</v>
+      </c>
+      <c r="G281" s="37">
+        <v>3.5205E-2</v>
+      </c>
+      <c r="H281" s="37">
+        <v>2.343E-3</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B282" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C282" s="29">
+        <v>0.97952399999999995</v>
+      </c>
+      <c r="D282" s="37">
+        <v>2.0166E-2</v>
+      </c>
+      <c r="E282" s="37">
+        <v>3.1E-4</v>
+      </c>
+      <c r="F282" s="37">
+        <v>0.8334180000000001</v>
+      </c>
+      <c r="G282" s="37">
+        <v>0.157748</v>
+      </c>
+      <c r="H282" s="37">
+        <v>8.8339999999999998E-3</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B283" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C283" s="29">
+        <v>0.98680599999999996</v>
+      </c>
+      <c r="D283" s="37">
+        <v>1.2837000000000001E-2</v>
+      </c>
+      <c r="E283" s="37">
+        <v>3.57E-4</v>
+      </c>
+      <c r="F283" s="37">
+        <v>0.825658</v>
+      </c>
+      <c r="G283" s="37">
+        <v>0.16295100000000001</v>
+      </c>
+      <c r="H283" s="37">
+        <v>1.1391E-2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B284" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="C284" s="29">
+        <v>0.98374700000000004</v>
+      </c>
+      <c r="D284" s="37">
+        <v>1.6253E-2</v>
+      </c>
+      <c r="E284" s="20">
+        <v>4.6700000000000002E-4</v>
+      </c>
+      <c r="F284" s="37">
+        <v>0.84771699999999994</v>
+      </c>
+      <c r="G284" s="37">
+        <v>0.149064</v>
+      </c>
+      <c r="H284" s="37">
+        <v>3.2200000000000002E-3</v>
+      </c>
+    </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B285" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="C285" s="29">
+        <v>0.98370900000000006</v>
+      </c>
+      <c r="D285" s="37">
+        <v>1.5713999999999999E-2</v>
+      </c>
+      <c r="E285" s="37">
+        <v>5.7700000000000004E-4</v>
+      </c>
+      <c r="F285" s="37">
+        <v>0.86167599999999989</v>
+      </c>
+      <c r="G285" s="37">
+        <v>0.13456400000000002</v>
+      </c>
+      <c r="H285" s="37">
+        <v>3.7599999999999999E-3</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B286" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="C286" s="29">
+        <v>0.99171000000000009</v>
+      </c>
+      <c r="D286" s="37">
+        <v>7.8080000000000007E-3</v>
+      </c>
+      <c r="E286" s="37">
+        <v>4.8200000000000001E-4</v>
+      </c>
+      <c r="F286" s="37">
+        <v>0.88590000000000002</v>
+      </c>
+      <c r="G286" s="37">
+        <v>0.11090999999999999</v>
+      </c>
+      <c r="H286" s="37">
+        <v>3.1900000000000001E-3</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B287" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="C287" s="29">
+        <v>0.99118399999999995</v>
+      </c>
+      <c r="D287" s="37">
+        <v>8.8160000000000009E-3</v>
+      </c>
+      <c r="E287" s="37">
+        <v>0</v>
+      </c>
+      <c r="F287" s="37">
+        <v>0.87293999999999994</v>
+      </c>
+      <c r="G287" s="37">
+        <v>0.126001</v>
+      </c>
+      <c r="H287" s="37">
+        <v>1.059E-3</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B288" s="37" t="s">
+        <v>392</v>
+      </c>
+      <c r="C288" s="29">
+        <v>0.99118399999999995</v>
+      </c>
+      <c r="D288" s="37">
+        <v>8.8160000000000009E-3</v>
+      </c>
+      <c r="E288" s="37">
+        <v>0</v>
+      </c>
+      <c r="F288" s="37">
+        <v>0.88538499999999998</v>
+      </c>
+      <c r="G288" s="37">
+        <v>0.10356299999999999</v>
+      </c>
+      <c r="H288" s="37">
+        <v>1.1051999999999999E-2</v>
+      </c>
+    </row>
+    <row r="289" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B289" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="C289" s="29">
+        <v>0.99118399999999995</v>
+      </c>
+      <c r="D289" s="37">
+        <v>8.8160000000000009E-3</v>
+      </c>
+      <c r="E289" s="37">
+        <v>0</v>
+      </c>
+      <c r="F289" s="37">
+        <v>0.88538499999999998</v>
+      </c>
+      <c r="G289" s="37">
+        <v>0.10356299999999999</v>
+      </c>
+      <c r="H289" s="37">
+        <v>1.1051999999999999E-2</v>
+      </c>
+    </row>
+    <row r="290" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B290" s="37" t="s">
+        <v>324</v>
+      </c>
+      <c r="C290" s="29">
+        <v>0.99118399999999995</v>
+      </c>
+      <c r="D290" s="37">
+        <v>8.8160000000000009E-3</v>
+      </c>
+      <c r="E290" s="37">
+        <v>0</v>
+      </c>
+      <c r="F290" s="37">
+        <v>0.88538499999999998</v>
+      </c>
+      <c r="G290" s="37">
+        <v>0.10356299999999999</v>
+      </c>
+      <c r="H290" s="37">
+        <v>1.1051999999999999E-2</v>
+      </c>
+    </row>
+    <row r="291" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B291" s="37" t="s">
+        <v>462</v>
+      </c>
+      <c r="C291" s="29">
+        <v>0.99118399999999995</v>
+      </c>
+      <c r="D291" s="37">
+        <v>8.8160000000000009E-3</v>
+      </c>
+      <c r="E291" s="37">
+        <v>0</v>
+      </c>
+      <c r="F291" s="37">
+        <v>0.88538499999999998</v>
+      </c>
+      <c r="G291" s="37">
+        <v>0.10356299999999999</v>
+      </c>
+      <c r="H291" s="37">
+        <v>1.1051999999999999E-2</v>
+      </c>
+    </row>
+    <row r="292" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B292" s="37" t="s">
+        <v>463</v>
+      </c>
+      <c r="C292" s="29">
+        <v>0.99118399999999995</v>
+      </c>
+      <c r="D292" s="37">
+        <v>8.8160000000000009E-3</v>
+      </c>
+      <c r="E292" s="37">
+        <v>0</v>
+      </c>
+      <c r="F292" s="37">
+        <v>0.88538499999999998</v>
+      </c>
+      <c r="G292" s="37">
+        <v>0.10356299999999999</v>
+      </c>
+      <c r="H292" s="37">
+        <v>1.1051999999999999E-2</v>
+      </c>
+    </row>
+    <row r="293" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B293" s="37" t="s">
+        <v>464</v>
+      </c>
+      <c r="C293" s="29">
+        <v>0.99118399999999995</v>
+      </c>
+      <c r="D293" s="37">
+        <v>8.8160000000000009E-3</v>
+      </c>
+      <c r="E293" s="37">
+        <v>0</v>
+      </c>
+      <c r="F293" s="37">
+        <v>0.88538499999999998</v>
+      </c>
+      <c r="G293" s="37">
+        <v>0.10356299999999999</v>
+      </c>
+      <c r="H293" s="37">
+        <v>1.1051999999999999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -58300,7 +59628,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S68"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
@@ -58326,10 +59654,10 @@
         <v>158</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="O2" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -58343,7 +59671,7 @@
         <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="G3" t="s">
         <v>575</v>
@@ -58573,7 +59901,7 @@
         <v>59.412199999999999</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="K9" s="7">
         <v>39.2258</v>
@@ -58628,15 +59956,15 @@
     <row r="12" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="14" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="37" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="15" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -58665,7 +59993,7 @@
         <v>576</v>
       </c>
       <c r="L15" s="37" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -58829,7 +60157,7 @@
         <v>80.099999999999994</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="H21" s="7">
         <v>39.386299999999999</v>
@@ -58862,7 +60190,7 @@
     <row r="23" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -58890,7 +60218,7 @@
         <v>246</v>
       </c>
       <c r="G27" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="H27" t="s">
         <v>575</v>
@@ -58922,22 +60250,22 @@
         <v>155</v>
       </c>
       <c r="G28" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="H28" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="I28" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="J28" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="K28" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="L28" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -58951,48 +60279,48 @@
         <v>91.2</v>
       </c>
       <c r="F29" s="37" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="H29" s="37" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="I29" s="37" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="J29" s="37" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="K29" s="37" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="L29" s="37" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F30" s="37" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="G30" s="37" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="H30" s="37" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="I30" s="37" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="J30" s="37" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="K30" s="37" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="L30" s="37" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -59000,25 +60328,25 @@
         <v>418</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="G31" s="37" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="H31" s="37" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="I31" s="37" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="J31" s="37" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="K31" s="37" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="L31" s="37" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -59029,25 +60357,25 @@
         <v>2012</v>
       </c>
       <c r="F32" s="37" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="G32" s="37" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="H32" s="37" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="I32" s="37" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="J32" s="37" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="K32" s="37" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="L32" s="37" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -59085,7 +60413,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -59099,7 +60427,7 @@
         <v>179</v>
       </c>
       <c r="J38" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -59334,7 +60662,7 @@
         <v>68</v>
       </c>
       <c r="J45" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="K45" s="7">
         <v>60.636200000000002</v>
@@ -59391,17 +60719,17 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="37" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -59411,7 +60739,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="57" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -59594,7 +60922,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AL153"/>
   <sheetViews>
     <sheetView topLeftCell="A127" workbookViewId="0">
@@ -62874,7 +64202,7 @@
         <v>456</v>
       </c>
       <c r="J103" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="104" spans="2:32" x14ac:dyDescent="0.25">
@@ -63504,7 +64832,7 @@
         <v>7.4809999999999999</v>
       </c>
       <c r="K127" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="128" spans="2:11" x14ac:dyDescent="0.25">
@@ -63515,7 +64843,7 @@
         <v>7.4809999999999999</v>
       </c>
       <c r="K128" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="129" spans="6:11" x14ac:dyDescent="0.25">
@@ -63526,7 +64854,7 @@
         <v>7.4809999999999999</v>
       </c>
       <c r="K129" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="130" spans="6:11" x14ac:dyDescent="0.25">
@@ -63540,7 +64868,7 @@
         <v>7.4809999999999999</v>
       </c>
       <c r="K130" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="131" spans="6:11" x14ac:dyDescent="0.25">
@@ -63554,7 +64882,7 @@
         <v>7.7850000000000001</v>
       </c>
       <c r="K131" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="132" spans="6:11" x14ac:dyDescent="0.25">
@@ -63568,7 +64896,7 @@
         <v>8.0650000000000013</v>
       </c>
       <c r="K132" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="133" spans="6:11" x14ac:dyDescent="0.25">
@@ -63582,7 +64910,7 @@
         <v>8.1100000000000012</v>
       </c>
       <c r="K133" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="134" spans="6:11" x14ac:dyDescent="0.25">
@@ -63596,7 +64924,7 @@
         <v>7.99</v>
       </c>
       <c r="K134" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="135" spans="6:11" x14ac:dyDescent="0.25">
@@ -63610,7 +64938,7 @@
         <v>7.64</v>
       </c>
       <c r="K135" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="136" spans="6:11" x14ac:dyDescent="0.25">
@@ -63624,7 +64952,7 @@
         <v>7.2160000000000002</v>
       </c>
       <c r="K136" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="137" spans="6:11" x14ac:dyDescent="0.25">
@@ -64216,7 +65544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AX132"/>
   <sheetViews>
     <sheetView topLeftCell="A92" workbookViewId="0">
@@ -65124,25 +66452,25 @@
         <v>80</v>
       </c>
       <c r="C71" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D71" t="s">
         <v>1310</v>
       </c>
-      <c r="D71" t="s">
-        <v>1311</v>
-      </c>
       <c r="E71" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="F71" t="s">
         <v>246</v>
       </c>
       <c r="G71" t="s">
+        <v>1311</v>
+      </c>
+      <c r="H71" t="s">
         <v>1312</v>
       </c>
-      <c r="H71" t="s">
-        <v>1313</v>
-      </c>
       <c r="I71" s="37" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="J71" s="37" t="s">
         <v>246</v>
@@ -65876,10 +67204,10 @@
     </row>
     <row r="91" spans="1:50" x14ac:dyDescent="0.25">
       <c r="U91" t="s">
+        <v>1228</v>
+      </c>
+      <c r="AF91" t="s">
         <v>1229</v>
-      </c>
-      <c r="AF91" t="s">
-        <v>1230</v>
       </c>
     </row>
     <row r="92" spans="1:50" x14ac:dyDescent="0.25">
@@ -65887,16 +67215,16 @@
         <v>1071</v>
       </c>
       <c r="R92" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="U92" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="V92">
         <v>0.5</v>
       </c>
       <c r="W92" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="X92">
         <v>0.4</v>
@@ -65908,23 +67236,23 @@
         <v>0.25</v>
       </c>
       <c r="AA92" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="AB92">
         <v>0.15</v>
       </c>
       <c r="AC92" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="AD92">
         <v>0.15</v>
       </c>
       <c r="AF92" s="37" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="AG92" s="37"/>
       <c r="AH92" s="37" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="AI92" s="37"/>
       <c r="AJ92" s="37">
@@ -65932,11 +67260,11 @@
       </c>
       <c r="AK92" s="37"/>
       <c r="AL92" s="37" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="AM92" s="37"/>
       <c r="AN92" s="37" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="AO92" s="37"/>
       <c r="AP92" s="37"/>
@@ -65990,7 +67318,7 @@
         <v>222</v>
       </c>
       <c r="R93" s="37" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="S93" s="37">
         <v>1.5</v>
@@ -66108,7 +67436,7 @@
         <v>2.6945755989701607E-2</v>
       </c>
       <c r="R94" s="37" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="S94" s="37">
         <v>1.4</v>
@@ -66317,7 +67645,7 @@
         <v>5.2077410999999999E-4</v>
       </c>
       <c r="R96" s="37" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="S96" s="37">
         <v>1.1499999999999999</v>
@@ -66423,7 +67751,7 @@
         <v>8.5921136E-4</v>
       </c>
       <c r="R97" s="37" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="S97" s="37">
         <v>1.1499999999999999</v>
@@ -68121,7 +69449,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R247"/>
   <sheetViews>
     <sheetView topLeftCell="A112" workbookViewId="0">
@@ -69007,7 +70335,7 @@
         <v>106</v>
       </c>
       <c r="H71" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -69621,7 +70949,7 @@
         <v>1</v>
       </c>
       <c r="H130" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -70533,13 +71861,13 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="198" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="37" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
@@ -70569,12 +71897,12 @@
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.25">
@@ -70582,15 +71910,15 @@
         <v>74</v>
       </c>
       <c r="D210" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="E210" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="211" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C211">
         <v>36</v>
@@ -70601,7 +71929,7 @@
     </row>
     <row r="212" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C212">
         <v>67</v>
@@ -70612,7 +71940,7 @@
     </row>
     <row r="213" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C213">
         <v>51</v>
@@ -70623,7 +71951,7 @@
     </row>
     <row r="214" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C214">
         <v>43</v>
@@ -70634,7 +71962,7 @@
     </row>
     <row r="215" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C215">
         <v>52</v>
@@ -70682,35 +72010,35 @@
     </row>
     <row r="220" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="221" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="222" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C222" s="66" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D222" s="66" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E222" s="66" t="s">
         <v>1181</v>
-      </c>
-      <c r="C222" s="66" t="s">
-        <v>1185</v>
-      </c>
-      <c r="D222" s="66" t="s">
-        <v>1179</v>
-      </c>
-      <c r="E222" s="66" t="s">
-        <v>1182</v>
       </c>
       <c r="F222" s="66" t="s">
         <v>576</v>
       </c>
       <c r="G222" s="67" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="H222" s="67" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="I222" s="67" t="s">
         <v>575</v>
@@ -70728,24 +72056,24 @@
         <v>576</v>
       </c>
       <c r="N222" s="69" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="O222" s="69" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="P222" s="69" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="223" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B223" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C223" s="66" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="D223" s="66">
         <v>22.2</v>
@@ -70757,7 +72085,7 @@
         <v>29.8</v>
       </c>
       <c r="G223" s="67" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="H223" s="67">
         <v>76.900000000000006</v>
@@ -70781,21 +72109,21 @@
         <v>7.8</v>
       </c>
       <c r="O223" s="69" t="s">
+        <v>1206</v>
+      </c>
+      <c r="P223" s="69" t="s">
         <v>1207</v>
-      </c>
-      <c r="P223" s="69" t="s">
-        <v>1208</v>
       </c>
     </row>
     <row r="224" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B224" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="C224" s="66" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="D224" s="66">
         <v>15.8</v>
@@ -70807,7 +72135,7 @@
         <v>17.7</v>
       </c>
       <c r="G224" s="67" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="H224" s="67">
         <v>25.7</v>
@@ -70832,24 +72160,24 @@
         <v>7.7220077220077217</v>
       </c>
       <c r="O224" s="69" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="P224" s="69">
         <v>2009</v>
       </c>
       <c r="Q224" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B225" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C225" s="66" t="s">
         <v>1192</v>
-      </c>
-      <c r="C225" s="66" t="s">
-        <v>1193</v>
       </c>
       <c r="D225" s="66">
         <v>38.700000000000003</v>
@@ -70861,7 +72189,7 @@
         <v>41.8</v>
       </c>
       <c r="G225" s="67" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="H225" s="67">
         <v>74.099999999999994</v>
@@ -70885,7 +72213,7 @@
         <v>30</v>
       </c>
       <c r="O225" s="69" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="P225" s="69">
         <v>2006</v>
@@ -70893,15 +72221,15 @@
     </row>
     <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="M227" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="M228" t="s">
         <v>559</v>
@@ -70921,7 +72249,7 @@
         <v>106</v>
       </c>
       <c r="E229" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F229" t="s">
         <v>575</v>
@@ -70936,10 +72264,10 @@
         <v>106</v>
       </c>
       <c r="K229" s="37" t="s">
+        <v>1203</v>
+      </c>
+      <c r="M229" t="s">
         <v>1204</v>
-      </c>
-      <c r="M229" t="s">
-        <v>1205</v>
       </c>
       <c r="N229" t="s">
         <v>575</v>
@@ -70948,7 +72276,7 @@
         <v>576</v>
       </c>
       <c r="P229" s="37" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="Q229" s="37" t="s">
         <v>575</v>
@@ -70959,7 +72287,7 @@
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="C230">
         <v>9</v>
@@ -71241,7 +72569,7 @@
     </row>
     <row r="236" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="C236">
         <v>54</v>
@@ -71288,7 +72616,7 @@
     </row>
     <row r="238" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="I238" s="37" t="s">
         <v>559</v>
@@ -71491,7 +72819,7 @@
     </row>
     <row r="244" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C244">
         <v>189</v>
@@ -71533,7 +72861,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L38" r:id="rId1"/>
+    <hyperlink ref="L38" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -71542,7 +72870,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -71940,12 +73268,12 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -71969,7 +73297,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="C59" s="18">
         <v>0.13100000000000001</v>
@@ -71991,7 +73319,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C61" s="18">
         <v>0.27400000000000002</v>
@@ -72003,17 +73331,17 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
@@ -72026,7 +73354,7 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C67">
         <v>112</v>
@@ -72085,7 +73413,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
@@ -72785,30 +74113,30 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="65" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="37" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="E65" s="37" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="E66" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="F66" t="s">
         <v>188</v>
       </c>
       <c r="G66" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -72864,7 +74192,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="C70">
         <v>1.2</v>
@@ -72898,7 +74226,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -72921,7 +74249,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView topLeftCell="A69" workbookViewId="0">
@@ -73219,13 +74547,13 @@
         <v>150</v>
       </c>
       <c r="C45" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E45" t="s">
         <v>1165</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>1166</v>
-      </c>
-      <c r="F45" t="s">
-        <v>1167</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
@@ -73543,12 +74871,12 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="C79">
         <v>20.5</v>
@@ -73562,12 +74890,12 @@
         <v>32.5</v>
       </c>
       <c r="D80" s="37" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -73577,23 +74905,23 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C84">
         <v>34.5</v>
       </c>
       <c r="D84" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -73606,7 +74934,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C89">
         <v>42.7</v>
@@ -73614,13 +74942,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="37" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
increase partnerships in medium risk
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Kenya_model_HPV-HIVacq\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439A778B-5E26-4CE1-941E-87EC09E4DE75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D587688-4C12-4E46-99D0-61383D7559E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9345" windowHeight="12195" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="10" r:id="rId1"/>
@@ -53467,8 +53467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="D193" sqref="D193:F193"/>
+    <sheetView tabSelected="1" topLeftCell="A254" workbookViewId="0">
+      <selection activeCell="F269" sqref="F269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58743,20 +58743,20 @@
         <v>137</v>
       </c>
       <c r="C262" s="59">
-        <v>0.87735600000000002</v>
+        <v>0.75735600000000003</v>
       </c>
       <c r="D262" s="59">
-        <v>0.11361499999999999</v>
+        <v>0.23361499999999999</v>
       </c>
       <c r="E262" s="59">
         <f>1-(C262+D262)</f>
         <v>9.0289999999999537E-3</v>
       </c>
       <c r="F262" s="59">
-        <v>0.87935600000000003</v>
+        <v>0.77935600000000005</v>
       </c>
       <c r="G262" s="59">
-        <v>0.11615</v>
+        <v>0.21615000000000001</v>
       </c>
       <c r="H262" s="59">
         <f>1-(F262+G262)</f>
@@ -58771,20 +58771,20 @@
         <v>138</v>
       </c>
       <c r="C263" s="59">
-        <v>0.70302699999999996</v>
+        <v>0.503027</v>
       </c>
       <c r="D263" s="59">
-        <v>0.26659899999999997</v>
+        <v>0.46659899999999999</v>
       </c>
       <c r="E263" s="59">
         <f t="shared" ref="E263:E274" si="6">1-(C263+D263)</f>
-        <v>3.0374000000000123E-2</v>
+        <v>3.0374000000000012E-2</v>
       </c>
       <c r="F263" s="59">
-        <v>0.73402699999999999</v>
+        <v>0.53402700000000003</v>
       </c>
       <c r="G263" s="59">
-        <v>0.25359900000000002</v>
+        <v>0.45359899999999997</v>
       </c>
       <c r="H263" s="59">
         <f t="shared" ref="H263:H274" si="7">1-(F263+G263)</f>
@@ -58799,20 +58799,20 @@
         <v>139</v>
       </c>
       <c r="C264" s="59">
-        <v>0.72545599999999999</v>
+        <v>0.52545600000000003</v>
       </c>
       <c r="D264" s="59">
-        <v>0.26419700000000002</v>
+        <v>0.46419700000000003</v>
       </c>
       <c r="E264" s="59">
         <f t="shared" si="6"/>
-        <v>1.0346999999999995E-2</v>
+        <v>1.0346999999999884E-2</v>
       </c>
       <c r="F264" s="59">
-        <v>0.75145600000000001</v>
+        <v>0.55145599999999995</v>
       </c>
       <c r="G264" s="59">
-        <v>0.22519700000000001</v>
+        <v>0.42519699999999999</v>
       </c>
       <c r="H264" s="59">
         <f t="shared" si="7"/>
@@ -58827,20 +58827,20 @@
         <v>140</v>
       </c>
       <c r="C265" s="59">
-        <v>0.73932100000000001</v>
+        <v>0.609321</v>
       </c>
       <c r="D265" s="59">
-        <v>0.25078</v>
+        <v>0.38078000000000001</v>
       </c>
       <c r="E265" s="59">
         <f t="shared" si="6"/>
         <v>9.8989999999999911E-3</v>
       </c>
       <c r="F265" s="59">
-        <v>0.731321</v>
+        <v>0.60132099999999999</v>
       </c>
       <c r="G265" s="59">
-        <v>0.2505868</v>
+        <v>0.3805868</v>
       </c>
       <c r="H265" s="59">
         <f t="shared" si="7"/>
@@ -58855,24 +58855,24 @@
         <v>141</v>
       </c>
       <c r="C266" s="59">
-        <v>0.76990499999999995</v>
+        <v>0.72990500000000003</v>
       </c>
       <c r="D266" s="59">
-        <v>0.22307099999999999</v>
+        <v>0.263071</v>
       </c>
       <c r="E266" s="59">
         <f t="shared" si="6"/>
-        <v>7.0240000000000302E-3</v>
+        <v>7.0239999999999192E-3</v>
       </c>
       <c r="F266" s="59">
-        <v>0.76510500000000004</v>
+        <v>0.70510499999999998</v>
       </c>
       <c r="G266" s="59">
-        <v>0.22507099999999999</v>
+        <v>0.28507100000000002</v>
       </c>
       <c r="H266" s="59">
         <f t="shared" si="7"/>
-        <v>9.8239999999999439E-3</v>
+        <v>9.8240000000000549E-3</v>
       </c>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.25">
@@ -58893,14 +58893,14 @@
         <v>3.4269999999999579E-3</v>
       </c>
       <c r="F267" s="59">
-        <v>0.781223</v>
+        <v>0.73122299999999996</v>
       </c>
       <c r="G267" s="59">
-        <v>0.21535000000000001</v>
+        <v>0.26534999999999997</v>
       </c>
       <c r="H267" s="59">
         <f t="shared" si="7"/>
-        <v>3.4269999999999579E-3</v>
+        <v>3.4270000000000689E-3</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
@@ -58921,10 +58921,10 @@
         <v>9.6000000000000529E-3</v>
       </c>
       <c r="F268" s="59">
-        <v>0.82640999999999998</v>
+        <v>0.80640999999999996</v>
       </c>
       <c r="G268" s="59">
-        <v>0.16399</v>
+        <v>0.18398999999999999</v>
       </c>
       <c r="H268" s="59">
         <f t="shared" si="7"/>
@@ -59255,7 +59255,7 @@
         <v>138</v>
       </c>
       <c r="C283" s="7">
-        <v>0.67400099999999996</v>
+        <v>0.87400100000000003</v>
       </c>
       <c r="D283" s="7">
         <v>2.173962</v>
@@ -59264,7 +59264,7 @@
         <v>7.7805770000000001</v>
       </c>
       <c r="F283" s="7">
-        <v>0.67400099999999996</v>
+        <v>0.87400100000000003</v>
       </c>
       <c r="G283" s="7">
         <v>2.173962</v>
@@ -59303,7 +59303,7 @@
         <v>140</v>
       </c>
       <c r="C285" s="7">
-        <v>0.93245599999999995</v>
+        <v>0.95</v>
       </c>
       <c r="D285" s="7">
         <v>2.1315270000000002</v>
@@ -59313,7 +59313,7 @@
         <v>11.7085092</v>
       </c>
       <c r="F285" s="7">
-        <v>0.93245599999999995</v>
+        <v>0.95</v>
       </c>
       <c r="G285" s="7">
         <v>2.1315270000000002</v>
@@ -59351,7 +59351,7 @@
         <v>142</v>
       </c>
       <c r="C287" s="7">
-        <v>0.94899599999999995</v>
+        <v>0.93</v>
       </c>
       <c r="D287" s="7">
         <v>2.0623269999999998</v>
@@ -59361,7 +59361,7 @@
         <v>8.2758765000000007</v>
       </c>
       <c r="F287" s="7">
-        <v>0.94899599999999995</v>
+        <v>0.93</v>
       </c>
       <c r="G287" s="7">
         <v>2.0623269999999998</v>

</xml_diff>

<commit_message>
add riskAdj back in
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Kenya_model_HPV-HIVacq\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D587688-4C12-4E46-99D0-61383D7559E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235D0CA0-BE19-4822-9A77-5875087583A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9345" windowHeight="12195" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53467,8 +53467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A254" workbookViewId="0">
-      <selection activeCell="F269" sqref="F269"/>
+    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
+      <selection activeCell="C264" sqref="C264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58771,14 +58771,14 @@
         <v>138</v>
       </c>
       <c r="C263" s="59">
-        <v>0.503027</v>
+        <v>0.505027</v>
       </c>
       <c r="D263" s="59">
         <v>0.46659899999999999</v>
       </c>
       <c r="E263" s="59">
         <f t="shared" ref="E263:E274" si="6">1-(C263+D263)</f>
-        <v>3.0374000000000012E-2</v>
+        <v>2.837400000000001E-2</v>
       </c>
       <c r="F263" s="59">
         <v>0.53402700000000003</v>
@@ -58799,14 +58799,14 @@
         <v>139</v>
       </c>
       <c r="C264" s="59">
-        <v>0.52545600000000003</v>
+        <v>0.58545599999999998</v>
       </c>
       <c r="D264" s="59">
-        <v>0.46419700000000003</v>
+        <v>0.40419699999999997</v>
       </c>
       <c r="E264" s="59">
         <f t="shared" si="6"/>
-        <v>1.0346999999999884E-2</v>
+        <v>1.0347000000000106E-2</v>
       </c>
       <c r="F264" s="59">
         <v>0.55145599999999995</v>
@@ -58827,24 +58827,24 @@
         <v>140</v>
       </c>
       <c r="C265" s="59">
-        <v>0.609321</v>
+        <v>0.62932100000000002</v>
       </c>
       <c r="D265" s="59">
-        <v>0.38078000000000001</v>
+        <v>0.36077999999999999</v>
       </c>
       <c r="E265" s="59">
         <f t="shared" si="6"/>
         <v>9.8989999999999911E-3</v>
       </c>
       <c r="F265" s="59">
-        <v>0.60132099999999999</v>
+        <v>0.605321</v>
       </c>
       <c r="G265" s="59">
         <v>0.3805868</v>
       </c>
       <c r="H265" s="59">
         <f t="shared" si="7"/>
-        <v>1.8092200000000003E-2</v>
+        <v>1.4092199999999999E-2</v>
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.25">
@@ -58886,21 +58886,21 @@
         <v>0.781223</v>
       </c>
       <c r="D267" s="59">
-        <v>0.21535000000000001</v>
+        <v>0.21335000000000001</v>
       </c>
       <c r="E267" s="59">
         <f t="shared" si="6"/>
-        <v>3.4269999999999579E-3</v>
+        <v>5.4269999999999596E-3</v>
       </c>
       <c r="F267" s="59">
         <v>0.73122299999999996</v>
       </c>
       <c r="G267" s="59">
-        <v>0.26534999999999997</v>
+        <v>0.26235000000000003</v>
       </c>
       <c r="H267" s="59">
         <f t="shared" si="7"/>
-        <v>3.4270000000000689E-3</v>
+        <v>6.4269999999999605E-3</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
@@ -58914,21 +58914,21 @@
         <v>0.82640999999999998</v>
       </c>
       <c r="D268" s="59">
-        <v>0.16399</v>
+        <v>0.16899</v>
       </c>
       <c r="E268" s="59">
         <f t="shared" si="6"/>
-        <v>9.6000000000000529E-3</v>
+        <v>4.6000000000000485E-3</v>
       </c>
       <c r="F268" s="59">
         <v>0.80640999999999996</v>
       </c>
       <c r="G268" s="59">
-        <v>0.18398999999999999</v>
+        <v>0.18798999999999999</v>
       </c>
       <c r="H268" s="59">
         <f t="shared" si="7"/>
-        <v>9.6000000000000529E-3</v>
+        <v>5.6000000000000494E-3</v>
       </c>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.25">
@@ -58942,21 +58942,21 @@
         <v>0.87985000000000002</v>
       </c>
       <c r="D269" s="59">
-        <v>0.11162999999999999</v>
+        <v>0.11563</v>
       </c>
       <c r="E269" s="59">
         <f t="shared" si="6"/>
-        <v>8.519999999999972E-3</v>
+        <v>4.5199999999999685E-3</v>
       </c>
       <c r="F269" s="59">
         <v>0.87985000000000002</v>
       </c>
       <c r="G269" s="59">
-        <v>0.11162999999999999</v>
+        <v>0.11563</v>
       </c>
       <c r="H269" s="59">
         <f t="shared" si="7"/>
-        <v>8.519999999999972E-3</v>
+        <v>4.5199999999999685E-3</v>
       </c>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.25">
@@ -58970,21 +58970,21 @@
         <v>0.87985000000000002</v>
       </c>
       <c r="D270" s="59">
-        <v>0.11162999999999999</v>
+        <v>0.11563</v>
       </c>
       <c r="E270" s="59">
         <f t="shared" si="6"/>
-        <v>8.519999999999972E-3</v>
+        <v>4.5199999999999685E-3</v>
       </c>
       <c r="F270" s="59">
         <v>0.87985000000000002</v>
       </c>
       <c r="G270" s="59">
-        <v>0.11162999999999999</v>
+        <v>0.11563</v>
       </c>
       <c r="H270" s="59">
         <f t="shared" si="7"/>
-        <v>8.519999999999972E-3</v>
+        <v>4.5199999999999685E-3</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.25">
@@ -58998,21 +58998,21 @@
         <v>0.87985000000000002</v>
       </c>
       <c r="D271" s="59">
-        <v>0.11162999999999999</v>
+        <v>0.11563</v>
       </c>
       <c r="E271" s="59">
         <f t="shared" si="6"/>
-        <v>8.519999999999972E-3</v>
+        <v>4.5199999999999685E-3</v>
       </c>
       <c r="F271" s="59">
         <v>0.87985000000000002</v>
       </c>
       <c r="G271" s="59">
-        <v>0.11162999999999999</v>
+        <v>0.11563</v>
       </c>
       <c r="H271" s="59">
         <f t="shared" si="7"/>
-        <v>8.519999999999972E-3</v>
+        <v>4.5199999999999685E-3</v>
       </c>
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.25">
@@ -59026,21 +59026,21 @@
         <v>0.87985000000000002</v>
       </c>
       <c r="D272" s="59">
-        <v>0.11162999999999999</v>
+        <v>0.11563</v>
       </c>
       <c r="E272" s="59">
         <f t="shared" si="6"/>
-        <v>8.519999999999972E-3</v>
+        <v>4.5199999999999685E-3</v>
       </c>
       <c r="F272" s="59">
         <v>0.87985000000000002</v>
       </c>
       <c r="G272" s="59">
-        <v>0.11162999999999999</v>
+        <v>0.11563</v>
       </c>
       <c r="H272" s="59">
         <f t="shared" si="7"/>
-        <v>8.519999999999972E-3</v>
+        <v>4.5199999999999685E-3</v>
       </c>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.25">
@@ -59054,21 +59054,21 @@
         <v>0.87985000000000002</v>
       </c>
       <c r="D273" s="59">
-        <v>0.11162999999999999</v>
+        <v>0.11563</v>
       </c>
       <c r="E273" s="59">
         <f t="shared" si="6"/>
-        <v>8.519999999999972E-3</v>
+        <v>4.5199999999999685E-3</v>
       </c>
       <c r="F273" s="59">
         <v>0.87985000000000002</v>
       </c>
       <c r="G273" s="59">
-        <v>0.11162999999999999</v>
+        <v>0.11563</v>
       </c>
       <c r="H273" s="59">
         <f t="shared" si="7"/>
-        <v>8.519999999999972E-3</v>
+        <v>4.5199999999999685E-3</v>
       </c>
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.25">
@@ -59082,21 +59082,21 @@
         <v>0.87985000000000002</v>
       </c>
       <c r="D274" s="59">
-        <v>0.11162999999999999</v>
+        <v>0.11563</v>
       </c>
       <c r="E274" s="59">
         <f t="shared" si="6"/>
-        <v>8.519999999999972E-3</v>
+        <v>4.5199999999999685E-3</v>
       </c>
       <c r="F274" s="59">
         <v>0.87985000000000002</v>
       </c>
       <c r="G274" s="59">
-        <v>0.11162999999999999</v>
+        <v>0.11563</v>
       </c>
       <c r="H274" s="59">
         <f t="shared" si="7"/>
-        <v>8.519999999999972E-3</v>
+        <v>4.5199999999999685E-3</v>
       </c>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
@@ -59284,8 +59284,8 @@
         <v>2.105747</v>
       </c>
       <c r="E284" s="87">
-        <f>19.478731 * 0.6</f>
-        <v>11.687238599999999</v>
+        <f>19.478731 * 0.57</f>
+        <v>11.102876669999999</v>
       </c>
       <c r="F284" s="7">
         <v>0.87036999999999998</v>
@@ -59294,8 +59294,8 @@
         <v>2.105747</v>
       </c>
       <c r="H284" s="87">
-        <f>19.478731 * 0.6</f>
-        <v>11.687238599999999</v>
+        <f>19.478731 * 0.57</f>
+        <v>11.102876669999999</v>
       </c>
     </row>
     <row r="285" spans="1:8" x14ac:dyDescent="0.25">
@@ -59309,8 +59309,8 @@
         <v>2.1315270000000002</v>
       </c>
       <c r="E285" s="87">
-        <f>19.514182 * 0.6</f>
-        <v>11.7085092</v>
+        <f>19.514182 * 0.52</f>
+        <v>10.147374640000001</v>
       </c>
       <c r="F285" s="7">
         <v>0.95</v>
@@ -59319,8 +59319,8 @@
         <v>2.1315270000000002</v>
       </c>
       <c r="H285" s="87">
-        <f>19.514182 * 0.6</f>
-        <v>11.7085092</v>
+        <f>19.514182 * 0.52</f>
+        <v>10.147374640000001</v>
       </c>
     </row>
     <row r="286" spans="1:8" x14ac:dyDescent="0.25">
@@ -59379,7 +59379,7 @@
         <v>0.93038500000000002</v>
       </c>
       <c r="D288" s="7">
-        <v>2.1220140000000001</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="E288" s="87">
         <f xml:space="preserve"> 24.516099 * 0.3</f>
@@ -59389,7 +59389,7 @@
         <v>0.93038500000000002</v>
       </c>
       <c r="G288" s="7">
-        <v>2.1220140000000001</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="H288" s="87">
         <f xml:space="preserve"> 24.516099 * 0.3</f>
@@ -59404,7 +59404,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="D289" s="7">
-        <v>2.1227469999999999</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="E289" s="7">
         <v>7.0254260000000004</v>
@@ -59413,7 +59413,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="G289" s="7">
-        <v>2.1227469999999999</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="H289" s="7">
         <v>7.0254260000000004</v>
@@ -59427,7 +59427,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="D290" s="7">
-        <v>2.1227469999999999</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="E290" s="7">
         <v>1</v>
@@ -59436,7 +59436,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="G290" s="7">
-        <v>2.1227469999999999</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="H290" s="7">
         <v>1</v>
@@ -59450,7 +59450,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="D291" s="7">
-        <v>2.1227469999999999</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="E291" s="7">
         <v>1</v>
@@ -59459,7 +59459,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="G291" s="7">
-        <v>2.1227469999999999</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="H291" s="7">
         <v>1</v>
@@ -59473,7 +59473,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="D292" s="7">
-        <v>2.1227469999999999</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="E292" s="7">
         <v>1</v>
@@ -59482,7 +59482,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="G292" s="7">
-        <v>2.1227469999999999</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="H292" s="7">
         <v>1</v>
@@ -59496,7 +59496,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="D293" s="7">
-        <v>2.1227469999999999</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="E293" s="7">
         <v>1</v>
@@ -59505,7 +59505,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="G293" s="7">
-        <v>2.1227469999999999</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="H293" s="7">
         <v>1</v>
@@ -59519,7 +59519,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="D294" s="7">
-        <v>2.1227469999999999</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="E294" s="7">
         <v>1</v>
@@ -59528,7 +59528,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="G294" s="7">
-        <v>2.1227469999999999</v>
+        <v>2.0623269999999998</v>
       </c>
       <c r="H294" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
Reduce HIV transmission prob
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Kenya_model_HPV-HIVacq\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293019DF-7BD5-44EF-AD6D-A77F9CF62FB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCA0D68-290D-4E64-AF36-4D1B3211C1F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9345" windowHeight="12195" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53467,8 +53467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
-      <selection activeCell="I275" sqref="I275"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="H283" sqref="H283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58771,24 +58771,24 @@
         <v>138</v>
       </c>
       <c r="C263" s="59">
-        <v>0.55502700000000005</v>
+        <v>0.59502699999999997</v>
       </c>
       <c r="D263" s="59">
-        <v>0.416599</v>
+        <v>0.37659900000000002</v>
       </c>
       <c r="E263" s="59">
         <f t="shared" ref="E263:E274" si="6">1-(C263+D263)</f>
-        <v>2.8373999999999899E-2</v>
+        <v>2.837400000000001E-2</v>
       </c>
       <c r="F263" s="59">
-        <v>0.54402700000000004</v>
+        <v>0.56402699999999995</v>
       </c>
       <c r="G263" s="59">
-        <v>0.44359900000000002</v>
+        <v>0.423599</v>
       </c>
       <c r="H263" s="59">
         <f t="shared" ref="H263:H274" si="7">1-(F263+G263)</f>
-        <v>1.2373999999999885E-2</v>
+        <v>1.2374000000000107E-2</v>
       </c>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.25">
@@ -58799,20 +58799,20 @@
         <v>139</v>
       </c>
       <c r="C264" s="59">
-        <v>0.58545599999999998</v>
+        <v>0.63545600000000002</v>
       </c>
       <c r="D264" s="59">
-        <v>0.40419699999999997</v>
+        <v>0.35419699999999998</v>
       </c>
       <c r="E264" s="59">
         <f t="shared" si="6"/>
-        <v>1.0347000000000106E-2</v>
+        <v>1.0346999999999995E-2</v>
       </c>
       <c r="F264" s="59">
-        <v>0.57145599999999996</v>
+        <v>0.611456</v>
       </c>
       <c r="G264" s="59">
-        <v>0.40519699999999997</v>
+        <v>0.36519699999999999</v>
       </c>
       <c r="H264" s="59">
         <f t="shared" si="7"/>
@@ -58827,20 +58827,20 @@
         <v>140</v>
       </c>
       <c r="C265" s="59">
-        <v>0.65932100000000005</v>
+        <v>0.68932099999999996</v>
       </c>
       <c r="D265" s="59">
-        <v>0.33078000000000002</v>
+        <v>0.30077999999999999</v>
       </c>
       <c r="E265" s="59">
         <f t="shared" si="6"/>
-        <v>9.8989999999998801E-3</v>
+        <v>9.8990000000001022E-3</v>
       </c>
       <c r="F265" s="59">
-        <v>0.64532100000000003</v>
+        <v>0.65532100000000004</v>
       </c>
       <c r="G265" s="59">
-        <v>0.34058680000000002</v>
+        <v>0.33058680000000001</v>
       </c>
       <c r="H265" s="59">
         <f t="shared" si="7"/>
@@ -59247,7 +59247,7 @@
         <v>2.1546289999999999</v>
       </c>
       <c r="H282" s="7">
-        <v>6.4129969999999998</v>
+        <v>5.4129969999999998</v>
       </c>
     </row>
     <row r="283" spans="1:8" x14ac:dyDescent="0.25">
@@ -59258,7 +59258,7 @@
         <v>0.87400100000000003</v>
       </c>
       <c r="D283" s="7">
-        <v>2.173962</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="E283" s="7">
         <v>7.7805770000000001</v>
@@ -59281,7 +59281,7 @@
         <v>0.87036999999999998</v>
       </c>
       <c r="D284" s="7">
-        <v>2.105747</v>
+        <v>2.13</v>
       </c>
       <c r="E284" s="87">
         <f>19.478731 * 0.57</f>
@@ -59291,7 +59291,7 @@
         <v>0.87036999999999998</v>
       </c>
       <c r="G284" s="7">
-        <v>2.105747</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="H284" s="87">
         <f>19.478731 * 0.57</f>
@@ -59306,7 +59306,7 @@
         <v>0.95</v>
       </c>
       <c r="D285" s="7">
-        <v>2.1315270000000002</v>
+        <v>2.11</v>
       </c>
       <c r="E285" s="87">
         <f>19.514182 * 0.52</f>
@@ -59331,7 +59331,7 @@
         <v>0.93322700000000003</v>
       </c>
       <c r="D286" s="7">
-        <v>2.181549</v>
+        <v>2.08</v>
       </c>
       <c r="E286" s="7">
         <v>9.6671910000000008</v>
@@ -59340,7 +59340,7 @@
         <v>0.93322700000000003</v>
       </c>
       <c r="G286" s="7">
-        <v>2.181549</v>
+        <v>2.11</v>
       </c>
       <c r="H286" s="7">
         <v>9.6671910000000008</v>

</xml_diff>

<commit_message>
reduce % in high risk group
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Kenya_model_HPV-HIVacq\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCA0D68-290D-4E64-AF36-4D1B3211C1F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADE0460-AD27-48BD-BDBC-88932FEE6792}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9345" windowHeight="12195" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9345" windowHeight="9495" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="10" r:id="rId1"/>
@@ -53467,8 +53467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="H283" sqref="H283"/>
+    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="G287" sqref="G287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59238,7 +59238,7 @@
         <v>2.1546289999999999</v>
       </c>
       <c r="E282" s="7">
-        <v>6.4129969999999998</v>
+        <v>6.112997</v>
       </c>
       <c r="F282" s="7">
         <v>0.22517599999999999</v>
@@ -59255,22 +59255,22 @@
         <v>138</v>
       </c>
       <c r="C283" s="7">
-        <v>0.87400100000000003</v>
+        <v>0.85400100000000001</v>
       </c>
       <c r="D283" s="7">
-        <v>2.1800000000000002</v>
+        <v>2.15</v>
       </c>
       <c r="E283" s="7">
-        <v>7.7805770000000001</v>
+        <v>10.080577</v>
       </c>
       <c r="F283" s="7">
-        <v>0.87400100000000003</v>
+        <v>0.85400100000000001</v>
       </c>
       <c r="G283" s="7">
-        <v>2.173962</v>
+        <v>2.1539619999999999</v>
       </c>
       <c r="H283" s="7">
-        <v>7.7805770000000001</v>
+        <v>7.0805769999999999</v>
       </c>
     </row>
     <row r="284" spans="1:8" x14ac:dyDescent="0.25">
@@ -59284,18 +59284,18 @@
         <v>2.13</v>
       </c>
       <c r="E284" s="87">
-        <f>19.478731 * 0.57</f>
-        <v>11.102876669999999</v>
+        <f>19.478731 * 0.51</f>
+        <v>9.9341528100000005</v>
       </c>
       <c r="F284" s="7">
         <v>0.87036999999999998</v>
       </c>
       <c r="G284" s="7">
-        <v>2.1800000000000002</v>
+        <v>2.13</v>
       </c>
       <c r="H284" s="87">
-        <f>19.478731 * 0.57</f>
-        <v>11.102876669999999</v>
+        <f>19.478731 * 0.52</f>
+        <v>10.128940120000001</v>
       </c>
     </row>
     <row r="285" spans="1:8" x14ac:dyDescent="0.25">
@@ -59303,24 +59303,24 @@
         <v>140</v>
       </c>
       <c r="C285" s="7">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="D285" s="7">
         <v>2.11</v>
       </c>
       <c r="E285" s="87">
-        <f>19.514182 * 0.52</f>
-        <v>10.147374640000001</v>
+        <f>19.514182 * 0.5</f>
+        <v>9.7570910000000008</v>
       </c>
       <c r="F285" s="7">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="G285" s="7">
-        <v>2.1315270000000002</v>
+        <v>2.1115270000000002</v>
       </c>
       <c r="H285" s="87">
-        <f>19.514182 * 0.52</f>
-        <v>10.147374640000001</v>
+        <f>19.514182 * 0.5</f>
+        <v>9.7570910000000008</v>
       </c>
     </row>
     <row r="286" spans="1:8" x14ac:dyDescent="0.25">
@@ -59340,7 +59340,7 @@
         <v>0.93322700000000003</v>
       </c>
       <c r="G286" s="7">
-        <v>2.11</v>
+        <v>2.08</v>
       </c>
       <c r="H286" s="7">
         <v>9.6671910000000008</v>

</xml_diff>

<commit_message>
increease HPV transmission prob
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Kenya_model_HPV-HIVacq\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FC6F01-F33C-48E3-940B-27EF537D5E81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735EFE5E-96A1-4EEA-B8A7-317771CABB4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9345" windowHeight="9495" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3264" uniqueCount="1350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3263" uniqueCount="1349">
   <si>
     <t>Metric</t>
   </si>
@@ -4087,9 +4087,6 @@
   </si>
   <si>
     <t>60–64</t>
-  </si>
-  <si>
-    <t>=</t>
   </si>
   <si>
     <t>*HIV clinic</t>
@@ -4829,7 +4826,7 @@
     <xf numFmtId="0" fontId="1" fillId="36" borderId="8" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4952,6 +4949,7 @@
     <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -53471,8 +53469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="G287" sqref="G287"/>
+    <sheetView tabSelected="1" topLeftCell="B165" workbookViewId="0">
+      <selection activeCell="H190" sqref="H190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57170,6 +57168,9 @@
         <f t="shared" ref="F171:F183" si="2">0.8*O171</f>
         <v>4.4927999999999999</v>
       </c>
+      <c r="G171" s="90"/>
+      <c r="H171" s="90"/>
+      <c r="I171" s="90"/>
       <c r="J171" s="37" t="s">
         <v>311</v>
       </c>
@@ -57204,9 +57205,12 @@
         <v>29.951999999999998</v>
       </c>
       <c r="F172" s="75">
-        <f t="shared" si="2"/>
-        <v>17.9712</v>
-      </c>
+        <f>0.9*O172</f>
+        <v>20.217600000000001</v>
+      </c>
+      <c r="G172" s="90"/>
+      <c r="H172" s="90"/>
+      <c r="I172" s="90"/>
       <c r="J172" s="37" t="s">
         <v>602</v>
       </c>
@@ -57869,16 +57873,16 @@
         <v>0.1</v>
       </c>
       <c r="D191" s="75">
-        <f t="shared" ref="D191:D203" si="3">0.8*M191</f>
-        <v>12.48</v>
+        <f>M191</f>
+        <v>15.6</v>
       </c>
       <c r="E191" s="75">
-        <f t="shared" ref="E191:E203" si="4">0.8*N191</f>
-        <v>7.4879999999999995</v>
+        <f>N191</f>
+        <v>9.36</v>
       </c>
       <c r="F191" s="75">
-        <f t="shared" ref="F191:F203" si="5">0.8*O191</f>
-        <v>4.4927999999999999</v>
+        <f>O191</f>
+        <v>5.6159999999999997</v>
       </c>
       <c r="G191" s="72"/>
       <c r="H191" s="72"/>
@@ -57911,16 +57915,16 @@
         <v>0.4</v>
       </c>
       <c r="D192" s="75">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D191:D203" si="3">0.8*M192</f>
         <v>49.92</v>
       </c>
       <c r="E192" s="75">
-        <f t="shared" si="4"/>
-        <v>29.951999999999998</v>
+        <f>0.9*N192</f>
+        <v>33.695999999999998</v>
       </c>
       <c r="F192" s="75">
-        <f t="shared" si="5"/>
-        <v>17.9712</v>
+        <f>0.9*O192</f>
+        <v>20.217600000000001</v>
       </c>
       <c r="G192" s="72"/>
       <c r="H192" s="72"/>
@@ -57957,11 +57961,11 @@
         <v>124.80000000000001</v>
       </c>
       <c r="E193" s="75">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="E191:E203" si="4">0.8*N193</f>
         <v>74.88</v>
       </c>
       <c r="F193" s="75">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="F191:F203" si="5">0.8*O193</f>
         <v>44.927999999999997</v>
       </c>
       <c r="G193" s="72"/>
@@ -58007,9 +58011,7 @@
         <v>31.768893464000001</v>
       </c>
       <c r="G194" s="72"/>
-      <c r="H194" s="72" t="s">
-        <v>1345</v>
-      </c>
+      <c r="H194" s="72"/>
       <c r="I194" s="72"/>
       <c r="J194" s="72" t="s">
         <v>314</v>
@@ -58618,7 +58620,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.25">
@@ -58970,7 +58972,7 @@
       <c r="B270" s="37" t="s">
         <v>461</v>
       </c>
-      <c r="C270" s="91">
+      <c r="C270" s="92">
         <v>0.88085000000000002</v>
       </c>
       <c r="D270" s="59">
@@ -58980,7 +58982,7 @@
         <f t="shared" si="6"/>
         <v>3.5199999999999676E-3</v>
       </c>
-      <c r="F270" s="91">
+      <c r="F270" s="92">
         <v>0.88085000000000002</v>
       </c>
       <c r="G270" s="59">
@@ -58998,7 +59000,7 @@
       <c r="B271" s="37" t="s">
         <v>324</v>
       </c>
-      <c r="C271" s="91">
+      <c r="C271" s="92">
         <v>0.88085000000000002</v>
       </c>
       <c r="D271" s="59">
@@ -59008,7 +59010,7 @@
         <f t="shared" si="6"/>
         <v>3.5199999999999676E-3</v>
       </c>
-      <c r="F271" s="91">
+      <c r="F271" s="92">
         <v>0.88085000000000002</v>
       </c>
       <c r="G271" s="59">
@@ -59026,7 +59028,7 @@
       <c r="B272" s="37" t="s">
         <v>462</v>
       </c>
-      <c r="C272" s="91">
+      <c r="C272" s="92">
         <v>0.88085000000000002</v>
       </c>
       <c r="D272" s="59">
@@ -59036,7 +59038,7 @@
         <f t="shared" si="6"/>
         <v>3.5199999999999676E-3</v>
       </c>
-      <c r="F272" s="91">
+      <c r="F272" s="92">
         <v>0.88085000000000002</v>
       </c>
       <c r="G272" s="59">
@@ -59054,7 +59056,7 @@
       <c r="B273" s="37" t="s">
         <v>463</v>
       </c>
-      <c r="C273" s="91">
+      <c r="C273" s="92">
         <v>0.88085000000000002</v>
       </c>
       <c r="D273" s="59">
@@ -59064,7 +59066,7 @@
         <f t="shared" si="6"/>
         <v>3.5199999999999676E-3</v>
       </c>
-      <c r="F273" s="91">
+      <c r="F273" s="92">
         <v>0.88085000000000002</v>
       </c>
       <c r="G273" s="59">
@@ -59082,7 +59084,7 @@
       <c r="B274" s="37" t="s">
         <v>464</v>
       </c>
-      <c r="C274" s="91">
+      <c r="C274" s="92">
         <v>0.88085000000000002</v>
       </c>
       <c r="D274" s="59">
@@ -59092,7 +59094,7 @@
         <f t="shared" si="6"/>
         <v>3.5199999999999676E-3</v>
       </c>
-      <c r="F274" s="91">
+      <c r="F274" s="92">
         <v>0.88085000000000002</v>
       </c>
       <c r="G274" s="59">
@@ -59114,7 +59116,7 @@
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="B276" s="37"/>
       <c r="C276" s="37"/>
@@ -59169,7 +59171,7 @@
       <c r="C279" s="88">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D279" s="90">
+      <c r="D279" s="91">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E279" s="7">
@@ -59192,7 +59194,7 @@
       <c r="C280" s="88">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D280" s="90">
+      <c r="D280" s="91">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E280" s="7">
@@ -59215,7 +59217,7 @@
       <c r="C281" s="89">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="D281" s="90">
+      <c r="D281" s="91">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E281" s="7">
@@ -59238,8 +59240,8 @@
       <c r="C282" s="88">
         <v>0.22517599999999999</v>
       </c>
-      <c r="D282" s="90">
-        <v>2.1546289999999999</v>
+      <c r="D282" s="91">
+        <v>2.4546290000000002</v>
       </c>
       <c r="E282" s="7">
         <v>6.4129969999999998</v>
@@ -59247,8 +59249,8 @@
       <c r="F282" s="7">
         <v>0.22517599999999999</v>
       </c>
-      <c r="G282" s="7">
-        <v>2.1546289999999999</v>
+      <c r="G282" s="91">
+        <v>2.4546290000000002</v>
       </c>
       <c r="H282" s="7">
         <v>5.4129969999999998</v>
@@ -59261,8 +59263,8 @@
       <c r="C283" s="88">
         <v>0.87400100000000003</v>
       </c>
-      <c r="D283" s="90">
-        <v>2.38</v>
+      <c r="D283" s="91">
+        <v>2.58</v>
       </c>
       <c r="E283" s="7">
         <v>11.080577</v>
@@ -59270,11 +59272,11 @@
       <c r="F283" s="7">
         <v>0.87400100000000003</v>
       </c>
-      <c r="G283" s="7">
-        <v>2.3839619999999999</v>
+      <c r="G283" s="91">
+        <v>2.58</v>
       </c>
       <c r="H283" s="7">
-        <v>8.7805769999999992</v>
+        <v>9.7805769999999992</v>
       </c>
     </row>
     <row r="284" spans="1:8" x14ac:dyDescent="0.25">
@@ -59284,8 +59286,8 @@
       <c r="C284" s="88">
         <v>0.87036999999999998</v>
       </c>
-      <c r="D284" s="90">
-        <v>2.23</v>
+      <c r="D284" s="91">
+        <v>2.33</v>
       </c>
       <c r="E284" s="87">
         <v>10.15</v>
@@ -59294,7 +59296,7 @@
         <v>0.87036999999999998</v>
       </c>
       <c r="G284" s="7">
-        <v>2.23</v>
+        <v>2.33</v>
       </c>
       <c r="H284" s="87">
         <f>19.478731 * 0.57</f>
@@ -59308,7 +59310,7 @@
       <c r="C285" s="88">
         <v>0.95</v>
       </c>
-      <c r="D285" s="90">
+      <c r="D285" s="91">
         <v>2.11</v>
       </c>
       <c r="E285" s="87">
@@ -59333,7 +59335,7 @@
       <c r="C286" s="88">
         <v>0.93322700000000003</v>
       </c>
-      <c r="D286" s="90">
+      <c r="D286" s="91">
         <v>2.08</v>
       </c>
       <c r="E286" s="7">
@@ -59356,7 +59358,7 @@
       <c r="C287" s="88">
         <v>0.93</v>
       </c>
-      <c r="D287" s="90">
+      <c r="D287" s="91">
         <v>2.0623269999999998</v>
       </c>
       <c r="E287" s="87">
@@ -59381,7 +59383,7 @@
       <c r="C288" s="88">
         <v>0.93038500000000002</v>
       </c>
-      <c r="D288" s="90">
+      <c r="D288" s="91">
         <v>2.0623269999999998</v>
       </c>
       <c r="E288" s="87">
@@ -59406,7 +59408,7 @@
       <c r="C289" s="88">
         <v>0.91735900000000004</v>
       </c>
-      <c r="D289" s="90">
+      <c r="D289" s="91">
         <v>2.0623269999999998</v>
       </c>
       <c r="E289" s="7">
@@ -59429,7 +59431,7 @@
       <c r="C290" s="88">
         <v>0.91735900000000004</v>
       </c>
-      <c r="D290" s="90">
+      <c r="D290" s="91">
         <v>2.0623269999999998</v>
       </c>
       <c r="E290" s="7">
@@ -59452,7 +59454,7 @@
       <c r="C291" s="88">
         <v>0.91735900000000004</v>
       </c>
-      <c r="D291" s="90">
+      <c r="D291" s="91">
         <v>2.0623269999999998</v>
       </c>
       <c r="E291" s="7">
@@ -59475,7 +59477,7 @@
       <c r="C292" s="88">
         <v>0.91735900000000004</v>
       </c>
-      <c r="D292" s="90">
+      <c r="D292" s="91">
         <v>2.0623269999999998</v>
       </c>
       <c r="E292" s="7">
@@ -59498,7 +59500,7 @@
       <c r="C293" s="88">
         <v>0.91735900000000004</v>
       </c>
-      <c r="D293" s="90">
+      <c r="D293" s="91">
         <v>2.0623269999999998</v>
       </c>
       <c r="E293" s="7">
@@ -59521,7 +59523,7 @@
       <c r="C294" s="88">
         <v>0.91735900000000004</v>
       </c>
-      <c r="D294" s="90">
+      <c r="D294" s="91">
         <v>2.0623269999999998</v>
       </c>
       <c r="E294" s="7">
@@ -70252,7 +70254,7 @@
         <v>106</v>
       </c>
       <c r="H71" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -70866,7 +70868,7 @@
         <v>1</v>
       </c>
       <c r="H130" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
reduced riskAdj and partners in older ages
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -53496,8 +53496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
-      <selection activeCell="D282" sqref="D282"/>
+    <sheetView tabSelected="1" topLeftCell="A269" workbookViewId="0">
+      <selection activeCell="G291" sqref="G291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58870,14 +58870,14 @@
         <v>9.8990000000001022E-3</v>
       </c>
       <c r="F265" s="59">
-        <v>0.65532100000000004</v>
+        <v>0.65632100000000004</v>
       </c>
       <c r="G265" s="59">
         <v>0.33058680000000001</v>
       </c>
       <c r="H265" s="59">
         <f t="shared" si="7"/>
-        <v>1.4092199999999888E-2</v>
+        <v>1.3092199999999998E-2</v>
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.25">
@@ -58898,14 +58898,14 @@
         <v>7.0239999999999192E-3</v>
       </c>
       <c r="F266" s="59">
-        <v>0.71510499999999999</v>
+        <v>0.71710499999999999</v>
       </c>
       <c r="G266" s="59">
         <v>0.27507100000000001</v>
       </c>
       <c r="H266" s="59">
         <f t="shared" si="7"/>
-        <v>9.8240000000000549E-3</v>
+        <v>7.8240000000000531E-3</v>
       </c>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.25">
@@ -58926,14 +58926,14 @@
         <v>5.4269999999999596E-3</v>
       </c>
       <c r="F267" s="59">
-        <v>0.73122299999999996</v>
+        <v>0.73212299999999997</v>
       </c>
       <c r="G267" s="59">
         <v>0.26235000000000003</v>
       </c>
       <c r="H267" s="59">
         <f t="shared" si="7"/>
-        <v>6.4269999999999605E-3</v>
+        <v>5.5270000000000596E-3</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
@@ -58954,14 +58954,14 @@
         <v>4.6000000000000485E-3</v>
       </c>
       <c r="F268" s="59">
-        <v>0.80640999999999996</v>
+        <v>0.80681000000000003</v>
       </c>
       <c r="G268" s="59">
         <v>0.18798999999999999</v>
       </c>
       <c r="H268" s="59">
         <f t="shared" si="7"/>
-        <v>5.6000000000000494E-3</v>
+        <v>5.1999999999999824E-3</v>
       </c>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.25">
@@ -58972,20 +58972,20 @@
         <v>392</v>
       </c>
       <c r="C269" s="59">
-        <v>0.88085000000000002</v>
+        <v>0.89085000000000003</v>
       </c>
       <c r="D269" s="59">
-        <v>0.11563</v>
+        <v>0.10563</v>
       </c>
       <c r="E269" s="59">
         <f t="shared" si="6"/>
         <v>3.5199999999999676E-3</v>
       </c>
       <c r="F269" s="59">
-        <v>0.88085000000000002</v>
+        <v>0.89085000000000003</v>
       </c>
       <c r="G269" s="59">
-        <v>0.11563</v>
+        <v>0.10563</v>
       </c>
       <c r="H269" s="59">
         <f t="shared" si="7"/>
@@ -59000,20 +59000,20 @@
         <v>461</v>
       </c>
       <c r="C270" s="91">
-        <v>0.88085000000000002</v>
-      </c>
-      <c r="D270" s="59">
-        <v>0.11563</v>
+        <v>0.89085000000000003</v>
+      </c>
+      <c r="D270" s="91">
+        <v>0.10563</v>
       </c>
       <c r="E270" s="59">
         <f t="shared" si="6"/>
         <v>3.5199999999999676E-3</v>
       </c>
       <c r="F270" s="91">
-        <v>0.88085000000000002</v>
-      </c>
-      <c r="G270" s="59">
-        <v>0.11563</v>
+        <v>0.89085000000000003</v>
+      </c>
+      <c r="G270" s="91">
+        <v>0.10563</v>
       </c>
       <c r="H270" s="59">
         <f t="shared" si="7"/>
@@ -59028,20 +59028,20 @@
         <v>324</v>
       </c>
       <c r="C271" s="91">
-        <v>0.88085000000000002</v>
-      </c>
-      <c r="D271" s="59">
-        <v>0.11563</v>
+        <v>0.89085000000000003</v>
+      </c>
+      <c r="D271" s="91">
+        <v>0.10563</v>
       </c>
       <c r="E271" s="59">
         <f t="shared" si="6"/>
         <v>3.5199999999999676E-3</v>
       </c>
       <c r="F271" s="91">
-        <v>0.88085000000000002</v>
-      </c>
-      <c r="G271" s="59">
-        <v>0.11563</v>
+        <v>0.89085000000000003</v>
+      </c>
+      <c r="G271" s="91">
+        <v>0.10563</v>
       </c>
       <c r="H271" s="59">
         <f t="shared" si="7"/>
@@ -59056,20 +59056,20 @@
         <v>462</v>
       </c>
       <c r="C272" s="91">
-        <v>0.88085000000000002</v>
-      </c>
-      <c r="D272" s="59">
-        <v>0.11563</v>
+        <v>0.89085000000000003</v>
+      </c>
+      <c r="D272" s="91">
+        <v>0.10563</v>
       </c>
       <c r="E272" s="59">
         <f t="shared" si="6"/>
         <v>3.5199999999999676E-3</v>
       </c>
       <c r="F272" s="91">
-        <v>0.88085000000000002</v>
-      </c>
-      <c r="G272" s="59">
-        <v>0.11563</v>
+        <v>0.89085000000000003</v>
+      </c>
+      <c r="G272" s="91">
+        <v>0.10563</v>
       </c>
       <c r="H272" s="59">
         <f t="shared" si="7"/>
@@ -59084,20 +59084,20 @@
         <v>463</v>
       </c>
       <c r="C273" s="91">
-        <v>0.88085000000000002</v>
-      </c>
-      <c r="D273" s="59">
-        <v>0.11563</v>
+        <v>0.89085000000000003</v>
+      </c>
+      <c r="D273" s="91">
+        <v>0.10563</v>
       </c>
       <c r="E273" s="59">
         <f t="shared" si="6"/>
         <v>3.5199999999999676E-3</v>
       </c>
       <c r="F273" s="91">
-        <v>0.88085000000000002</v>
-      </c>
-      <c r="G273" s="59">
-        <v>0.11563</v>
+        <v>0.89085000000000003</v>
+      </c>
+      <c r="G273" s="91">
+        <v>0.10563</v>
       </c>
       <c r="H273" s="59">
         <f t="shared" si="7"/>
@@ -59112,20 +59112,20 @@
         <v>464</v>
       </c>
       <c r="C274" s="91">
-        <v>0.88085000000000002</v>
-      </c>
-      <c r="D274" s="59">
-        <v>0.11563</v>
+        <v>0.89085000000000003</v>
+      </c>
+      <c r="D274" s="91">
+        <v>0.10563</v>
       </c>
       <c r="E274" s="59">
         <f t="shared" si="6"/>
         <v>3.5199999999999676E-3</v>
       </c>
       <c r="F274" s="91">
-        <v>0.88085000000000002</v>
-      </c>
-      <c r="G274" s="59">
-        <v>0.11563</v>
+        <v>0.89085000000000003</v>
+      </c>
+      <c r="G274" s="91">
+        <v>0.10563</v>
       </c>
       <c r="H274" s="59">
         <f t="shared" si="7"/>
@@ -59411,7 +59411,7 @@
         <v>0.93038500000000002</v>
       </c>
       <c r="D288" s="90">
-        <v>2.0623269999999998</v>
+        <v>2</v>
       </c>
       <c r="E288" s="86">
         <f xml:space="preserve"> 24.516099 * 0.3</f>
@@ -59421,7 +59421,7 @@
         <v>0.93038500000000002</v>
       </c>
       <c r="G288" s="7">
-        <v>2.0623269999999998</v>
+        <v>2</v>
       </c>
       <c r="H288" s="86">
         <f xml:space="preserve"> 24.516099 * 0.3</f>
@@ -59436,7 +59436,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="D289" s="90">
-        <v>2.0623269999999998</v>
+        <v>1.9</v>
       </c>
       <c r="E289" s="7">
         <v>7.0254260000000004</v>
@@ -59445,7 +59445,7 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="G289" s="7">
-        <v>2.0623269999999998</v>
+        <v>1.9</v>
       </c>
       <c r="H289" s="7">
         <v>7.0254260000000004</v>
@@ -59459,19 +59459,19 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="D290" s="90">
-        <v>2.0623269999999998</v>
+        <v>1.85</v>
       </c>
       <c r="E290" s="7">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="F290" s="7">
         <v>0.91735900000000004</v>
       </c>
-      <c r="G290" s="7">
-        <v>2.0623269999999998</v>
+      <c r="G290" s="90">
+        <v>1.85</v>
       </c>
       <c r="H290" s="7">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="291" spans="2:8" x14ac:dyDescent="0.25">
@@ -59482,19 +59482,19 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="D291" s="90">
-        <v>2.0623269999999998</v>
-      </c>
-      <c r="E291" s="7">
-        <v>3</v>
+        <v>1.8</v>
+      </c>
+      <c r="E291" s="90">
+        <v>2.5</v>
       </c>
       <c r="F291" s="7">
         <v>0.91735900000000004</v>
       </c>
-      <c r="G291" s="7">
-        <v>2.0623269999999998</v>
-      </c>
-      <c r="H291" s="7">
-        <v>3</v>
+      <c r="G291" s="90">
+        <v>1.8</v>
+      </c>
+      <c r="H291" s="90">
+        <v>2.5</v>
       </c>
     </row>
     <row r="292" spans="2:8" x14ac:dyDescent="0.25">
@@ -59505,19 +59505,19 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="D292" s="90">
-        <v>2.0623269999999998</v>
-      </c>
-      <c r="E292" s="7">
-        <v>3</v>
+        <v>1.8</v>
+      </c>
+      <c r="E292" s="90">
+        <v>2.5</v>
       </c>
       <c r="F292" s="7">
         <v>0.91735900000000004</v>
       </c>
-      <c r="G292" s="7">
-        <v>2.0623269999999998</v>
-      </c>
-      <c r="H292" s="7">
-        <v>3</v>
+      <c r="G292" s="90">
+        <v>1.8</v>
+      </c>
+      <c r="H292" s="90">
+        <v>2.5</v>
       </c>
     </row>
     <row r="293" spans="2:8" x14ac:dyDescent="0.25">
@@ -59528,19 +59528,19 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="D293" s="90">
-        <v>2.0623269999999998</v>
-      </c>
-      <c r="E293" s="7">
-        <v>3</v>
+        <v>1.8</v>
+      </c>
+      <c r="E293" s="90">
+        <v>2.5</v>
       </c>
       <c r="F293" s="7">
         <v>0.91735900000000004</v>
       </c>
-      <c r="G293" s="7">
-        <v>2.0623269999999998</v>
-      </c>
-      <c r="H293" s="7">
-        <v>3</v>
+      <c r="G293" s="90">
+        <v>1.8</v>
+      </c>
+      <c r="H293" s="90">
+        <v>2.5</v>
       </c>
     </row>
     <row r="294" spans="2:8" x14ac:dyDescent="0.25">
@@ -59551,19 +59551,19 @@
         <v>0.91735900000000004</v>
       </c>
       <c r="D294" s="90">
-        <v>2.0623269999999998</v>
-      </c>
-      <c r="E294" s="7">
-        <v>3</v>
+        <v>1.8</v>
+      </c>
+      <c r="E294" s="90">
+        <v>2.5</v>
       </c>
       <c r="F294" s="7">
         <v>0.91735900000000004</v>
       </c>
-      <c r="G294" s="7">
-        <v>2.0623269999999998</v>
-      </c>
-      <c r="H294" s="7">
-        <v>3</v>
+      <c r="G294" s="90">
+        <v>1.8</v>
+      </c>
+      <c r="H294" s="90">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add comments to script
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters_Feb20.xlsx
+++ b/Config/Kenya_parameters_Feb20.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20363"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Kenya_model_Feb20\HHCoM\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\udrive.uw.edu\udrive\Kenya_model_Feb20\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDF8645-CC3A-4C46-BEF4-79D132674587}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="4770" tabRatio="835" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9090" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="10" r:id="rId1"/>
@@ -21,15 +22,17 @@
     <sheet name="CIN prevalence" sheetId="15" r:id="rId7"/>
     <sheet name="Screening" sheetId="2" r:id="rId8"/>
     <sheet name="CC prevalence" sheetId="3" r:id="rId9"/>
-    <sheet name="HIV prevalence" sheetId="11" r:id="rId10"/>
-    <sheet name="HIV mortality" sheetId="16" r:id="rId11"/>
-    <sheet name="HIV testing " sheetId="6" r:id="rId12"/>
-    <sheet name="ART" sheetId="12" r:id="rId13"/>
-    <sheet name="CD4" sheetId="13" r:id="rId14"/>
-    <sheet name="MTCT" sheetId="14" r:id="rId15"/>
-    <sheet name="DALY" sheetId="1" r:id="rId16"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId10"/>
+    <sheet name="HIV prevalence" sheetId="11" r:id="rId11"/>
+    <sheet name="HIV mortality" sheetId="16" r:id="rId12"/>
+    <sheet name="HIV testing " sheetId="6" r:id="rId13"/>
+    <sheet name="ART" sheetId="12" r:id="rId14"/>
+    <sheet name="CD4" sheetId="13" r:id="rId15"/>
+    <sheet name="MTCT" sheetId="14" r:id="rId16"/>
+    <sheet name="DALY" sheetId="1" r:id="rId17"/>
+    <sheet name="Param bounds" sheetId="18" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3226" uniqueCount="1351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3249" uniqueCount="1372">
   <si>
     <t>Metric</t>
   </si>
@@ -3467,9 +3470,6 @@
     <t>%virally suppresion among all PLHIV</t>
   </si>
   <si>
-    <t xml:space="preserve">Source: </t>
-  </si>
-  <si>
     <t>Source: population_validation_targets_kenya.xlsx</t>
   </si>
   <si>
@@ -4104,12 +4104,78 @@
   </si>
   <si>
     <t>Globocan 2012</t>
+  </si>
+  <si>
+    <t>Eldoret, 2012-2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Params for calibration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UB </t>
+  </si>
+  <si>
+    <t>ParamsAll num</t>
+  </si>
+  <si>
+    <t>partnersM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sources for bounds </t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-14, high risk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-19, high risk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20-24, high risk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-29, high risk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30-44, high risk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">45+, high risk </t>
+  </si>
+  <si>
+    <t>partnersF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: DHS 2014 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condom use </t>
+  </si>
+  <si>
+    <t>LCL</t>
+  </si>
+  <si>
+    <t>UCL</t>
+  </si>
+  <si>
+    <t>condUse</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DHS 2014; based on self-reported condom use at all sex acts with the most recent sex partner in the past 12 months. LB = LCL of estimates from women, UB = UCL of estimates from men </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="12">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
@@ -4768,7 +4834,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -4830,8 +4896,9 @@
     <xf numFmtId="0" fontId="1" fillId="35" borderId="8" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="8" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="8" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4946,11 +5013,13 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="54" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="56">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -4977,13 +5046,14 @@
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="CC" xfId="55" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Comma" xfId="54" builtinId="3"/>
-    <cellStyle name="Data" xfId="46"/>
-    <cellStyle name="Data 2" xfId="48"/>
+    <cellStyle name="Data" xfId="46" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Data 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Header" xfId="45"/>
+    <cellStyle name="Header" xfId="45" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
@@ -4993,17 +5063,17 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="43"/>
-    <cellStyle name="Normal 2 2" xfId="47"/>
+    <cellStyle name="Normal 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 2 2" xfId="47" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Note 2" xfId="51"/>
-    <cellStyle name="Note 3" xfId="52"/>
-    <cellStyle name="Note 4" xfId="53"/>
+    <cellStyle name="Note 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Note 3" xfId="52" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Note 4" xfId="53" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="44"/>
-    <cellStyle name="Style 1" xfId="50"/>
-    <cellStyle name="Title 2" xfId="42"/>
+    <cellStyle name="Percent 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Style 1" xfId="50" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Title 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
@@ -12876,7 +12946,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13212,7 +13281,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -32179,7 +32247,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -32209,7 +32283,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -32239,7 +32319,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -32269,7 +32355,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -32301,7 +32393,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -32331,7 +32429,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -32363,7 +32467,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -32398,7 +32508,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -32436,7 +32552,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -32565,7 +32687,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Baseline estimates of coverage of 90-90-90 targets in Nyanza region, Kenya AIDS Indicator Survey, 2012–2013*."/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Baseline estimates of coverage of 90-90-90 targets in Nyanza region, Kenya AIDS Indicator Survey, 2012–2013*.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -32620,7 +32748,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -32658,7 +32792,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="https://www.dovepress.com/cr_data/article_fulltext/s153000/153185/img/hiv-153185_T003.jpg"/>
+        <xdr:cNvPr id="6" name="Picture 5" descr="https://www.dovepress.com/cr_data/article_fulltext/s153000/153185/img/hiv-153185_T003.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -32713,7 +32853,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9219" name="AutoShape 3" descr="https://images.journals.lww.com/aidsonline/Original.00002030-201207310-00012.F3-12.jpeg"/>
+        <xdr:cNvPr id="9219" name="AutoShape 3" descr="https://images.journals.lww.com/aidsonline/Original.00002030-201207310-00012.F3-12.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000003240000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -32755,7 +32901,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -32793,7 +32945,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextBox 7"/>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -32896,7 +33054,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="An external file that holds a picture, illustration, etc.&#10;Object name is peerj-06-4427-g002.jpg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="An external file that holds a picture, illustration, etc.&#10;Object name is peerj-06-4427-g002.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -32956,7 +33120,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -32994,7 +33164,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -33035,7 +33211,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33106,7 +33282,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33174,7 +33350,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2049" name="AutoShape 1" descr="https://images.journals.lww.com/aidsonline/Original.00002030-200108004-00006.T2-6.jpeg"/>
+        <xdr:cNvPr id="2049" name="AutoShape 1" descr="https://images.journals.lww.com/aidsonline/Original.00002030-200108004-00006.T2-6.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -33216,7 +33398,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -33260,7 +33448,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -33298,7 +33492,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -33328,7 +33528,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -33360,7 +33566,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -33390,7 +33602,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -33422,7 +33640,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="TextBox 10"/>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -33532,7 +33756,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -33569,7 +33799,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="TextBox 13"/>
+        <xdr:cNvPr id="14" name="TextBox 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -33643,7 +33879,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -33781,7 +34023,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -33819,7 +34067,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -33856,7 +34110,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -33886,7 +34146,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -33916,7 +34182,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -33951,7 +34223,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -33981,7 +34259,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34011,7 +34295,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34046,7 +34336,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="An external file that holds a picture, illustration, etc.&#10;Object name is 12879_2019_3982_Fig1_HTML.jpg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="An external file that holds a picture, illustration, etc.&#10;Object name is 12879_2019_3982_Fig1_HTML.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -34106,7 +34402,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="image"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -34166,7 +34468,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34204,7 +34512,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34242,7 +34556,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34280,7 +34600,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="7" name="Group 6"/>
+        <xdr:cNvPr id="7" name="Group 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
@@ -34293,7 +34619,13 @@
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="5" name="Picture 4"/>
+          <xdr:cNvPr id="5" name="Picture 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000005000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -34316,7 +34648,13 @@
       </xdr:pic>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="TextBox 5"/>
+          <xdr:cNvPr id="6" name="TextBox 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000006000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -34386,7 +34724,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34424,7 +34768,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34462,7 +34812,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34500,7 +34856,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34530,7 +34892,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34560,7 +34928,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34598,7 +34972,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34641,7 +35021,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34685,7 +35071,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -34979,7 +35371,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y231"/>
   <sheetViews>
     <sheetView topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -41407,7 +41799,7 @@
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B167" s="49"/>
       <c r="C167" s="49"/>
@@ -41416,7 +41808,7 @@
       <c r="F167" s="49"/>
       <c r="G167" s="77"/>
       <c r="H167" s="77" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="I167" s="49"/>
       <c r="J167" s="49"/>
@@ -41445,10 +41837,10 @@
         <v>196</v>
       </c>
       <c r="I168" t="s">
+        <v>1242</v>
+      </c>
+      <c r="J168" s="76" t="s">
         <v>1243</v>
-      </c>
-      <c r="J168" s="76" t="s">
-        <v>1244</v>
       </c>
       <c r="K168" s="76" t="s">
         <v>1011</v>
@@ -41460,10 +41852,10 @@
         <v>157</v>
       </c>
       <c r="N168" s="76" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="O168" s="49" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="P168" s="37"/>
       <c r="Q168" s="16"/>
@@ -41769,7 +42161,7 @@
         <v>63.501959516313946</v>
       </c>
       <c r="H176" s="77" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="J176" s="37"/>
       <c r="K176" s="37"/>
@@ -41786,10 +42178,10 @@
         <v>196</v>
       </c>
       <c r="I177" s="37" t="s">
+        <v>1242</v>
+      </c>
+      <c r="J177" s="76" t="s">
         <v>1243</v>
-      </c>
-      <c r="J177" s="76" t="s">
-        <v>1244</v>
       </c>
       <c r="K177" s="76" t="s">
         <v>1011</v>
@@ -41801,10 +42193,10 @@
         <v>157</v>
       </c>
       <c r="N177" s="76" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="O177" s="49" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="178" spans="2:15" x14ac:dyDescent="0.25">
@@ -42085,7 +42477,7 @@
     </row>
     <row r="186" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H186" s="77" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="I186" s="37"/>
       <c r="J186" s="37"/>
@@ -42100,10 +42492,10 @@
         <v>196</v>
       </c>
       <c r="I187" s="37" t="s">
+        <v>1242</v>
+      </c>
+      <c r="J187" s="76" t="s">
         <v>1243</v>
-      </c>
-      <c r="J187" s="76" t="s">
-        <v>1244</v>
       </c>
       <c r="K187" s="76" t="s">
         <v>1011</v>
@@ -42115,10 +42507,10 @@
         <v>157</v>
       </c>
       <c r="N187" s="76" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="O187" s="49" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="188" spans="2:15" x14ac:dyDescent="0.25">
@@ -42354,10 +42746,10 @@
     </row>
     <row r="196" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="H196" s="77" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="I196" s="49"/>
       <c r="J196" s="49"/>
@@ -42372,13 +42764,13 @@
         <v>1072</v>
       </c>
       <c r="C197" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D197" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E197" t="s">
         <v>1298</v>
-      </c>
-      <c r="D197" t="s">
-        <v>1306</v>
-      </c>
-      <c r="E197" t="s">
-        <v>1299</v>
       </c>
       <c r="F197" s="37"/>
       <c r="G197" s="37"/>
@@ -42386,10 +42778,10 @@
         <v>196</v>
       </c>
       <c r="I197" s="37" t="s">
+        <v>1242</v>
+      </c>
+      <c r="J197" s="76" t="s">
         <v>1243</v>
-      </c>
-      <c r="J197" s="76" t="s">
-        <v>1244</v>
       </c>
       <c r="K197" s="76" t="s">
         <v>1011</v>
@@ -42401,10 +42793,10 @@
         <v>157</v>
       </c>
       <c r="N197" s="76" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="O197" s="49" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="198" spans="1:15" x14ac:dyDescent="0.25">
@@ -42562,13 +42954,13 @@
         <v>1072</v>
       </c>
       <c r="C203" s="37" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D203" s="37" t="s">
+        <v>1306</v>
+      </c>
+      <c r="E203" s="37" t="s">
         <v>1300</v>
-      </c>
-      <c r="D203" s="37" t="s">
-        <v>1307</v>
-      </c>
-      <c r="E203" s="37" t="s">
-        <v>1301</v>
       </c>
       <c r="F203" s="37"/>
       <c r="G203" s="37"/>
@@ -42651,13 +43043,13 @@
         <v>1072</v>
       </c>
       <c r="C209" s="37" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D209" s="37" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E209" s="37" t="s">
         <v>1302</v>
-      </c>
-      <c r="D209" s="37" t="s">
-        <v>1308</v>
-      </c>
-      <c r="E209" s="37" t="s">
-        <v>1303</v>
       </c>
     </row>
     <row r="210" spans="2:5" x14ac:dyDescent="0.25">
@@ -42730,13 +43122,13 @@
         <v>1072</v>
       </c>
       <c r="C215" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D215" t="s">
+        <v>1308</v>
+      </c>
+      <c r="E215" t="s">
         <v>1304</v>
-      </c>
-      <c r="D215" t="s">
-        <v>1309</v>
-      </c>
-      <c r="E215" t="s">
-        <v>1305</v>
       </c>
     </row>
     <row r="216" spans="2:5" x14ac:dyDescent="0.25">
@@ -42809,13 +43201,13 @@
         <v>1072</v>
       </c>
       <c r="C221" s="37" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D221" s="37" t="s">
+        <v>1328</v>
+      </c>
+      <c r="E221" s="37" t="s">
         <v>1327</v>
-      </c>
-      <c r="D221" s="37" t="s">
-        <v>1329</v>
-      </c>
-      <c r="E221" s="37" t="s">
-        <v>1328</v>
       </c>
     </row>
     <row r="222" spans="2:5" x14ac:dyDescent="0.25">
@@ -42890,13 +43282,13 @@
         <v>1072</v>
       </c>
       <c r="C227" s="37" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D227" s="37" t="s">
         <v>1330</v>
       </c>
-      <c r="D227" s="37" t="s">
+      <c r="E227" s="37" t="s">
         <v>1331</v>
-      </c>
-      <c r="E227" s="37" t="s">
-        <v>1332</v>
       </c>
     </row>
     <row r="228" spans="2:6" x14ac:dyDescent="0.25">
@@ -42976,7 +43368,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E836CD1-F16D-4F6D-B065-35D50B596CED}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AD213"/>
   <sheetViews>
     <sheetView topLeftCell="A115" workbookViewId="0">
@@ -43026,10 +43430,10 @@
         <v>144</v>
       </c>
       <c r="J3" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K3" t="s">
         <v>1334</v>
-      </c>
-      <c r="K3" t="s">
-        <v>1335</v>
       </c>
       <c r="N3" s="21" t="s">
         <v>80</v>
@@ -43038,28 +43442,28 @@
         <v>222</v>
       </c>
       <c r="P3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="Q3" t="s">
         <v>1246</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>1247</v>
       </c>
       <c r="R3" s="21" t="s">
         <v>217</v>
       </c>
       <c r="S3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="T3" t="s">
         <v>1246</v>
-      </c>
-      <c r="T3" t="s">
-        <v>1247</v>
       </c>
       <c r="U3" s="21" t="s">
         <v>144</v>
       </c>
       <c r="V3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="W3" t="s">
         <v>1246</v>
-      </c>
-      <c r="W3" t="s">
-        <v>1247</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -43524,13 +43928,13 @@
         <v>392</v>
       </c>
       <c r="O11" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="P11" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="Q11" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="R11" s="8">
         <v>20.7746</v>
@@ -43966,7 +44370,7 @@
       </c>
       <c r="E34" s="54"/>
       <c r="F34" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="G34" s="37">
         <v>1</v>
@@ -44004,7 +44408,7 @@
       </c>
       <c r="E35" s="54"/>
       <c r="F35" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="G35" s="37">
         <v>3.1</v>
@@ -44042,7 +44446,7 @@
       </c>
       <c r="E36" s="54"/>
       <c r="F36" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="G36" s="37">
         <v>6.3</v>
@@ -44080,7 +44484,7 @@
       </c>
       <c r="E37" s="54"/>
       <c r="F37" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="G37" s="37">
         <v>6.6</v>
@@ -44118,7 +44522,7 @@
       </c>
       <c r="E38" s="54"/>
       <c r="F38" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="G38" s="37">
         <v>8.6999999999999993</v>
@@ -44156,7 +44560,7 @@
       </c>
       <c r="E39" s="54"/>
       <c r="F39" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="G39" s="37">
         <v>9.3000000000000007</v>
@@ -44194,7 +44598,7 @@
       </c>
       <c r="E40" s="54"/>
       <c r="F40" s="21" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="G40" s="37">
         <v>9.8000000000000007</v>
@@ -44225,7 +44629,7 @@
       </c>
       <c r="E41" s="54"/>
       <c r="F41" s="21" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="G41" s="37">
         <v>8.4</v>
@@ -44256,7 +44660,7 @@
       </c>
       <c r="E42" s="54"/>
       <c r="F42" s="21" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="G42" s="37">
         <v>4.4000000000000004</v>
@@ -44287,7 +44691,7 @@
       </c>
       <c r="E43" s="54"/>
       <c r="F43" s="21" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="G43" s="37">
         <v>4</v>
@@ -44607,28 +45011,28 @@
         <v>222</v>
       </c>
       <c r="D61" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E61" t="s">
         <v>1246</v>
-      </c>
-      <c r="E61" t="s">
-        <v>1247</v>
       </c>
       <c r="F61" s="21" t="s">
         <v>217</v>
       </c>
       <c r="G61" t="s">
+        <v>1245</v>
+      </c>
+      <c r="H61" t="s">
         <v>1246</v>
-      </c>
-      <c r="H61" t="s">
-        <v>1247</v>
       </c>
       <c r="I61" s="21" t="s">
         <v>144</v>
       </c>
       <c r="J61" t="s">
+        <v>1245</v>
+      </c>
+      <c r="K61" t="s">
         <v>1246</v>
-      </c>
-      <c r="K61" t="s">
-        <v>1247</v>
       </c>
       <c r="M61" s="37" t="s">
         <v>80</v>
@@ -44637,28 +45041,28 @@
         <v>222</v>
       </c>
       <c r="O61" s="37" t="s">
+        <v>1245</v>
+      </c>
+      <c r="P61" s="37" t="s">
         <v>1246</v>
-      </c>
-      <c r="P61" s="37" t="s">
-        <v>1247</v>
       </c>
       <c r="Q61" s="37" t="s">
         <v>217</v>
       </c>
       <c r="R61" s="37" t="s">
+        <v>1245</v>
+      </c>
+      <c r="S61" s="37" t="s">
         <v>1246</v>
-      </c>
-      <c r="S61" s="37" t="s">
-        <v>1247</v>
       </c>
       <c r="T61" s="37" t="s">
         <v>144</v>
       </c>
       <c r="U61" s="37" t="s">
+        <v>1245</v>
+      </c>
+      <c r="V61" s="37" t="s">
         <v>1246</v>
-      </c>
-      <c r="V61" s="37" t="s">
-        <v>1247</v>
       </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
@@ -45100,13 +45504,13 @@
         <v>392</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="D69" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="E69" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="F69" s="8">
         <v>15.9094</v>
@@ -45118,7 +45522,7 @@
         <v>28.742100000000001</v>
       </c>
       <c r="I69" s="31" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="J69" s="8">
         <v>3.0767000000000002</v>
@@ -45130,13 +45534,13 @@
         <v>392</v>
       </c>
       <c r="N69" s="37" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="O69" s="37" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="P69" s="37" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="Q69" s="7">
         <v>9.1097999999999999</v>
@@ -46514,7 +46918,7 @@
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.25">
@@ -46531,7 +46935,7 @@
         <v>576</v>
       </c>
       <c r="G183" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="I183" t="s">
         <v>222</v>
@@ -47694,8 +48098,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
@@ -48973,7 +49377,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -49362,17 +49766,17 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -49383,19 +49787,19 @@
         <v>561</v>
       </c>
       <c r="D74" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E74" t="s">
         <v>1234</v>
       </c>
-      <c r="E74" t="s">
+      <c r="F74" t="s">
         <v>1235</v>
       </c>
-      <c r="F74" t="s">
+      <c r="I74" t="s">
         <v>1236</v>
       </c>
-      <c r="I74" t="s">
-        <v>1237</v>
-      </c>
       <c r="J74" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -49586,8 +49990,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -49698,8 +50102,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:Z194"/>
   <sheetViews>
     <sheetView topLeftCell="A172" workbookViewId="0">
@@ -49944,7 +50348,7 @@
     </row>
     <row r="25" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="37" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>1125</v>
@@ -49956,13 +50360,13 @@
         <v>1127</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="G25" s="18" t="s">
         <v>1125</v>
       </c>
       <c r="H25" s="37" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="I25" s="37" t="s">
         <v>1127</v>
@@ -50135,11 +50539,11 @@
       <c r="Z33" s="4"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C34" s="84">
+      <c r="C34" s="86">
         <v>2015</v>
       </c>
-      <c r="D34" s="84"/>
-      <c r="E34" s="84"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
       <c r="F34" s="23">
         <v>2015</v>
       </c>
@@ -50941,7 +51345,7 @@
         <v>576</v>
       </c>
       <c r="J99" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -51610,7 +52014,7 @@
     <mergeCell ref="C34:E34"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A155" r:id="rId1"/>
+    <hyperlink ref="A155" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -51618,8 +52022,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -51684,8 +52088,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A2:H90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -52568,8 +52972,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -53140,12 +53544,121 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E3F8A6-BB0F-4F7C-B697-F36F790CC179}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="84"/>
+    <col min="3" max="3" width="9.140625" style="84"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="84" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1353</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="84" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="84" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="84" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="84" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="84" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C14" s="84" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>25</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y256"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Y259"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="B174" sqref="B174"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="S103" sqref="S102:S103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54931,7 +55444,7 @@
         <v>137</v>
       </c>
       <c r="L76" s="37">
-        <v>0.22517599999999999</v>
+        <v>0.425176</v>
       </c>
       <c r="M76" s="37">
         <v>2.1546289999999999</v>
@@ -55799,7 +56312,7 @@
       </c>
       <c r="H92" s="41"/>
       <c r="K92" s="71" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.25">
@@ -55844,7 +56357,7 @@
         <v>16.8</v>
       </c>
       <c r="K95" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.25">
@@ -55864,7 +56377,7 @@
         <v>490</v>
       </c>
       <c r="M96" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="N96" t="s">
         <v>492</v>
@@ -57684,7 +58197,7 @@
       </c>
       <c r="G194" s="72"/>
       <c r="H194" s="72" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="I194" s="72"/>
       <c r="J194" s="72" t="s">
@@ -58284,17 +58797,56 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>1138</v>
+      <c r="A256" s="2" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B257" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C257" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D257" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B258" s="6">
+        <v>11.364000000000001</v>
+      </c>
+      <c r="C258" s="6">
+        <v>10.2683</v>
+      </c>
+      <c r="D258" s="6">
+        <v>12.4597</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B259" s="6">
+        <v>23.3659</v>
+      </c>
+      <c r="C259" s="6">
+        <v>21.858599999999999</v>
+      </c>
+      <c r="D259" s="6">
+        <v>24.873200000000001</v>
       </c>
     </row>
   </sheetData>
@@ -58305,7 +58857,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S68"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
@@ -58331,10 +58883,10 @@
         <v>158</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="O2" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -58348,7 +58900,7 @@
         <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="G3" t="s">
         <v>575</v>
@@ -58578,7 +59130,7 @@
         <v>59.412199999999999</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="K9" s="7">
         <v>39.2258</v>
@@ -58633,15 +59185,15 @@
     <row r="12" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="14" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="37" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="15" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -58670,7 +59222,7 @@
         <v>576</v>
       </c>
       <c r="L15" s="37" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -58834,7 +59386,7 @@
         <v>80.099999999999994</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="H21" s="7">
         <v>39.386299999999999</v>
@@ -58867,7 +59419,7 @@
     <row r="23" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -58895,7 +59447,7 @@
         <v>246</v>
       </c>
       <c r="G27" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="H27" t="s">
         <v>575</v>
@@ -58927,22 +59479,22 @@
         <v>155</v>
       </c>
       <c r="G28" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="H28" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="I28" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="J28" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="K28" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="L28" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -58956,48 +59508,48 @@
         <v>91.2</v>
       </c>
       <c r="F29" s="37" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="H29" s="37" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="I29" s="37" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="J29" s="37" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="K29" s="37" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="L29" s="37" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F30" s="37" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="G30" s="37" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="H30" s="37" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="I30" s="37" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="J30" s="37" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="K30" s="37" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="L30" s="37" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -59005,25 +59557,25 @@
         <v>418</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="G31" s="37" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="H31" s="37" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="I31" s="37" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="J31" s="37" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="K31" s="37" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="L31" s="37" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -59034,25 +59586,25 @@
         <v>2012</v>
       </c>
       <c r="F32" s="37" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="G32" s="37" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="H32" s="37" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="I32" s="37" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="J32" s="37" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="K32" s="37" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="L32" s="37" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -59090,7 +59642,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -59104,7 +59656,7 @@
         <v>179</v>
       </c>
       <c r="J38" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -59339,7 +59891,7 @@
         <v>68</v>
       </c>
       <c r="J45" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="K45" s="7">
         <v>60.636200000000002</v>
@@ -59396,17 +59948,17 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="37" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -59416,7 +59968,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="57" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -59599,7 +60151,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AL153"/>
   <sheetViews>
     <sheetView topLeftCell="A127" workbookViewId="0">
@@ -62879,7 +63431,7 @@
         <v>456</v>
       </c>
       <c r="J103" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="104" spans="2:32" x14ac:dyDescent="0.25">
@@ -63509,7 +64061,7 @@
         <v>7.4809999999999999</v>
       </c>
       <c r="K127" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="128" spans="2:11" x14ac:dyDescent="0.25">
@@ -63520,7 +64072,7 @@
         <v>7.4809999999999999</v>
       </c>
       <c r="K128" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="129" spans="6:11" x14ac:dyDescent="0.25">
@@ -63531,7 +64083,7 @@
         <v>7.4809999999999999</v>
       </c>
       <c r="K129" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="130" spans="6:11" x14ac:dyDescent="0.25">
@@ -63545,7 +64097,7 @@
         <v>7.4809999999999999</v>
       </c>
       <c r="K130" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="131" spans="6:11" x14ac:dyDescent="0.25">
@@ -63559,7 +64111,7 @@
         <v>7.7850000000000001</v>
       </c>
       <c r="K131" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="132" spans="6:11" x14ac:dyDescent="0.25">
@@ -63573,7 +64125,7 @@
         <v>8.0650000000000013</v>
       </c>
       <c r="K132" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="133" spans="6:11" x14ac:dyDescent="0.25">
@@ -63587,7 +64139,7 @@
         <v>8.1100000000000012</v>
       </c>
       <c r="K133" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="134" spans="6:11" x14ac:dyDescent="0.25">
@@ -63601,7 +64153,7 @@
         <v>7.99</v>
       </c>
       <c r="K134" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="135" spans="6:11" x14ac:dyDescent="0.25">
@@ -63615,7 +64167,7 @@
         <v>7.64</v>
       </c>
       <c r="K135" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="136" spans="6:11" x14ac:dyDescent="0.25">
@@ -63629,7 +64181,7 @@
         <v>7.2160000000000002</v>
       </c>
       <c r="K136" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="137" spans="6:11" x14ac:dyDescent="0.25">
@@ -64221,7 +64773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AX132"/>
   <sheetViews>
     <sheetView topLeftCell="A92" workbookViewId="0">
@@ -65129,25 +65681,25 @@
         <v>80</v>
       </c>
       <c r="C71" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D71" t="s">
         <v>1310</v>
       </c>
-      <c r="D71" t="s">
-        <v>1311</v>
-      </c>
       <c r="E71" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="F71" t="s">
         <v>246</v>
       </c>
       <c r="G71" t="s">
+        <v>1311</v>
+      </c>
+      <c r="H71" t="s">
         <v>1312</v>
       </c>
-      <c r="H71" t="s">
-        <v>1313</v>
-      </c>
       <c r="I71" s="37" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="J71" s="37" t="s">
         <v>246</v>
@@ -65881,10 +66433,10 @@
     </row>
     <row r="91" spans="1:50" x14ac:dyDescent="0.25">
       <c r="U91" t="s">
+        <v>1228</v>
+      </c>
+      <c r="AF91" t="s">
         <v>1229</v>
-      </c>
-      <c r="AF91" t="s">
-        <v>1230</v>
       </c>
     </row>
     <row r="92" spans="1:50" x14ac:dyDescent="0.25">
@@ -65892,16 +66444,16 @@
         <v>1071</v>
       </c>
       <c r="R92" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="U92" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="V92">
         <v>0.5</v>
       </c>
       <c r="W92" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="X92">
         <v>0.4</v>
@@ -65913,23 +66465,23 @@
         <v>0.25</v>
       </c>
       <c r="AA92" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="AB92">
         <v>0.15</v>
       </c>
       <c r="AC92" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="AD92">
         <v>0.15</v>
       </c>
       <c r="AF92" s="37" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="AG92" s="37"/>
       <c r="AH92" s="37" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="AI92" s="37"/>
       <c r="AJ92" s="37">
@@ -65937,11 +66489,11 @@
       </c>
       <c r="AK92" s="37"/>
       <c r="AL92" s="37" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="AM92" s="37"/>
       <c r="AN92" s="37" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="AO92" s="37"/>
       <c r="AP92" s="37"/>
@@ -65995,7 +66547,7 @@
         <v>222</v>
       </c>
       <c r="R93" s="37" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="S93" s="37">
         <v>1.5</v>
@@ -66113,7 +66665,7 @@
         <v>2.6945755989701607E-2</v>
       </c>
       <c r="R94" s="37" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="S94" s="37">
         <v>1.4</v>
@@ -66322,7 +66874,7 @@
         <v>5.2077410999999999E-4</v>
       </c>
       <c r="R96" s="37" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="S96" s="37">
         <v>1.1499999999999999</v>
@@ -66428,7 +66980,7 @@
         <v>8.5921136E-4</v>
       </c>
       <c r="R97" s="37" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="S97" s="37">
         <v>1.1499999999999999</v>
@@ -68126,7 +68678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R247"/>
   <sheetViews>
     <sheetView topLeftCell="A112" workbookViewId="0">
@@ -69012,7 +69564,7 @@
         <v>106</v>
       </c>
       <c r="H71" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -69626,7 +70178,7 @@
         <v>1</v>
       </c>
       <c r="H130" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -70538,13 +71090,13 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="198" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="37" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
@@ -70574,12 +71126,12 @@
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.25">
@@ -70587,15 +71139,15 @@
         <v>74</v>
       </c>
       <c r="D210" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="E210" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="211" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C211">
         <v>36</v>
@@ -70606,7 +71158,7 @@
     </row>
     <row r="212" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C212">
         <v>67</v>
@@ -70617,7 +71169,7 @@
     </row>
     <row r="213" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C213">
         <v>51</v>
@@ -70628,7 +71180,7 @@
     </row>
     <row r="214" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C214">
         <v>43</v>
@@ -70639,7 +71191,7 @@
     </row>
     <row r="215" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C215">
         <v>52</v>
@@ -70687,35 +71239,35 @@
     </row>
     <row r="220" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="221" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="222" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C222" s="66" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D222" s="66" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E222" s="66" t="s">
         <v>1181</v>
-      </c>
-      <c r="C222" s="66" t="s">
-        <v>1185</v>
-      </c>
-      <c r="D222" s="66" t="s">
-        <v>1179</v>
-      </c>
-      <c r="E222" s="66" t="s">
-        <v>1182</v>
       </c>
       <c r="F222" s="66" t="s">
         <v>576</v>
       </c>
       <c r="G222" s="67" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="H222" s="67" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="I222" s="67" t="s">
         <v>575</v>
@@ -70733,24 +71285,24 @@
         <v>576</v>
       </c>
       <c r="N222" s="69" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="O222" s="69" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="P222" s="69" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="223" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B223" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C223" s="66" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="D223" s="66">
         <v>22.2</v>
@@ -70762,7 +71314,7 @@
         <v>29.8</v>
       </c>
       <c r="G223" s="67" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="H223" s="67">
         <v>76.900000000000006</v>
@@ -70786,21 +71338,21 @@
         <v>7.8</v>
       </c>
       <c r="O223" s="69" t="s">
+        <v>1206</v>
+      </c>
+      <c r="P223" s="69" t="s">
         <v>1207</v>
-      </c>
-      <c r="P223" s="69" t="s">
-        <v>1208</v>
       </c>
     </row>
     <row r="224" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B224" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="C224" s="66" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="D224" s="66">
         <v>15.8</v>
@@ -70812,7 +71364,7 @@
         <v>17.7</v>
       </c>
       <c r="G224" s="67" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="H224" s="67">
         <v>25.7</v>
@@ -70837,24 +71389,24 @@
         <v>7.7220077220077217</v>
       </c>
       <c r="O224" s="69" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="P224" s="69">
         <v>2009</v>
       </c>
       <c r="Q224" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B225" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C225" s="66" t="s">
         <v>1192</v>
-      </c>
-      <c r="C225" s="66" t="s">
-        <v>1193</v>
       </c>
       <c r="D225" s="66">
         <v>38.700000000000003</v>
@@ -70866,7 +71418,7 @@
         <v>41.8</v>
       </c>
       <c r="G225" s="67" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="H225" s="67">
         <v>74.099999999999994</v>
@@ -70890,7 +71442,7 @@
         <v>30</v>
       </c>
       <c r="O225" s="69" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="P225" s="69">
         <v>2006</v>
@@ -70898,15 +71450,15 @@
     </row>
     <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="M227" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="M228" t="s">
         <v>559</v>
@@ -70926,7 +71478,7 @@
         <v>106</v>
       </c>
       <c r="E229" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F229" t="s">
         <v>575</v>
@@ -70941,10 +71493,10 @@
         <v>106</v>
       </c>
       <c r="K229" s="37" t="s">
+        <v>1203</v>
+      </c>
+      <c r="M229" t="s">
         <v>1204</v>
-      </c>
-      <c r="M229" t="s">
-        <v>1205</v>
       </c>
       <c r="N229" t="s">
         <v>575</v>
@@ -70953,7 +71505,7 @@
         <v>576</v>
       </c>
       <c r="P229" s="37" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="Q229" s="37" t="s">
         <v>575</v>
@@ -70964,7 +71516,7 @@
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="C230">
         <v>9</v>
@@ -71246,7 +71798,7 @@
     </row>
     <row r="236" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="C236">
         <v>54</v>
@@ -71293,7 +71845,7 @@
     </row>
     <row r="238" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="I238" s="37" t="s">
         <v>559</v>
@@ -71496,7 +72048,7 @@
     </row>
     <row r="244" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C244">
         <v>189</v>
@@ -71538,7 +72090,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L38" r:id="rId1"/>
+    <hyperlink ref="L38" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -71547,7 +72099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -71945,12 +72497,12 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -71974,7 +72526,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="C59" s="18">
         <v>0.13100000000000001</v>
@@ -71996,7 +72548,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C61" s="18">
         <v>0.27400000000000002</v>
@@ -72008,17 +72560,17 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
@@ -72031,7 +72583,7 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C67">
         <v>112</v>
@@ -72090,7 +72642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
@@ -72790,30 +73342,30 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="65" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="37" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="E65" s="37" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="E66" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="F66" t="s">
         <v>188</v>
       </c>
       <c r="G66" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -72869,7 +73421,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="C70">
         <v>1.2</v>
@@ -72903,7 +73455,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -72926,11 +73478,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:S136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46:F58"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -73140,7 +73692,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="37" t="s">
         <v>141</v>
       </c>
@@ -73148,7 +73700,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="37" t="s">
         <v>142</v>
       </c>
@@ -73156,7 +73708,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="37" t="s">
         <v>143</v>
       </c>
@@ -73164,7 +73716,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="37" t="s">
         <v>318</v>
       </c>
@@ -73172,7 +73724,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="37" t="s">
         <v>319</v>
       </c>
@@ -73180,7 +73732,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="37" t="s">
         <v>324</v>
       </c>
@@ -73188,7 +73740,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="37" t="s">
         <v>325</v>
       </c>
@@ -73196,7 +73748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="37" t="s">
         <v>326</v>
       </c>
@@ -73204,7 +73756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="37" t="s">
         <v>617</v>
       </c>
@@ -73212,266 +73764,313 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="37" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="44" spans="2:6" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="37" t="s">
+    <row r="44" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="84"/>
+      <c r="C44" s="84" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="37" t="s">
+      <c r="D44" s="84"/>
+      <c r="E44" s="84"/>
+      <c r="F44" s="84"/>
+      <c r="G44" s="84"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="84" t="s">
         <v>150</v>
       </c>
-      <c r="C45" t="s">
-        <v>1167</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C45" s="84" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D45" s="84" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E45" s="84" t="s">
         <v>1165</v>
       </c>
-      <c r="E45" t="s">
-        <v>1166</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="F45" s="84" t="s">
         <v>1350</v>
       </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="37" t="s">
+      <c r="G45" s="84" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="84" t="s">
         <v>137</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="84">
         <v>0</v>
       </c>
-      <c r="D46" s="37">
+      <c r="D46" s="84">
         <v>1</v>
       </c>
-      <c r="E46" s="37">
+      <c r="E46" s="84">
         <v>2</v>
       </c>
-      <c r="F46" s="8">
-        <v>0.71663276499999995</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="37" t="s">
+      <c r="F46" s="84">
+        <v>0</v>
+      </c>
+      <c r="G46" s="85">
+        <v>0.71663276482550398</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="84" t="s">
         <v>138</v>
       </c>
-      <c r="C47" s="37">
+      <c r="C47" s="84">
         <v>1.67</v>
       </c>
-      <c r="D47" s="37">
+      <c r="D47" s="84">
         <v>12</v>
       </c>
-      <c r="E47" s="37">
+      <c r="E47" s="84">
         <v>3</v>
       </c>
-      <c r="F47" s="8">
-        <v>0.84806759499999995</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="37" t="s">
+      <c r="F47" s="84">
+        <v>1</v>
+      </c>
+      <c r="G47" s="85">
+        <v>0.84806759505553897</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="84" t="s">
         <v>139</v>
       </c>
-      <c r="C48" s="37">
+      <c r="C48" s="84">
         <v>3.63</v>
       </c>
-      <c r="D48" s="37">
+      <c r="D48" s="84">
         <v>34</v>
       </c>
-      <c r="E48" s="37">
+      <c r="E48" s="84">
         <v>7</v>
       </c>
-      <c r="F48" s="8">
-        <v>7.9909247380000004</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="37" t="s">
+      <c r="F48" s="84">
+        <v>7</v>
+      </c>
+      <c r="G48" s="85">
+        <v>7.9909247379126498</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="84" t="s">
         <v>140</v>
       </c>
-      <c r="C49" s="37">
+      <c r="C49" s="84">
         <v>14.37</v>
       </c>
-      <c r="D49" s="37">
+      <c r="D49" s="84">
         <v>86</v>
       </c>
-      <c r="E49" s="37">
+      <c r="E49" s="84">
         <v>21</v>
       </c>
-      <c r="F49" s="8">
-        <v>20.97637302</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="37" t="s">
+      <c r="F49" s="84">
+        <v>9</v>
+      </c>
+      <c r="G49" s="85">
+        <v>20.976373024565699</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="84" t="s">
         <v>141</v>
       </c>
-      <c r="C50" s="37">
+      <c r="C50" s="84">
         <v>41.72</v>
       </c>
-      <c r="D50" s="37">
+      <c r="D50" s="84">
         <v>156</v>
       </c>
-      <c r="E50" s="37">
+      <c r="E50" s="84">
         <v>27</v>
       </c>
-      <c r="F50" s="8">
-        <v>40.716632760000003</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="37" t="s">
+      <c r="F50" s="84">
+        <v>24</v>
+      </c>
+      <c r="G50" s="85">
+        <v>40.716632764825398</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="84" t="s">
         <v>142</v>
       </c>
-      <c r="C51" s="37">
+      <c r="C51" s="84">
         <v>70.34</v>
       </c>
-      <c r="D51" s="37">
+      <c r="D51" s="84">
         <v>187</v>
       </c>
-      <c r="E51" s="37">
+      <c r="E51" s="84">
         <v>35</v>
       </c>
-      <c r="F51" s="8">
-        <v>62.664684710000003</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="37" t="s">
+      <c r="F51" s="84">
+        <v>28</v>
+      </c>
+      <c r="G51" s="85">
+        <v>62.664684712877403</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="84" t="s">
         <v>143</v>
       </c>
-      <c r="C52" s="37">
+      <c r="C52" s="84">
         <v>74.19</v>
       </c>
-      <c r="D52" s="37">
+      <c r="D52" s="84">
         <v>163</v>
       </c>
-      <c r="E52" s="37">
+      <c r="E52" s="84">
         <v>36</v>
       </c>
-      <c r="F52" s="8">
-        <v>83.052730400000002</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="37" t="s">
+      <c r="F52" s="84">
+        <v>31</v>
+      </c>
+      <c r="G52" s="85">
+        <v>83.052730402127906</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="84" t="s">
         <v>318</v>
       </c>
-      <c r="C53" s="37">
+      <c r="C53" s="84">
         <v>127.79</v>
       </c>
-      <c r="D53" s="37">
+      <c r="D53" s="84">
         <v>144</v>
       </c>
-      <c r="E53" s="37">
+      <c r="E53" s="84">
         <v>27</v>
       </c>
-      <c r="F53" s="8">
-        <v>103.4423408</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="37" t="s">
+      <c r="F53" s="84">
+        <v>30</v>
+      </c>
+      <c r="G53" s="85">
+        <v>103.442340791738</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="84" t="s">
         <v>319</v>
       </c>
-      <c r="C54" s="37">
+      <c r="C54" s="84">
         <v>148.35</v>
       </c>
-      <c r="D54" s="37">
+      <c r="D54" s="84">
         <v>120</v>
       </c>
-      <c r="E54" s="37">
+      <c r="E54" s="84">
         <v>21</v>
       </c>
-      <c r="F54" s="8">
-        <v>130.323893</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="37" t="s">
+      <c r="F54" s="84">
+        <v>23</v>
+      </c>
+      <c r="G54" s="85">
+        <v>130.32389297449501</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="84" t="s">
         <v>324</v>
       </c>
-      <c r="C55" s="37">
+      <c r="C55" s="84">
         <v>193.66</v>
       </c>
-      <c r="D55" s="37">
+      <c r="D55" s="84">
         <v>90</v>
       </c>
-      <c r="E55" s="37">
+      <c r="E55" s="84">
         <v>15</v>
       </c>
-      <c r="F55" s="8">
-        <v>150.4537631</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="37" t="s">
+      <c r="F55" s="84">
+        <v>23</v>
+      </c>
+      <c r="G55" s="85">
+        <v>150.45376310436501</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="84" t="s">
         <v>325</v>
       </c>
-      <c r="C56" s="37">
+      <c r="C56" s="84">
         <v>199.95</v>
       </c>
-      <c r="D56" s="37">
+      <c r="D56" s="84">
         <v>57</v>
       </c>
-      <c r="E56" s="37">
+      <c r="E56" s="84">
         <v>11</v>
       </c>
-      <c r="F56" s="8">
-        <v>156.29791890000001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="37" t="s">
+      <c r="F56" s="84">
+        <v>11</v>
+      </c>
+      <c r="G56" s="85">
+        <v>156.29791894852099</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="84" t="s">
         <v>326</v>
       </c>
-      <c r="C57" s="37">
+      <c r="C57" s="84">
         <v>170.4</v>
       </c>
-      <c r="D57" s="37">
+      <c r="D57" s="84">
         <v>40</v>
       </c>
-      <c r="E57" s="37">
+      <c r="E57" s="84">
         <v>9</v>
       </c>
-      <c r="F57" s="8">
-        <v>150.71350340000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="37" t="s">
+      <c r="F57" s="84">
+        <v>15</v>
+      </c>
+      <c r="G57" s="85">
+        <v>150.71350336410501</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="84" t="s">
         <v>617</v>
       </c>
-      <c r="C58" s="37">
+      <c r="C58" s="84">
         <v>134.78</v>
       </c>
-      <c r="D58" s="37">
+      <c r="D58" s="84">
         <v>48</v>
       </c>
-      <c r="E58" s="37">
+      <c r="E58" s="84">
         <v>15</v>
       </c>
-      <c r="F58" s="8">
-        <v>133.18103579999999</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="84">
+        <v>10</v>
+      </c>
+      <c r="G58" s="85">
+        <v>133.18103583163801</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" s="37" t="s">
         <v>982</v>
       </c>
       <c r="C61" s="37"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B62" s="37" t="s">
         <v>150</v>
       </c>
@@ -73479,7 +74078,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B63" s="37" t="s">
         <v>137</v>
       </c>
@@ -73487,7 +74086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B64" s="37" t="s">
         <v>138</v>
       </c>
@@ -73593,12 +74192,12 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="C79">
         <v>20.5</v>
@@ -73612,12 +74211,12 @@
         <v>32.5</v>
       </c>
       <c r="D80" s="37" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
@@ -73627,23 +74226,23 @@
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C84">
         <v>34.5</v>
       </c>
       <c r="D84" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
@@ -73656,7 +74255,7 @@
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C89">
         <v>42.7</v>
@@ -73686,7 +74285,7 @@
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="37"/>
       <c r="B91" s="37" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="C91" s="37"/>
       <c r="D91" s="37"/>
@@ -74016,13 +74615,13 @@
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="37" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="C107" s="37"/>
       <c r="D107" s="37"/>

</xml_diff>